<commit_message>
Update Clan Games data - 2025-12-24
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2107,7 +2107,7 @@
         <v/>
       </c>
       <c r="E8" s="5" t="n">
-        <v>34550</v>
+        <v>35250</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>4000</v>
@@ -2116,7 +2116,7 @@
         <v>4000</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>6200</v>
+        <v>6900</v>
       </c>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
@@ -2608,7 +2608,7 @@
         <v/>
       </c>
       <c r="E19" s="5" t="n">
-        <v>19900</v>
+        <v>20850</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>4000</v>
@@ -2617,7 +2617,7 @@
         <v>4000</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>2800</v>
+        <v>3750</v>
       </c>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-25
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2428,14 +2428,14 @@
         <v/>
       </c>
       <c r="E15" s="5" t="n">
-        <v>5750</v>
+        <v>6050</v>
       </c>
       <c r="F15" s="1" t="n"/>
       <c r="G15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>4050</v>
+        <v>4350</v>
       </c>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-26
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3336,7 +3336,7 @@
         <v/>
       </c>
       <c r="E35" s="5" t="n">
-        <v>31250</v>
+        <v>32100</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>4000</v>
@@ -3345,7 +3345,7 @@
         <v>4000</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>1500</v>
+        <v>2350</v>
       </c>
       <c r="I35" s="1" t="n"/>
       <c r="J35" s="1" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-27
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2702,12 +2702,12 @@
         <v/>
       </c>
       <c r="E21" s="5" t="n">
-        <v>97320</v>
+        <v>99120</v>
       </c>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n">
-        <v>2050</v>
+        <v>3850</v>
       </c>
       <c r="I21" s="1" t="n"/>
       <c r="J21" s="1" t="n"/>
@@ -3598,12 +3598,12 @@
         <v/>
       </c>
       <c r="E41" s="5" t="n">
-        <v>64950</v>
+        <v>66100</v>
       </c>
       <c r="F41" s="1" t="n"/>
       <c r="G41" s="1" t="n"/>
       <c r="H41" s="1" t="n">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="I41" s="1" t="n"/>
       <c r="J41" s="1" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-28
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3637,12 +3637,12 @@
         <v/>
       </c>
       <c r="E42" s="5" t="n">
-        <v>25100</v>
+        <v>25300</v>
       </c>
       <c r="F42" s="1" t="n"/>
       <c r="G42" s="1" t="n"/>
       <c r="H42" s="1" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I42" s="1" t="n"/>
       <c r="J42" s="1" t="n"/>

</xml_diff>

<commit_message>
Added google sheet feature
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Documents\GitHub\clashMacacos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAB414E9-3F2A-4136-BDAB-AD0F256B33F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A85A931-ED74-40F0-90F1-F4D1B206C9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clan games" sheetId="1" r:id="rId1"/>
@@ -1993,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
@@ -3937,7 +3937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-16
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3453,7 +3453,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2" s="48" t="n"/>
       <c r="N2" s="48" t="n"/>
@@ -5201,7 +5201,7 @@
       <c r="J32" s="57" t="n"/>
       <c r="K32" s="57" t="n"/>
       <c r="L32" s="59" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M32" s="57" t="n"/>
       <c r="N32" s="57" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-17
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -372,6 +372,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3233,7 +3242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH48"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
@@ -3453,7 +3462,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="50" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" s="48" t="n"/>
       <c r="N2" s="48" t="n"/>
@@ -3769,7 +3778,7 @@
       <c r="J8" s="57" t="n"/>
       <c r="K8" s="57" t="n"/>
       <c r="L8" s="59" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M8" s="57" t="n"/>
       <c r="N8" s="57" t="n"/>
@@ -4184,7 +4193,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M15" s="53" t="n"/>
       <c r="N15" s="53" t="n"/>
@@ -4249,7 +4258,7 @@
         <v>6</v>
       </c>
       <c r="L16" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M16" s="57" t="n"/>
       <c r="N16" s="57" t="n"/>
@@ -4605,7 +4614,7 @@
         <v>6</v>
       </c>
       <c r="L22" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M22" s="57" t="n"/>
       <c r="N22" s="57" t="n"/>
@@ -5034,7 +5043,7 @@
         <v>6</v>
       </c>
       <c r="L29" s="54" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M29" s="53" t="n"/>
       <c r="N29" s="53" t="n"/>
@@ -5366,7 +5375,7 @@
         <v>6</v>
       </c>
       <c r="L35" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M35" s="53" t="n"/>
       <c r="N35" s="53" t="n"/>
@@ -5496,7 +5505,7 @@
         <v>6</v>
       </c>
       <c r="L37" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M37" s="53" t="n"/>
       <c r="N37" s="53" t="n"/>
@@ -5691,7 +5700,7 @@
         <v>6</v>
       </c>
       <c r="L40" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M40" s="57" t="n"/>
       <c r="N40" s="57" t="n"/>
@@ -5750,7 +5759,7 @@
         <v>6</v>
       </c>
       <c r="L41" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M41" s="53" t="n"/>
       <c r="N41" s="53" t="n"/>
@@ -5866,7 +5875,7 @@
         <v>6</v>
       </c>
       <c r="L43" s="54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M43" s="53" t="n"/>
       <c r="N43" s="53" t="n"/>
@@ -6147,7 +6156,7 @@
       <c r="J48" s="63" t="n"/>
       <c r="K48" s="63" t="n"/>
       <c r="L48" s="63" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M48" s="63" t="n"/>
       <c r="N48" s="63" t="n"/>
@@ -6171,6 +6180,55 @@
       <c r="AF48" s="63" t="n"/>
       <c r="AG48" s="63" t="n"/>
       <c r="AH48" s="63" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="64" t="inlineStr">
+        <is>
+          <t>francesco</t>
+        </is>
+      </c>
+      <c r="B49" s="65" t="inlineStr">
+        <is>
+          <t>17/01/2026</t>
+        </is>
+      </c>
+      <c r="C49" s="64">
+        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
+        <v/>
+      </c>
+      <c r="D49" s="64" t="n"/>
+      <c r="E49" s="66" t="n"/>
+      <c r="F49" s="66" t="n"/>
+      <c r="G49" s="66" t="n"/>
+      <c r="H49" s="66" t="n"/>
+      <c r="I49" s="66" t="n"/>
+      <c r="J49" s="66" t="n"/>
+      <c r="K49" s="66" t="n"/>
+      <c r="L49" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="66" t="n"/>
+      <c r="N49" s="66" t="n"/>
+      <c r="O49" s="66" t="n"/>
+      <c r="P49" s="66" t="n"/>
+      <c r="Q49" s="66" t="n"/>
+      <c r="R49" s="66" t="n"/>
+      <c r="S49" s="66" t="n"/>
+      <c r="T49" s="66" t="n"/>
+      <c r="U49" s="66" t="n"/>
+      <c r="V49" s="66" t="n"/>
+      <c r="W49" s="66" t="n"/>
+      <c r="X49" s="66" t="n"/>
+      <c r="Y49" s="66" t="n"/>
+      <c r="Z49" s="66" t="n"/>
+      <c r="AA49" s="66" t="n"/>
+      <c r="AB49" s="66" t="n"/>
+      <c r="AC49" s="66" t="n"/>
+      <c r="AD49" s="66" t="n"/>
+      <c r="AE49" s="66" t="n"/>
+      <c r="AF49" s="66" t="n"/>
+      <c r="AG49" s="66" t="n"/>
+      <c r="AH49" s="66" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" thickBot="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-18
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3242,7 +3242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH49"/>
+  <dimension ref="A1:AH48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
@@ -3951,7 +3951,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="54" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M11" s="53" t="n"/>
       <c r="N11" s="53" t="n"/>
@@ -4075,7 +4075,7 @@
         <v>6</v>
       </c>
       <c r="L13" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M13" s="53" t="n"/>
       <c r="N13" s="53" t="n"/>
@@ -4323,7 +4323,7 @@
         <v>6</v>
       </c>
       <c r="L17" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M17" s="53" t="n"/>
       <c r="N17" s="53" t="n"/>
@@ -4378,7 +4378,7 @@
         <v>6</v>
       </c>
       <c r="L18" s="59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M18" s="57" t="n"/>
       <c r="N18" s="57" t="n"/>
@@ -4500,7 +4500,7 @@
         <v>6</v>
       </c>
       <c r="L20" s="59" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M20" s="57" t="n"/>
       <c r="N20" s="57" t="n"/>
@@ -4742,7 +4742,7 @@
         <v>6</v>
       </c>
       <c r="L24" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24" s="57" t="n"/>
       <c r="N24" s="57" t="n"/>
@@ -5102,7 +5102,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M30" s="57" t="n"/>
       <c r="N30" s="57" t="n"/>
@@ -5161,7 +5161,7 @@
         <v>6</v>
       </c>
       <c r="L31" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M31" s="53" t="n"/>
       <c r="N31" s="53" t="n"/>
@@ -5238,12 +5238,12 @@
     <row r="33">
       <c r="A33" s="51" t="inlineStr">
         <is>
-          <t>Punpie69</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B33" s="52" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C33" s="51">
@@ -5257,9 +5257,11 @@
       <c r="H33" s="53" t="n"/>
       <c r="I33" s="53" t="n"/>
       <c r="J33" s="53" t="n"/>
-      <c r="K33" s="53" t="n"/>
+      <c r="K33" s="60" t="n">
+        <v>6</v>
+      </c>
       <c r="L33" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M33" s="53" t="n"/>
       <c r="N33" s="53" t="n"/>
@@ -5287,25 +5289,39 @@
     <row r="34">
       <c r="A34" s="55" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B34" s="56" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C34" s="55">
         <f>ROUND(AVERAGE(D34:AH34), 0)</f>
         <v/>
       </c>
-      <c r="D34" s="55" t="n"/>
-      <c r="E34" s="57" t="n"/>
-      <c r="F34" s="57" t="n"/>
-      <c r="G34" s="57" t="n"/>
-      <c r="H34" s="57" t="n"/>
-      <c r="I34" s="57" t="n"/>
-      <c r="J34" s="57" t="n"/>
+      <c r="D34" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="H34" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="I34" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" s="58" t="n">
+        <v>6</v>
+      </c>
       <c r="K34" s="58" t="n">
         <v>6</v>
       </c>
@@ -5338,7 +5354,7 @@
     <row r="35">
       <c r="A35" s="51" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B35" s="52" t="inlineStr">
@@ -5351,7 +5367,7 @@
         <v/>
       </c>
       <c r="D35" s="51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="53" t="n">
         <v>6</v>
@@ -5363,7 +5379,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I35" s="53" t="n">
         <v>6</v>
@@ -5403,7 +5419,7 @@
     <row r="36">
       <c r="A36" s="55" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B36" s="56" t="inlineStr">
@@ -5416,7 +5432,7 @@
         <v/>
       </c>
       <c r="D36" s="55" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E36" s="57" t="n">
         <v>6</v>
@@ -5428,7 +5444,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="57" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I36" s="57" t="n">
         <v>6</v>
@@ -5440,7 +5456,7 @@
         <v>6</v>
       </c>
       <c r="L36" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M36" s="57" t="n"/>
       <c r="N36" s="57" t="n"/>
@@ -5468,7 +5484,7 @@
     <row r="37">
       <c r="A37" s="51" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>sidcu js</t>
         </is>
       </c>
       <c r="B37" s="52" t="inlineStr">
@@ -5502,10 +5518,10 @@
         <v>6</v>
       </c>
       <c r="K37" s="60" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L37" s="54" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M37" s="53" t="n"/>
       <c r="N37" s="53" t="n"/>
@@ -5533,7 +5549,7 @@
     <row r="38">
       <c r="A38" s="55" t="inlineStr">
         <is>
-          <t>sidcu js</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B38" s="56" t="inlineStr">
@@ -5546,7 +5562,7 @@
         <v/>
       </c>
       <c r="D38" s="55" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38" s="57" t="n">
         <v>6</v>
@@ -5564,13 +5580,13 @@
         <v>6</v>
       </c>
       <c r="J38" s="58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K38" s="58" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L38" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M38" s="57" t="n"/>
       <c r="N38" s="57" t="n"/>
@@ -5598,7 +5614,7 @@
     <row r="39">
       <c r="A39" s="51" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B39" s="52" t="inlineStr">
@@ -5611,7 +5627,7 @@
         <v/>
       </c>
       <c r="D39" s="51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E39" s="53" t="n">
         <v>6</v>
@@ -5629,13 +5645,13 @@
         <v>6</v>
       </c>
       <c r="J39" s="60" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K39" s="60" t="n">
         <v>6</v>
       </c>
       <c r="L39" s="54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M39" s="53" t="n"/>
       <c r="N39" s="53" t="n"/>
@@ -5663,7 +5679,7 @@
     <row r="40">
       <c r="A40" s="55" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B40" s="56" t="inlineStr">
@@ -5675,26 +5691,20 @@
         <f>ROUND(AVERAGE(D40:AH40), 0)</f>
         <v/>
       </c>
-      <c r="D40" s="55" t="n">
-        <v>6</v>
-      </c>
-      <c r="E40" s="57" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" s="57" t="n">
-        <v>6</v>
-      </c>
+      <c r="D40" s="55" t="n"/>
+      <c r="E40" s="57" t="n"/>
+      <c r="F40" s="57" t="n"/>
       <c r="G40" s="57" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H40" s="57" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I40" s="57" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J40" s="58" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K40" s="58" t="n">
         <v>6</v>
@@ -5728,12 +5738,12 @@
     <row r="41">
       <c r="A41" s="51" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>tazio</t>
         </is>
       </c>
       <c r="B41" s="52" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C41" s="51">
@@ -5743,18 +5753,10 @@
       <c r="D41" s="51" t="n"/>
       <c r="E41" s="53" t="n"/>
       <c r="F41" s="53" t="n"/>
-      <c r="G41" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="60" t="n">
-        <v>0</v>
-      </c>
+      <c r="G41" s="53" t="n"/>
+      <c r="H41" s="53" t="n"/>
+      <c r="I41" s="53" t="n"/>
+      <c r="J41" s="53" t="n"/>
       <c r="K41" s="60" t="n">
         <v>6</v>
       </c>
@@ -5787,30 +5789,44 @@
     <row r="42">
       <c r="A42" s="55" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B42" s="56" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C42" s="55">
         <f>ROUND(AVERAGE(D42:AH42), 0)</f>
         <v/>
       </c>
-      <c r="D42" s="55" t="n"/>
-      <c r="E42" s="57" t="n"/>
-      <c r="F42" s="57" t="n"/>
-      <c r="G42" s="57" t="n"/>
-      <c r="H42" s="57" t="n"/>
-      <c r="I42" s="57" t="n"/>
-      <c r="J42" s="57" t="n"/>
+      <c r="D42" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="E42" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F42" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="H42" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="I42" s="57" t="n">
+        <v>6</v>
+      </c>
+      <c r="J42" s="58" t="n">
+        <v>6</v>
+      </c>
       <c r="K42" s="58" t="n">
         <v>6</v>
       </c>
       <c r="L42" s="59" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M42" s="57" t="n"/>
       <c r="N42" s="57" t="n"/>
@@ -5838,7 +5854,7 @@
     <row r="43">
       <c r="A43" s="51" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B43" s="52" t="inlineStr">
@@ -5850,32 +5866,26 @@
         <f>ROUND(AVERAGE(D43:AH43), 0)</f>
         <v/>
       </c>
-      <c r="D43" s="51" t="n">
-        <v>6</v>
-      </c>
-      <c r="E43" s="53" t="n">
-        <v>6</v>
-      </c>
-      <c r="F43" s="53" t="n">
-        <v>6</v>
-      </c>
+      <c r="D43" s="51" t="n"/>
+      <c r="E43" s="53" t="n"/>
+      <c r="F43" s="53" t="n"/>
       <c r="G43" s="53" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H43" s="53" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I43" s="53" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J43" s="60" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K43" s="60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L43" s="54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M43" s="53" t="n"/>
       <c r="N43" s="53" t="n"/>
@@ -5903,7 +5913,7 @@
     <row r="44">
       <c r="A44" s="55" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B44" s="56" t="inlineStr">
@@ -5919,22 +5929,22 @@
       <c r="E44" s="57" t="n"/>
       <c r="F44" s="57" t="n"/>
       <c r="G44" s="57" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H44" s="57" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I44" s="57" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J44" s="58" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K44" s="58" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L44" s="59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M44" s="57" t="n"/>
       <c r="N44" s="57" t="n"/>
@@ -5962,7 +5972,7 @@
     <row r="45">
       <c r="A45" s="51" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zombra</t>
         </is>
       </c>
       <c r="B45" s="52" t="inlineStr">
@@ -5975,25 +5985,29 @@
         <v/>
       </c>
       <c r="D45" s="51" t="n"/>
-      <c r="E45" s="53" t="n"/>
-      <c r="F45" s="53" t="n"/>
+      <c r="E45" s="53" t="n">
+        <v>6</v>
+      </c>
+      <c r="F45" s="53" t="n">
+        <v>6</v>
+      </c>
       <c r="G45" s="53" t="n">
         <v>6</v>
       </c>
       <c r="H45" s="53" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I45" s="53" t="n">
         <v>6</v>
       </c>
       <c r="J45" s="60" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K45" s="60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L45" s="54" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M45" s="53" t="n"/>
       <c r="N45" s="53" t="n"/>
@@ -6021,12 +6035,12 @@
     <row r="46">
       <c r="A46" s="55" t="inlineStr">
         <is>
-          <t>zombra</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B46" s="56" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C46" s="55">
@@ -6034,26 +6048,14 @@
         <v/>
       </c>
       <c r="D46" s="55" t="n"/>
-      <c r="E46" s="57" t="n">
-        <v>6</v>
-      </c>
-      <c r="F46" s="57" t="n">
-        <v>6</v>
-      </c>
-      <c r="G46" s="57" t="n">
-        <v>6</v>
-      </c>
-      <c r="H46" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="57" t="n">
-        <v>6</v>
-      </c>
-      <c r="J46" s="58" t="n">
-        <v>0</v>
-      </c>
+      <c r="E46" s="57" t="n"/>
+      <c r="F46" s="57" t="n"/>
+      <c r="G46" s="57" t="n"/>
+      <c r="H46" s="57" t="n"/>
+      <c r="I46" s="57" t="n"/>
+      <c r="J46" s="57" t="n"/>
       <c r="K46" s="58" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L46" s="59" t="n">
         <v>0</v>
@@ -6082,65 +6084,63 @@
       <c r="AH46" s="57" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="51" t="inlineStr">
-        <is>
-          <t>zordan</t>
-        </is>
-      </c>
-      <c r="B47" s="52" t="inlineStr">
-        <is>
-          <t>05/01/2026</t>
-        </is>
-      </c>
-      <c r="C47" s="51">
+      <c r="A47" s="64" t="inlineStr">
+        <is>
+          <t>Fryck</t>
+        </is>
+      </c>
+      <c r="B47" s="65" t="inlineStr">
+        <is>
+          <t>16/01/2026</t>
+        </is>
+      </c>
+      <c r="C47" s="64">
         <f>ROUND(AVERAGE(D47:AH47), 0)</f>
         <v/>
       </c>
-      <c r="D47" s="51" t="n"/>
-      <c r="E47" s="53" t="n"/>
-      <c r="F47" s="53" t="n"/>
-      <c r="G47" s="53" t="n"/>
-      <c r="H47" s="53" t="n"/>
-      <c r="I47" s="53" t="n"/>
-      <c r="J47" s="53" t="n"/>
-      <c r="K47" s="60" t="n">
-        <v>6</v>
-      </c>
-      <c r="L47" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" s="53" t="n"/>
-      <c r="N47" s="53" t="n"/>
-      <c r="O47" s="53" t="n"/>
-      <c r="P47" s="53" t="n"/>
-      <c r="Q47" s="53" t="n"/>
-      <c r="R47" s="53" t="n"/>
-      <c r="S47" s="53" t="n"/>
-      <c r="T47" s="53" t="n"/>
-      <c r="U47" s="53" t="n"/>
-      <c r="V47" s="53" t="n"/>
-      <c r="W47" s="53" t="n"/>
-      <c r="X47" s="53" t="n"/>
-      <c r="Y47" s="53" t="n"/>
-      <c r="Z47" s="53" t="n"/>
-      <c r="AA47" s="53" t="n"/>
-      <c r="AB47" s="53" t="n"/>
-      <c r="AC47" s="53" t="n"/>
-      <c r="AD47" s="53" t="n"/>
-      <c r="AE47" s="53" t="n"/>
-      <c r="AF47" s="53" t="n"/>
-      <c r="AG47" s="53" t="n"/>
-      <c r="AH47" s="53" t="n"/>
+      <c r="D47" s="64" t="n"/>
+      <c r="E47" s="66" t="n"/>
+      <c r="F47" s="66" t="n"/>
+      <c r="G47" s="66" t="n"/>
+      <c r="H47" s="66" t="n"/>
+      <c r="I47" s="66" t="n"/>
+      <c r="J47" s="66" t="n"/>
+      <c r="K47" s="66" t="n"/>
+      <c r="L47" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="M47" s="66" t="n"/>
+      <c r="N47" s="66" t="n"/>
+      <c r="O47" s="66" t="n"/>
+      <c r="P47" s="66" t="n"/>
+      <c r="Q47" s="66" t="n"/>
+      <c r="R47" s="66" t="n"/>
+      <c r="S47" s="66" t="n"/>
+      <c r="T47" s="66" t="n"/>
+      <c r="U47" s="66" t="n"/>
+      <c r="V47" s="66" t="n"/>
+      <c r="W47" s="66" t="n"/>
+      <c r="X47" s="66" t="n"/>
+      <c r="Y47" s="66" t="n"/>
+      <c r="Z47" s="66" t="n"/>
+      <c r="AA47" s="66" t="n"/>
+      <c r="AB47" s="66" t="n"/>
+      <c r="AC47" s="66" t="n"/>
+      <c r="AD47" s="66" t="n"/>
+      <c r="AE47" s="66" t="n"/>
+      <c r="AF47" s="66" t="n"/>
+      <c r="AG47" s="66" t="n"/>
+      <c r="AH47" s="66" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="61" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>francesco</t>
         </is>
       </c>
       <c r="B48" s="62" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C48" s="61">
@@ -6156,7 +6156,7 @@
       <c r="J48" s="63" t="n"/>
       <c r="K48" s="63" t="n"/>
       <c r="L48" s="63" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M48" s="63" t="n"/>
       <c r="N48" s="63" t="n"/>
@@ -6180,55 +6180,6 @@
       <c r="AF48" s="63" t="n"/>
       <c r="AG48" s="63" t="n"/>
       <c r="AH48" s="63" t="n"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="64" t="inlineStr">
-        <is>
-          <t>francesco</t>
-        </is>
-      </c>
-      <c r="B49" s="65" t="inlineStr">
-        <is>
-          <t>17/01/2026</t>
-        </is>
-      </c>
-      <c r="C49" s="64">
-        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
-        <v/>
-      </c>
-      <c r="D49" s="64" t="n"/>
-      <c r="E49" s="66" t="n"/>
-      <c r="F49" s="66" t="n"/>
-      <c r="G49" s="66" t="n"/>
-      <c r="H49" s="66" t="n"/>
-      <c r="I49" s="66" t="n"/>
-      <c r="J49" s="66" t="n"/>
-      <c r="K49" s="66" t="n"/>
-      <c r="L49" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" s="66" t="n"/>
-      <c r="N49" s="66" t="n"/>
-      <c r="O49" s="66" t="n"/>
-      <c r="P49" s="66" t="n"/>
-      <c r="Q49" s="66" t="n"/>
-      <c r="R49" s="66" t="n"/>
-      <c r="S49" s="66" t="n"/>
-      <c r="T49" s="66" t="n"/>
-      <c r="U49" s="66" t="n"/>
-      <c r="V49" s="66" t="n"/>
-      <c r="W49" s="66" t="n"/>
-      <c r="X49" s="66" t="n"/>
-      <c r="Y49" s="66" t="n"/>
-      <c r="Z49" s="66" t="n"/>
-      <c r="AA49" s="66" t="n"/>
-      <c r="AB49" s="66" t="n"/>
-      <c r="AC49" s="66" t="n"/>
-      <c r="AD49" s="66" t="n"/>
-      <c r="AE49" s="66" t="n"/>
-      <c r="AF49" s="66" t="n"/>
-      <c r="AG49" s="66" t="n"/>
-      <c r="AH49" s="66" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" thickBot="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-19
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3242,7 +3242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH48"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
@@ -6180,6 +6180,53 @@
       <c r="AF48" s="63" t="n"/>
       <c r="AG48" s="63" t="n"/>
       <c r="AH48" s="63" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="64" t="inlineStr">
+        <is>
+          <t>fabiovesco</t>
+        </is>
+      </c>
+      <c r="B49" s="65" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="C49" s="64">
+        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
+        <v/>
+      </c>
+      <c r="D49" s="64" t="n"/>
+      <c r="E49" s="66" t="n"/>
+      <c r="F49" s="66" t="n"/>
+      <c r="G49" s="66" t="n"/>
+      <c r="H49" s="66" t="n"/>
+      <c r="I49" s="66" t="n"/>
+      <c r="J49" s="66" t="n"/>
+      <c r="K49" s="66" t="n"/>
+      <c r="L49" s="66" t="n"/>
+      <c r="M49" s="66" t="n"/>
+      <c r="N49" s="66" t="n"/>
+      <c r="O49" s="66" t="n"/>
+      <c r="P49" s="66" t="n"/>
+      <c r="Q49" s="66" t="n"/>
+      <c r="R49" s="66" t="n"/>
+      <c r="S49" s="66" t="n"/>
+      <c r="T49" s="66" t="n"/>
+      <c r="U49" s="66" t="n"/>
+      <c r="V49" s="66" t="n"/>
+      <c r="W49" s="66" t="n"/>
+      <c r="X49" s="66" t="n"/>
+      <c r="Y49" s="66" t="n"/>
+      <c r="Z49" s="66" t="n"/>
+      <c r="AA49" s="66" t="n"/>
+      <c r="AB49" s="66" t="n"/>
+      <c r="AC49" s="66" t="n"/>
+      <c r="AD49" s="66" t="n"/>
+      <c r="AE49" s="66" t="n"/>
+      <c r="AF49" s="66" t="n"/>
+      <c r="AG49" s="66" t="n"/>
+      <c r="AH49" s="66" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1" thickBot="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-21
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -743,7 +743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -3229,7 +3229,51 @@
       <c r="Z50" s="42" t="n"/>
       <c r="AA50" s="42" t="n"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="51" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A51" s="35" t="inlineStr">
+        <is>
+          <t>Anton 48</t>
+        </is>
+      </c>
+      <c r="B51" s="36" t="inlineStr">
+        <is>
+          <t>21/01/2026</t>
+        </is>
+      </c>
+      <c r="C51" s="35">
+        <f>ROUND(AVERAGE(F51:AB51), 0)</f>
+        <v/>
+      </c>
+      <c r="D51" s="37">
+        <f>SUM(F51:AB51)</f>
+        <v/>
+      </c>
+      <c r="E51" s="35" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F51" s="35" t="n"/>
+      <c r="G51" s="37" t="n"/>
+      <c r="H51" s="37" t="n"/>
+      <c r="I51" s="37" t="n"/>
+      <c r="J51" s="37" t="n"/>
+      <c r="K51" s="37" t="n"/>
+      <c r="L51" s="37" t="n"/>
+      <c r="M51" s="37" t="n"/>
+      <c r="N51" s="37" t="n"/>
+      <c r="O51" s="37" t="n"/>
+      <c r="P51" s="37" t="n"/>
+      <c r="Q51" s="37" t="n"/>
+      <c r="R51" s="37" t="n"/>
+      <c r="S51" s="37" t="n"/>
+      <c r="T51" s="37" t="n"/>
+      <c r="U51" s="37" t="n"/>
+      <c r="V51" s="37" t="n"/>
+      <c r="W51" s="37" t="n"/>
+      <c r="X51" s="38" t="n"/>
+      <c r="Y51" s="38" t="n"/>
+      <c r="Z51" s="38" t="n"/>
+      <c r="AA51" s="38" t="n"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AA1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-22
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -931,7 +931,9 @@
       <c r="H2" s="33" t="n">
         <v>3400</v>
       </c>
-      <c r="I2" s="33" t="n"/>
+      <c r="I2" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="J2" s="33" t="n"/>
       <c r="K2" s="33" t="n"/>
       <c r="L2" s="33" t="n"/>
@@ -978,7 +980,9 @@
       <c r="H3" s="37" t="n">
         <v>500</v>
       </c>
-      <c r="I3" s="37" t="n"/>
+      <c r="I3" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J3" s="37" t="n"/>
       <c r="K3" s="37" t="n"/>
       <c r="L3" s="37" t="n"/>
@@ -1029,7 +1033,9 @@
       <c r="H4" s="41" t="n">
         <v>4100</v>
       </c>
-      <c r="I4" s="41" t="n"/>
+      <c r="I4" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J4" s="41" t="n"/>
       <c r="K4" s="41" t="n"/>
       <c r="L4" s="41" t="n"/>
@@ -1078,7 +1084,9 @@
       <c r="H5" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="37" t="n"/>
+      <c r="I5" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J5" s="37" t="n"/>
       <c r="K5" s="37" t="n"/>
       <c r="L5" s="37" t="n"/>
@@ -1125,7 +1133,9 @@
       <c r="H6" s="41" t="n">
         <v>1200</v>
       </c>
-      <c r="I6" s="41" t="n"/>
+      <c r="I6" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J6" s="41" t="n"/>
       <c r="K6" s="41" t="n"/>
       <c r="L6" s="41" t="n"/>
@@ -1172,7 +1182,9 @@
       <c r="H7" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="37" t="n"/>
+      <c r="I7" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J7" s="37" t="n"/>
       <c r="K7" s="37" t="n"/>
       <c r="L7" s="37" t="n"/>
@@ -1219,7 +1231,9 @@
       <c r="H8" s="41" t="n">
         <v>1300</v>
       </c>
-      <c r="I8" s="41" t="n"/>
+      <c r="I8" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J8" s="41" t="n"/>
       <c r="K8" s="41" t="n"/>
       <c r="L8" s="41" t="n"/>
@@ -1270,7 +1284,9 @@
       <c r="H9" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I9" s="37" t="n"/>
+      <c r="I9" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J9" s="37" t="n"/>
       <c r="K9" s="37" t="n"/>
       <c r="L9" s="37" t="n"/>
@@ -1319,7 +1335,9 @@
       <c r="H10" s="41" t="n">
         <v>6050</v>
       </c>
-      <c r="I10" s="41" t="n"/>
+      <c r="I10" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J10" s="41" t="n"/>
       <c r="K10" s="41" t="n"/>
       <c r="L10" s="41" t="n"/>
@@ -1366,7 +1384,9 @@
       <c r="H11" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="37" t="n"/>
+      <c r="I11" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J11" s="37" t="n"/>
       <c r="K11" s="37" t="n"/>
       <c r="L11" s="37" t="n"/>
@@ -1413,7 +1433,9 @@
       <c r="H12" s="41" t="n">
         <v>4050</v>
       </c>
-      <c r="I12" s="41" t="n"/>
+      <c r="I12" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J12" s="41" t="n"/>
       <c r="K12" s="41" t="n"/>
       <c r="L12" s="41" t="n"/>
@@ -1464,7 +1486,9 @@
       <c r="H13" s="37" t="n">
         <v>1800</v>
       </c>
-      <c r="I13" s="37" t="n"/>
+      <c r="I13" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J13" s="37" t="n"/>
       <c r="K13" s="37" t="n"/>
       <c r="L13" s="37" t="n"/>
@@ -1515,7 +1539,9 @@
       <c r="H14" s="41" t="n">
         <v>10000</v>
       </c>
-      <c r="I14" s="41" t="n"/>
+      <c r="I14" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J14" s="41" t="n"/>
       <c r="K14" s="41" t="n"/>
       <c r="L14" s="41" t="n"/>
@@ -1564,7 +1590,9 @@
       <c r="H15" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I15" s="37" t="n"/>
+      <c r="I15" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J15" s="37" t="n"/>
       <c r="K15" s="37" t="n"/>
       <c r="L15" s="37" t="n"/>
@@ -1613,7 +1641,9 @@
       <c r="H16" s="41" t="n">
         <v>10000</v>
       </c>
-      <c r="I16" s="41" t="n"/>
+      <c r="I16" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J16" s="41" t="n"/>
       <c r="K16" s="41" t="n"/>
       <c r="L16" s="41" t="n"/>
@@ -1660,7 +1690,9 @@
       <c r="H17" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I17" s="37" t="n"/>
+      <c r="I17" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J17" s="37" t="n"/>
       <c r="K17" s="37" t="n"/>
       <c r="L17" s="43" t="n"/>
@@ -1711,7 +1743,9 @@
       <c r="H18" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="41" t="n"/>
+      <c r="I18" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J18" s="41" t="n"/>
       <c r="K18" s="41" t="n"/>
       <c r="L18" s="41" t="n"/>
@@ -1762,7 +1796,9 @@
       <c r="H19" s="37" t="n">
         <v>5800</v>
       </c>
-      <c r="I19" s="37" t="n"/>
+      <c r="I19" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J19" s="37" t="n"/>
       <c r="K19" s="37" t="n"/>
       <c r="L19" s="37" t="n"/>
@@ -1809,7 +1845,9 @@
       <c r="H20" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="41" t="n"/>
+      <c r="I20" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J20" s="41" t="n"/>
       <c r="K20" s="41" t="n"/>
       <c r="L20" s="41" t="n"/>
@@ -1856,7 +1894,9 @@
       <c r="H21" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I21" s="37" t="n"/>
+      <c r="I21" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J21" s="37" t="n"/>
       <c r="K21" s="37" t="n"/>
       <c r="L21" s="37" t="n"/>
@@ -1903,7 +1943,9 @@
       <c r="H22" s="41" t="n">
         <v>10000</v>
       </c>
-      <c r="I22" s="41" t="n"/>
+      <c r="I22" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J22" s="41" t="n"/>
       <c r="K22" s="41" t="n"/>
       <c r="L22" s="41" t="n"/>
@@ -1954,7 +1996,9 @@
       <c r="H23" s="37" t="n">
         <v>4050</v>
       </c>
-      <c r="I23" s="37" t="n"/>
+      <c r="I23" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J23" s="37" t="n"/>
       <c r="K23" s="37" t="n"/>
       <c r="L23" s="37" t="n"/>
@@ -2003,7 +2047,9 @@
       <c r="H24" s="41" t="n">
         <v>5150</v>
       </c>
-      <c r="I24" s="41" t="n"/>
+      <c r="I24" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J24" s="41" t="n"/>
       <c r="K24" s="41" t="n"/>
       <c r="L24" s="41" t="n"/>
@@ -2054,7 +2100,9 @@
       <c r="H25" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I25" s="37" t="n"/>
+      <c r="I25" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J25" s="37" t="n"/>
       <c r="K25" s="37" t="n"/>
       <c r="L25" s="37" t="n"/>
@@ -2103,7 +2151,9 @@
       <c r="H26" s="41" t="n">
         <v>300</v>
       </c>
-      <c r="I26" s="41" t="n"/>
+      <c r="I26" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J26" s="41" t="n"/>
       <c r="K26" s="41" t="n"/>
       <c r="L26" s="41" t="n"/>
@@ -2152,7 +2202,9 @@
       <c r="H27" s="37" t="n">
         <v>10000</v>
       </c>
-      <c r="I27" s="37" t="n"/>
+      <c r="I27" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J27" s="37" t="n"/>
       <c r="K27" s="37" t="n"/>
       <c r="L27" s="37" t="n"/>
@@ -2203,7 +2255,9 @@
       <c r="H28" s="41" t="n">
         <v>4050</v>
       </c>
-      <c r="I28" s="41" t="n"/>
+      <c r="I28" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J28" s="41" t="n"/>
       <c r="K28" s="41" t="n"/>
       <c r="L28" s="41" t="n"/>
@@ -2250,7 +2304,9 @@
       <c r="H29" s="37" t="n">
         <v>3650</v>
       </c>
-      <c r="I29" s="37" t="n"/>
+      <c r="I29" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J29" s="37" t="n"/>
       <c r="K29" s="37" t="n"/>
       <c r="L29" s="37" t="n"/>
@@ -2301,7 +2357,9 @@
       <c r="H30" s="41" t="n">
         <v>5750</v>
       </c>
-      <c r="I30" s="41" t="n"/>
+      <c r="I30" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J30" s="41" t="n"/>
       <c r="K30" s="41" t="n"/>
       <c r="L30" s="41" t="n"/>
@@ -2348,7 +2406,9 @@
       <c r="H31" s="37" t="n">
         <v>150</v>
       </c>
-      <c r="I31" s="37" t="n"/>
+      <c r="I31" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J31" s="37" t="n"/>
       <c r="K31" s="37" t="n"/>
       <c r="L31" s="37" t="n"/>
@@ -2395,7 +2455,9 @@
       <c r="H32" s="41" t="n">
         <v>3850</v>
       </c>
-      <c r="I32" s="41" t="n"/>
+      <c r="I32" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J32" s="41" t="n"/>
       <c r="K32" s="41" t="n"/>
       <c r="L32" s="41" t="n"/>
@@ -2444,7 +2506,9 @@
       <c r="H33" s="37" t="n">
         <v>1200</v>
       </c>
-      <c r="I33" s="37" t="n"/>
+      <c r="I33" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J33" s="37" t="n"/>
       <c r="K33" s="37" t="n"/>
       <c r="L33" s="37" t="n"/>
@@ -2489,7 +2553,9 @@
       <c r="F34" s="39" t="n"/>
       <c r="G34" s="41" t="n"/>
       <c r="H34" s="41" t="n"/>
-      <c r="I34" s="41" t="n"/>
+      <c r="I34" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J34" s="41" t="n"/>
       <c r="K34" s="41" t="n"/>
       <c r="L34" s="41" t="n"/>
@@ -2534,7 +2600,9 @@
       <c r="F35" s="35" t="n"/>
       <c r="G35" s="37" t="n"/>
       <c r="H35" s="37" t="n"/>
-      <c r="I35" s="37" t="n"/>
+      <c r="I35" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J35" s="37" t="n"/>
       <c r="K35" s="37" t="n"/>
       <c r="L35" s="37" t="n"/>
@@ -2579,7 +2647,9 @@
       <c r="F36" s="39" t="n"/>
       <c r="G36" s="41" t="n"/>
       <c r="H36" s="41" t="n"/>
-      <c r="I36" s="41" t="n"/>
+      <c r="I36" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J36" s="41" t="n"/>
       <c r="K36" s="41" t="n"/>
       <c r="L36" s="41" t="n"/>
@@ -2624,7 +2694,9 @@
       <c r="F37" s="35" t="n"/>
       <c r="G37" s="37" t="n"/>
       <c r="H37" s="37" t="n"/>
-      <c r="I37" s="37" t="n"/>
+      <c r="I37" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J37" s="37" t="n"/>
       <c r="K37" s="37" t="n"/>
       <c r="L37" s="37" t="n"/>
@@ -2669,7 +2741,9 @@
       <c r="F38" s="39" t="n"/>
       <c r="G38" s="41" t="n"/>
       <c r="H38" s="41" t="n"/>
-      <c r="I38" s="41" t="n"/>
+      <c r="I38" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J38" s="41" t="n"/>
       <c r="K38" s="41" t="n"/>
       <c r="L38" s="41" t="n"/>
@@ -2714,7 +2788,9 @@
       <c r="F39" s="35" t="n"/>
       <c r="G39" s="37" t="n"/>
       <c r="H39" s="37" t="n"/>
-      <c r="I39" s="37" t="n"/>
+      <c r="I39" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J39" s="37" t="n"/>
       <c r="K39" s="37" t="n"/>
       <c r="L39" s="37" t="n"/>
@@ -2759,7 +2835,9 @@
       <c r="F40" s="39" t="n"/>
       <c r="G40" s="41" t="n"/>
       <c r="H40" s="41" t="n"/>
-      <c r="I40" s="41" t="n"/>
+      <c r="I40" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J40" s="41" t="n"/>
       <c r="K40" s="41" t="n"/>
       <c r="L40" s="41" t="n"/>
@@ -2804,7 +2882,9 @@
       <c r="F41" s="35" t="n"/>
       <c r="G41" s="37" t="n"/>
       <c r="H41" s="37" t="n"/>
-      <c r="I41" s="37" t="n"/>
+      <c r="I41" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J41" s="37" t="n"/>
       <c r="K41" s="37" t="n"/>
       <c r="L41" s="37" t="n"/>
@@ -2849,7 +2929,9 @@
       <c r="F42" s="39" t="n"/>
       <c r="G42" s="41" t="n"/>
       <c r="H42" s="41" t="n"/>
-      <c r="I42" s="41" t="n"/>
+      <c r="I42" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J42" s="41" t="n"/>
       <c r="K42" s="41" t="n"/>
       <c r="L42" s="41" t="n"/>
@@ -2894,7 +2976,9 @@
       <c r="F43" s="35" t="n"/>
       <c r="G43" s="37" t="n"/>
       <c r="H43" s="37" t="n"/>
-      <c r="I43" s="37" t="n"/>
+      <c r="I43" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J43" s="37" t="n"/>
       <c r="K43" s="37" t="n"/>
       <c r="L43" s="37" t="n"/>
@@ -2939,7 +3023,9 @@
       <c r="F44" s="39" t="n"/>
       <c r="G44" s="41" t="n"/>
       <c r="H44" s="41" t="n"/>
-      <c r="I44" s="41" t="n"/>
+      <c r="I44" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J44" s="41" t="n"/>
       <c r="K44" s="41" t="n"/>
       <c r="L44" s="41" t="n"/>
@@ -2984,7 +3070,9 @@
       <c r="F45" s="35" t="n"/>
       <c r="G45" s="37" t="n"/>
       <c r="H45" s="37" t="n"/>
-      <c r="I45" s="37" t="n"/>
+      <c r="I45" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J45" s="37" t="n"/>
       <c r="K45" s="37" t="n"/>
       <c r="L45" s="37" t="n"/>
@@ -3029,7 +3117,9 @@
       <c r="F46" s="39" t="n"/>
       <c r="G46" s="41" t="n"/>
       <c r="H46" s="41" t="n"/>
-      <c r="I46" s="41" t="n"/>
+      <c r="I46" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J46" s="41" t="n"/>
       <c r="K46" s="41" t="n"/>
       <c r="L46" s="41" t="n"/>
@@ -3074,7 +3164,9 @@
       <c r="F47" s="35" t="n"/>
       <c r="G47" s="37" t="n"/>
       <c r="H47" s="37" t="n"/>
-      <c r="I47" s="37" t="n"/>
+      <c r="I47" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J47" s="37" t="n"/>
       <c r="K47" s="37" t="n"/>
       <c r="L47" s="37" t="n"/>
@@ -3119,7 +3211,9 @@
       <c r="F48" s="39" t="n"/>
       <c r="G48" s="41" t="n"/>
       <c r="H48" s="41" t="n"/>
-      <c r="I48" s="41" t="n"/>
+      <c r="I48" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J48" s="41" t="n"/>
       <c r="K48" s="41" t="n"/>
       <c r="L48" s="41" t="n"/>
@@ -3164,7 +3258,9 @@
       <c r="F49" s="35" t="n"/>
       <c r="G49" s="37" t="n"/>
       <c r="H49" s="37" t="n"/>
-      <c r="I49" s="37" t="n"/>
+      <c r="I49" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J49" s="37" t="n"/>
       <c r="K49" s="37" t="n"/>
       <c r="L49" s="37" t="n"/>
@@ -3209,7 +3305,9 @@
       <c r="F50" s="39" t="n"/>
       <c r="G50" s="41" t="n"/>
       <c r="H50" s="41" t="n"/>
-      <c r="I50" s="41" t="n"/>
+      <c r="I50" s="41" t="n">
+        <v>0</v>
+      </c>
       <c r="J50" s="41" t="n"/>
       <c r="K50" s="41" t="n"/>
       <c r="L50" s="41" t="n"/>
@@ -3254,7 +3352,9 @@
       <c r="F51" s="35" t="n"/>
       <c r="G51" s="37" t="n"/>
       <c r="H51" s="37" t="n"/>
-      <c r="I51" s="37" t="n"/>
+      <c r="I51" s="37" t="n">
+        <v>0</v>
+      </c>
       <c r="J51" s="37" t="n"/>
       <c r="K51" s="37" t="n"/>
       <c r="L51" s="37" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-23
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -1224,7 +1224,7 @@
         <v/>
       </c>
       <c r="E8" s="39" t="n">
-        <v>66250</v>
+        <v>67250</v>
       </c>
       <c r="F8" s="39" t="n"/>
       <c r="G8" s="41" t="n"/>
@@ -1232,7 +1232,7 @@
         <v>1300</v>
       </c>
       <c r="I8" s="41" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J8" s="41" t="n"/>
       <c r="K8" s="41" t="n"/>
@@ -1732,7 +1732,7 @@
         <v/>
       </c>
       <c r="E18" s="39" t="n">
-        <v>5025</v>
+        <v>5175</v>
       </c>
       <c r="F18" s="39" t="n">
         <v>1000</v>
@@ -1744,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="41" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="J18" s="41" t="n"/>
       <c r="K18" s="41" t="n"/>
@@ -2244,7 +2244,7 @@
         <v/>
       </c>
       <c r="E28" s="39" t="n">
-        <v>26725</v>
+        <v>29025</v>
       </c>
       <c r="F28" s="39" t="n">
         <v>4000</v>
@@ -2256,7 +2256,7 @@
         <v>4050</v>
       </c>
       <c r="I28" s="41" t="n">
-        <v>2550</v>
+        <v>4850</v>
       </c>
       <c r="J28" s="41" t="n"/>
       <c r="K28" s="41" t="n"/>
@@ -3065,13 +3065,13 @@
         <v/>
       </c>
       <c r="E45" s="35" t="n">
-        <v>91125</v>
+        <v>92625</v>
       </c>
       <c r="F45" s="35" t="n"/>
       <c r="G45" s="37" t="n"/>
       <c r="H45" s="37" t="n"/>
       <c r="I45" s="37" t="n">
-        <v>4550</v>
+        <v>6050</v>
       </c>
       <c r="J45" s="37" t="n"/>
       <c r="K45" s="37" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-24
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3065,13 +3065,13 @@
         <v/>
       </c>
       <c r="E45" s="35" t="n">
-        <v>94625</v>
+        <v>96625</v>
       </c>
       <c r="F45" s="35" t="n"/>
       <c r="G45" s="37" t="n"/>
       <c r="H45" s="37" t="n"/>
       <c r="I45" s="37" t="n">
-        <v>8050</v>
+        <v>10000</v>
       </c>
       <c r="J45" s="37" t="n"/>
       <c r="K45" s="37" t="n"/>
@@ -3112,13 +3112,13 @@
         <v/>
       </c>
       <c r="E46" s="39" t="n">
-        <v>8200</v>
+        <v>9400</v>
       </c>
       <c r="F46" s="39" t="n"/>
       <c r="G46" s="41" t="n"/>
       <c r="H46" s="41" t="n"/>
       <c r="I46" s="41" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="J46" s="41" t="n"/>
       <c r="K46" s="41" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-25
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -763,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1"/>
@@ -1548,7 +1548,7 @@
         <v/>
       </c>
       <c r="E14" s="39" t="n">
-        <v>34900</v>
+        <v>36600</v>
       </c>
       <c r="F14" s="39" t="n">
         <v>4000</v>
@@ -1560,7 +1560,7 @@
         <v>10000</v>
       </c>
       <c r="I14" s="41" t="n">
-        <v>8450</v>
+        <v>10000</v>
       </c>
       <c r="J14" s="41" t="n"/>
       <c r="K14" s="41" t="n"/>
@@ -2468,7 +2468,7 @@
         <v/>
       </c>
       <c r="E32" s="39" t="n">
-        <v>100070</v>
+        <v>101570</v>
       </c>
       <c r="F32" s="39" t="n"/>
       <c r="G32" s="41" t="n"/>
@@ -2476,7 +2476,7 @@
         <v>3850</v>
       </c>
       <c r="I32" s="41" t="n">
-        <v>950</v>
+        <v>2450</v>
       </c>
       <c r="J32" s="41" t="n"/>
       <c r="K32" s="41" t="n"/>
@@ -2850,13 +2850,13 @@
         <v/>
       </c>
       <c r="E40" s="39" t="n">
-        <v>60070</v>
+        <v>60420</v>
       </c>
       <c r="F40" s="39" t="n"/>
       <c r="G40" s="41" t="n"/>
       <c r="H40" s="41" t="n"/>
       <c r="I40" s="41" t="n">
-        <v>5400</v>
+        <v>5750</v>
       </c>
       <c r="J40" s="41" t="n"/>
       <c r="K40" s="41" t="n"/>
@@ -3299,6 +3299,53 @@
       <c r="Y49" s="38" t="n"/>
       <c r="Z49" s="38" t="n"/>
       <c r="AA49" s="38" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="39" t="inlineStr">
+        <is>
+          <t>Kle</t>
+        </is>
+      </c>
+      <c r="B50" s="40" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="C50" s="39">
+        <f>ROUND(AVERAGE(F50:AB50), 0)</f>
+        <v/>
+      </c>
+      <c r="D50" s="41">
+        <f>SUM(F50:AB50)</f>
+        <v/>
+      </c>
+      <c r="E50" s="39" t="n">
+        <v>74050</v>
+      </c>
+      <c r="F50" s="39" t="n"/>
+      <c r="G50" s="41" t="n"/>
+      <c r="H50" s="41" t="n"/>
+      <c r="I50" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="41" t="n"/>
+      <c r="K50" s="41" t="n"/>
+      <c r="L50" s="41" t="n"/>
+      <c r="M50" s="41" t="n"/>
+      <c r="N50" s="41" t="n"/>
+      <c r="O50" s="41" t="n"/>
+      <c r="P50" s="41" t="n"/>
+      <c r="Q50" s="41" t="n"/>
+      <c r="R50" s="41" t="n"/>
+      <c r="S50" s="41" t="n"/>
+      <c r="T50" s="41" t="n"/>
+      <c r="U50" s="41" t="n"/>
+      <c r="V50" s="41" t="n"/>
+      <c r="W50" s="41" t="n"/>
+      <c r="X50" s="42" t="n"/>
+      <c r="Y50" s="42" t="n"/>
+      <c r="Z50" s="42" t="n"/>
+      <c r="AA50" s="42" t="n"/>
     </row>
     <row r="51" ht="15.75" customHeight="1" thickBot="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-25
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -4401,7 +4401,7 @@
         <v>6</v>
       </c>
       <c r="M15" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N15" s="48" t="n"/>
       <c r="O15" s="48" t="n"/>
@@ -4570,7 +4570,7 @@
         <v>6</v>
       </c>
       <c r="M18" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N18" s="44" t="n"/>
       <c r="O18" s="44" t="n"/>
@@ -4627,7 +4627,7 @@
         <v>2</v>
       </c>
       <c r="M19" s="48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" s="48" t="n"/>
       <c r="O19" s="48" t="n"/>
@@ -5607,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="M35" s="48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N35" s="48" t="n"/>
       <c r="O35" s="48" t="n"/>
@@ -6390,7 +6390,7 @@
     <row r="48">
       <c r="A48" s="44" t="inlineStr">
         <is>
-          <t>alesofi</t>
+          <t>DARKGOST9</t>
         </is>
       </c>
       <c r="B48" s="45" t="inlineStr">
@@ -6439,12 +6439,12 @@
     <row r="49">
       <c r="A49" s="48" t="inlineStr">
         <is>
-          <t>sammesc</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B49" s="49" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C49" s="48">
@@ -6461,7 +6461,7 @@
       <c r="K49" s="50" t="n"/>
       <c r="L49" s="51" t="n"/>
       <c r="M49" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N49" s="48" t="n"/>
       <c r="O49" s="48" t="n"/>
@@ -6488,12 +6488,12 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="44" t="inlineStr">
         <is>
-          <t>DARKGOST9</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B50" s="45" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C50" s="44">
@@ -6510,7 +6510,7 @@
       <c r="K50" s="46" t="n"/>
       <c r="L50" s="47" t="n"/>
       <c r="M50" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N50" s="44" t="n"/>
       <c r="O50" s="44" t="n"/>
@@ -6537,12 +6537,12 @@
     <row r="51">
       <c r="A51" s="48" t="inlineStr">
         <is>
-          <t>Anton 48</t>
+          <t>Rixxy</t>
         </is>
       </c>
       <c r="B51" s="49" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C51" s="48">

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-26
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3266,13 +3266,13 @@
         <v/>
       </c>
       <c r="E49" s="35" t="n">
-        <v>56275</v>
+        <v>58125</v>
       </c>
       <c r="F49" s="35" t="n"/>
       <c r="G49" s="37" t="n"/>
       <c r="H49" s="37" t="n"/>
       <c r="I49" s="37" t="n">
-        <v>400</v>
+        <v>2250</v>
       </c>
       <c r="J49" s="37" t="n"/>
       <c r="K49" s="37" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-26
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3354,7 +3354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
@@ -3982,7 +3982,7 @@
         <v>6</v>
       </c>
       <c r="M9" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N9" s="48" t="n"/>
       <c r="O9" s="48" t="n"/>
@@ -4110,7 +4110,7 @@
         <v>6</v>
       </c>
       <c r="M11" s="48" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N11" s="48" t="n"/>
       <c r="O11" s="48" t="n"/>
@@ -4574,7 +4574,7 @@
         <v>2</v>
       </c>
       <c r="M19" s="48" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N19" s="48" t="n"/>
       <c r="O19" s="48" t="n"/>
@@ -4660,47 +4660,31 @@
     <row r="21">
       <c r="A21" s="48" t="inlineStr">
         <is>
-          <t>giosan</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B21" s="49" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C21" s="48">
         <f>ROUND(AVERAGE(D21:AH21), 0)</f>
         <v/>
       </c>
-      <c r="D21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="E21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="G21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="H21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="I21" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="J21" s="50" t="n">
-        <v>6</v>
-      </c>
-      <c r="K21" s="50" t="n">
-        <v>6</v>
-      </c>
+      <c r="D21" s="48" t="n"/>
+      <c r="E21" s="48" t="n"/>
+      <c r="F21" s="48" t="n"/>
+      <c r="G21" s="48" t="n"/>
+      <c r="H21" s="48" t="n"/>
+      <c r="I21" s="48" t="n"/>
+      <c r="J21" s="48" t="n"/>
+      <c r="K21" s="48" t="n"/>
       <c r="L21" s="51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M21" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N21" s="48" t="n"/>
       <c r="O21" s="48" t="n"/>
@@ -4727,26 +4711,42 @@
     <row r="22">
       <c r="A22" s="44" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B22" s="45" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C22" s="44">
         <f>ROUND(AVERAGE(D22:AH22), 0)</f>
         <v/>
       </c>
-      <c r="D22" s="44" t="n"/>
-      <c r="E22" s="44" t="n"/>
-      <c r="F22" s="44" t="n"/>
-      <c r="G22" s="44" t="n"/>
-      <c r="H22" s="44" t="n"/>
-      <c r="I22" s="44" t="n"/>
-      <c r="J22" s="44" t="n"/>
-      <c r="K22" s="44" t="n"/>
+      <c r="D22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="H22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="I22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="J22" s="46" t="n">
+        <v>6</v>
+      </c>
+      <c r="K22" s="46" t="n">
+        <v>6</v>
+      </c>
       <c r="L22" s="47" t="n">
         <v>6</v>
       </c>
@@ -4778,7 +4778,7 @@
     <row r="23">
       <c r="A23" s="48" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B23" s="49" t="inlineStr">
@@ -4800,25 +4800,23 @@
         <v>6</v>
       </c>
       <c r="G23" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H23" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="I23" s="48" t="n">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I23" s="48" t="n"/>
       <c r="J23" s="50" t="n">
         <v>6</v>
       </c>
       <c r="K23" s="50" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L23" s="51" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M23" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N23" s="48" t="n"/>
       <c r="O23" s="48" t="n"/>
@@ -4845,7 +4843,7 @@
     <row r="24">
       <c r="A24" s="44" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B24" s="45" t="inlineStr">
@@ -4867,23 +4865,25 @@
         <v>6</v>
       </c>
       <c r="G24" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H24" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="44" t="n"/>
+        <v>6</v>
+      </c>
+      <c r="I24" s="44" t="n">
+        <v>6</v>
+      </c>
       <c r="J24" s="46" t="n">
         <v>6</v>
       </c>
       <c r="K24" s="46" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L24" s="47" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N24" s="44" t="n"/>
       <c r="O24" s="44" t="n"/>
@@ -4910,7 +4910,7 @@
     <row r="25">
       <c r="A25" s="48" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B25" s="49" t="inlineStr">
@@ -4922,17 +4922,11 @@
         <f>ROUND(AVERAGE(D25:AH25), 0)</f>
         <v/>
       </c>
-      <c r="D25" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="E25" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F25" s="48" t="n">
-        <v>6</v>
-      </c>
+      <c r="D25" s="48" t="n"/>
+      <c r="E25" s="48" t="n"/>
+      <c r="F25" s="48" t="n"/>
       <c r="G25" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H25" s="48" t="n">
         <v>6</v>
@@ -4977,7 +4971,7 @@
     <row r="26">
       <c r="A26" s="44" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B26" s="45" t="inlineStr">
@@ -4989,29 +4983,35 @@
         <f>ROUND(AVERAGE(D26:AH26), 0)</f>
         <v/>
       </c>
-      <c r="D26" s="44" t="n"/>
-      <c r="E26" s="44" t="n"/>
-      <c r="F26" s="44" t="n"/>
+      <c r="D26" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="44" t="n">
+        <v>6</v>
+      </c>
       <c r="G26" s="44" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="44" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I26" s="44" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J26" s="46" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K26" s="46" t="n">
         <v>6</v>
       </c>
       <c r="L26" s="47" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M26" s="44" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N26" s="44" t="n"/>
       <c r="O26" s="44" t="n"/>
@@ -5038,7 +5038,7 @@
     <row r="27">
       <c r="A27" s="48" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B27" s="49" t="inlineStr">
@@ -5063,16 +5063,16 @@
         <v>0</v>
       </c>
       <c r="H27" s="48" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I27" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J27" s="50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K27" s="50" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L27" s="51" t="n">
         <v>0</v>
@@ -5105,7 +5105,7 @@
     <row r="28">
       <c r="A28" s="44" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>marcojk007</t>
         </is>
       </c>
       <c r="B28" s="45" t="inlineStr">
@@ -5117,26 +5117,20 @@
         <f>ROUND(AVERAGE(D28:AH28), 0)</f>
         <v/>
       </c>
-      <c r="D28" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="E28" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="44" t="n">
-        <v>6</v>
-      </c>
+      <c r="D28" s="44" t="n"/>
+      <c r="E28" s="44" t="n"/>
+      <c r="F28" s="44" t="n"/>
       <c r="G28" s="44" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I28" s="44" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J28" s="46" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K28" s="46" t="n">
         <v>0</v>
@@ -5172,12 +5166,12 @@
     <row r="29">
       <c r="A29" s="48" t="inlineStr">
         <is>
-          <t>marcojk007</t>
+          <t>MASCHI</t>
         </is>
       </c>
       <c r="B29" s="49" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>29/12/2025</t>
         </is>
       </c>
       <c r="C29" s="48">
@@ -5187,26 +5181,20 @@
       <c r="D29" s="48" t="n"/>
       <c r="E29" s="48" t="n"/>
       <c r="F29" s="48" t="n"/>
-      <c r="G29" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="48" t="n">
-        <v>0</v>
-      </c>
+      <c r="G29" s="48" t="n"/>
+      <c r="H29" s="48" t="n"/>
+      <c r="I29" s="48" t="n"/>
       <c r="J29" s="50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K29" s="50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L29" s="51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M29" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N29" s="48" t="n"/>
       <c r="O29" s="48" t="n"/>
@@ -5233,12 +5221,12 @@
     <row r="30">
       <c r="A30" s="44" t="inlineStr">
         <is>
-          <t>MASCHI</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B30" s="45" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C30" s="44">
@@ -5248,9 +5236,15 @@
       <c r="D30" s="44" t="n"/>
       <c r="E30" s="44" t="n"/>
       <c r="F30" s="44" t="n"/>
-      <c r="G30" s="44" t="n"/>
-      <c r="H30" s="44" t="n"/>
-      <c r="I30" s="44" t="n"/>
+      <c r="G30" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="H30" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="I30" s="44" t="n">
+        <v>6</v>
+      </c>
       <c r="J30" s="46" t="n">
         <v>6</v>
       </c>
@@ -5288,7 +5282,7 @@
     <row r="31">
       <c r="A31" s="48" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B31" s="49" t="inlineStr">
@@ -5304,7 +5298,7 @@
       <c r="E31" s="48" t="n"/>
       <c r="F31" s="48" t="n"/>
       <c r="G31" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H31" s="48" t="n">
         <v>6</v>
@@ -5349,12 +5343,12 @@
     <row r="32">
       <c r="A32" s="44" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B32" s="45" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C32" s="44">
@@ -5364,21 +5358,11 @@
       <c r="D32" s="44" t="n"/>
       <c r="E32" s="44" t="n"/>
       <c r="F32" s="44" t="n"/>
-      <c r="G32" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="I32" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="J32" s="46" t="n">
-        <v>6</v>
-      </c>
-      <c r="K32" s="46" t="n">
-        <v>6</v>
-      </c>
+      <c r="G32" s="44" t="n"/>
+      <c r="H32" s="44" t="n"/>
+      <c r="I32" s="44" t="n"/>
+      <c r="J32" s="44" t="n"/>
+      <c r="K32" s="44" t="n"/>
       <c r="L32" s="47" t="n">
         <v>6</v>
       </c>
@@ -5410,12 +5394,12 @@
     <row r="33">
       <c r="A33" s="48" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B33" s="49" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C33" s="48">
@@ -5429,7 +5413,9 @@
       <c r="H33" s="48" t="n"/>
       <c r="I33" s="48" t="n"/>
       <c r="J33" s="48" t="n"/>
-      <c r="K33" s="48" t="n"/>
+      <c r="K33" s="50" t="n">
+        <v>6</v>
+      </c>
       <c r="L33" s="51" t="n">
         <v>6</v>
       </c>
@@ -5461,25 +5447,39 @@
     <row r="34">
       <c r="A34" s="44" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B34" s="45" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C34" s="44">
         <f>ROUND(AVERAGE(D34:AH34), 0)</f>
         <v/>
       </c>
-      <c r="D34" s="44" t="n"/>
-      <c r="E34" s="44" t="n"/>
-      <c r="F34" s="44" t="n"/>
-      <c r="G34" s="44" t="n"/>
-      <c r="H34" s="44" t="n"/>
-      <c r="I34" s="44" t="n"/>
-      <c r="J34" s="44" t="n"/>
+      <c r="D34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="H34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="I34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" s="46" t="n">
+        <v>6</v>
+      </c>
       <c r="K34" s="46" t="n">
         <v>6</v>
       </c>
@@ -5514,7 +5514,7 @@
     <row r="35">
       <c r="A35" s="48" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B35" s="49" t="inlineStr">
@@ -5527,7 +5527,7 @@
         <v/>
       </c>
       <c r="D35" s="48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="48" t="n">
         <v>6</v>
@@ -5539,7 +5539,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I35" s="48" t="n">
         <v>6</v>
@@ -5554,7 +5554,7 @@
         <v>6</v>
       </c>
       <c r="M35" s="48" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N35" s="48" t="n"/>
       <c r="O35" s="48" t="n"/>
@@ -5581,7 +5581,7 @@
     <row r="36">
       <c r="A36" s="44" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B36" s="45" t="inlineStr">
@@ -5594,7 +5594,7 @@
         <v/>
       </c>
       <c r="D36" s="44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E36" s="44" t="n">
         <v>6</v>
@@ -5606,7 +5606,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I36" s="44" t="n">
         <v>6</v>
@@ -5648,7 +5648,7 @@
     <row r="37">
       <c r="A37" s="48" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B37" s="49" t="inlineStr">
@@ -5661,7 +5661,7 @@
         <v/>
       </c>
       <c r="D37" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E37" s="48" t="n">
         <v>6</v>
@@ -5679,7 +5679,7 @@
         <v>6</v>
       </c>
       <c r="J37" s="50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K37" s="50" t="n">
         <v>6</v>
@@ -5715,7 +5715,7 @@
     <row r="38">
       <c r="A38" s="44" t="inlineStr">
         <is>
-          <t>sidcu js</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B38" s="45" t="inlineStr">
@@ -5749,13 +5749,13 @@
         <v>6</v>
       </c>
       <c r="K38" s="46" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L38" s="47" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M38" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N38" s="44" t="n"/>
       <c r="O38" s="44" t="n"/>
@@ -5782,7 +5782,7 @@
     <row r="39">
       <c r="A39" s="48" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B39" s="49" t="inlineStr">
@@ -5794,26 +5794,20 @@
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
-      <c r="D39" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" s="48" t="n">
-        <v>6</v>
-      </c>
+      <c r="D39" s="48" t="n"/>
+      <c r="E39" s="48" t="n"/>
+      <c r="F39" s="48" t="n"/>
       <c r="G39" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H39" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I39" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J39" s="50" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K39" s="50" t="n">
         <v>6</v>
@@ -5822,7 +5816,7 @@
         <v>6</v>
       </c>
       <c r="M39" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N39" s="48" t="n"/>
       <c r="O39" s="48" t="n"/>
@@ -5849,39 +5843,25 @@
     <row r="40">
       <c r="A40" s="44" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>tazio</t>
         </is>
       </c>
       <c r="B40" s="45" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C40" s="44">
         <f>ROUND(AVERAGE(D40:AH40), 0)</f>
         <v/>
       </c>
-      <c r="D40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="E40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="G40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="H40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="I40" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="J40" s="46" t="n">
-        <v>6</v>
-      </c>
+      <c r="D40" s="44" t="n"/>
+      <c r="E40" s="44" t="n"/>
+      <c r="F40" s="44" t="n"/>
+      <c r="G40" s="44" t="n"/>
+      <c r="H40" s="44" t="n"/>
+      <c r="I40" s="44" t="n"/>
+      <c r="J40" s="44" t="n"/>
       <c r="K40" s="46" t="n">
         <v>6</v>
       </c>
@@ -5916,7 +5896,7 @@
     <row r="41">
       <c r="A41" s="48" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B41" s="49" t="inlineStr">
@@ -5928,26 +5908,32 @@
         <f>ROUND(AVERAGE(D41:AH41), 0)</f>
         <v/>
       </c>
-      <c r="D41" s="48" t="n"/>
-      <c r="E41" s="48" t="n"/>
-      <c r="F41" s="48" t="n"/>
+      <c r="D41" s="48" t="n">
+        <v>6</v>
+      </c>
+      <c r="E41" s="48" t="n">
+        <v>6</v>
+      </c>
+      <c r="F41" s="48" t="n">
+        <v>6</v>
+      </c>
       <c r="G41" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I41" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J41" s="50" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K41" s="50" t="n">
         <v>6</v>
       </c>
       <c r="L41" s="51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M41" s="48" t="n">
         <v>6</v>
@@ -5977,12 +5963,12 @@
     <row r="42">
       <c r="A42" s="44" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B42" s="45" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C42" s="44">
@@ -5992,12 +5978,20 @@
       <c r="D42" s="44" t="n"/>
       <c r="E42" s="44" t="n"/>
       <c r="F42" s="44" t="n"/>
-      <c r="G42" s="44" t="n"/>
-      <c r="H42" s="44" t="n"/>
-      <c r="I42" s="44" t="n"/>
-      <c r="J42" s="44" t="n"/>
+      <c r="G42" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="46" t="n">
+        <v>0</v>
+      </c>
       <c r="K42" s="46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L42" s="47" t="n">
         <v>6</v>
@@ -6030,7 +6024,7 @@
     <row r="43">
       <c r="A43" s="48" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B43" s="49" t="inlineStr">
@@ -6042,15 +6036,9 @@
         <f>ROUND(AVERAGE(D43:AH43), 0)</f>
         <v/>
       </c>
-      <c r="D43" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="E43" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F43" s="48" t="n">
-        <v>6</v>
-      </c>
+      <c r="D43" s="48" t="n"/>
+      <c r="E43" s="48" t="n"/>
+      <c r="F43" s="48" t="n"/>
       <c r="G43" s="48" t="n">
         <v>6</v>
       </c>
@@ -6067,7 +6055,7 @@
         <v>6</v>
       </c>
       <c r="L43" s="51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M43" s="48" t="n">
         <v>6</v>
@@ -6097,7 +6085,7 @@
     <row r="44">
       <c r="A44" s="44" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>zombra</t>
         </is>
       </c>
       <c r="B44" s="45" t="inlineStr">
@@ -6110,16 +6098,20 @@
         <v/>
       </c>
       <c r="D44" s="44" t="n"/>
-      <c r="E44" s="44" t="n"/>
-      <c r="F44" s="44" t="n"/>
+      <c r="E44" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" s="44" t="n">
+        <v>6</v>
+      </c>
       <c r="G44" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H44" s="44" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J44" s="46" t="n">
         <v>0</v>
@@ -6128,7 +6120,7 @@
         <v>5</v>
       </c>
       <c r="L44" s="47" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M44" s="44" t="n">
         <v>0</v>
@@ -6158,12 +6150,12 @@
     <row r="45">
       <c r="A45" s="48" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B45" s="49" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C45" s="48">
@@ -6173,18 +6165,10 @@
       <c r="D45" s="48" t="n"/>
       <c r="E45" s="48" t="n"/>
       <c r="F45" s="48" t="n"/>
-      <c r="G45" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="H45" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="I45" s="48" t="n">
-        <v>6</v>
-      </c>
-      <c r="J45" s="50" t="n">
-        <v>6</v>
-      </c>
+      <c r="G45" s="48" t="n"/>
+      <c r="H45" s="48" t="n"/>
+      <c r="I45" s="48" t="n"/>
+      <c r="J45" s="48" t="n"/>
       <c r="K45" s="50" t="n">
         <v>6</v>
       </c>
@@ -6192,7 +6176,7 @@
         <v>6</v>
       </c>
       <c r="M45" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N45" s="48" t="n"/>
       <c r="O45" s="48" t="n"/>
@@ -6219,12 +6203,12 @@
     <row r="46">
       <c r="A46" s="44" t="inlineStr">
         <is>
-          <t>zombra</t>
+          <t>DARKGOST9</t>
         </is>
       </c>
       <c r="B46" s="45" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>24/01/2026</t>
         </is>
       </c>
       <c r="C46" s="44">
@@ -6232,30 +6216,14 @@
         <v/>
       </c>
       <c r="D46" s="44" t="n"/>
-      <c r="E46" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="F46" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="G46" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="H46" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="J46" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" s="46" t="n">
-        <v>5</v>
-      </c>
-      <c r="L46" s="47" t="n">
-        <v>2</v>
-      </c>
+      <c r="E46" s="44" t="n"/>
+      <c r="F46" s="44" t="n"/>
+      <c r="G46" s="44" t="n"/>
+      <c r="H46" s="44" t="n"/>
+      <c r="I46" s="44" t="n"/>
+      <c r="J46" s="44" t="n"/>
+      <c r="K46" s="46" t="n"/>
+      <c r="L46" s="47" t="n"/>
       <c r="M46" s="44" t="n">
         <v>0</v>
       </c>
@@ -6284,12 +6252,12 @@
     <row r="47">
       <c r="A47" s="48" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B47" s="49" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C47" s="48">
@@ -6303,14 +6271,10 @@
       <c r="H47" s="48" t="n"/>
       <c r="I47" s="48" t="n"/>
       <c r="J47" s="48" t="n"/>
-      <c r="K47" s="50" t="n">
-        <v>6</v>
-      </c>
-      <c r="L47" s="51" t="n">
-        <v>6</v>
-      </c>
+      <c r="K47" s="50" t="n"/>
+      <c r="L47" s="51" t="n"/>
       <c r="M47" s="48" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N47" s="48" t="n"/>
       <c r="O47" s="48" t="n"/>
@@ -6337,12 +6301,12 @@
     <row r="48">
       <c r="A48" s="44" t="inlineStr">
         <is>
-          <t>DARKGOST9</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B48" s="45" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C48" s="44">
@@ -6359,7 +6323,7 @@
       <c r="K48" s="46" t="n"/>
       <c r="L48" s="47" t="n"/>
       <c r="M48" s="44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N48" s="44" t="n"/>
       <c r="O48" s="44" t="n"/>
@@ -6386,7 +6350,7 @@
     <row r="49">
       <c r="A49" s="48" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Rixxy</t>
         </is>
       </c>
       <c r="B49" s="49" t="inlineStr">
@@ -6408,7 +6372,7 @@
       <c r="K49" s="50" t="n"/>
       <c r="L49" s="51" t="n"/>
       <c r="M49" s="48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N49" s="48" t="n"/>
       <c r="O49" s="48" t="n"/>
@@ -6435,12 +6399,12 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="44" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>luffy</t>
         </is>
       </c>
       <c r="B50" s="45" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>26/01/2026</t>
         </is>
       </c>
       <c r="C50" s="44">
@@ -6457,7 +6421,7 @@
       <c r="K50" s="46" t="n"/>
       <c r="L50" s="47" t="n"/>
       <c r="M50" s="44" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N50" s="44" t="n"/>
       <c r="O50" s="44" t="n"/>
@@ -6480,55 +6444,6 @@
       <c r="AF50" s="44" t="n"/>
       <c r="AG50" s="44" t="n"/>
       <c r="AH50" s="44" t="n"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="48" t="inlineStr">
-        <is>
-          <t>Rixxy</t>
-        </is>
-      </c>
-      <c r="B51" s="49" t="inlineStr">
-        <is>
-          <t>25/01/2026</t>
-        </is>
-      </c>
-      <c r="C51" s="48">
-        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
-        <v/>
-      </c>
-      <c r="D51" s="48" t="n"/>
-      <c r="E51" s="48" t="n"/>
-      <c r="F51" s="48" t="n"/>
-      <c r="G51" s="48" t="n"/>
-      <c r="H51" s="48" t="n"/>
-      <c r="I51" s="48" t="n"/>
-      <c r="J51" s="48" t="n"/>
-      <c r="K51" s="50" t="n"/>
-      <c r="L51" s="51" t="n"/>
-      <c r="M51" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" s="48" t="n"/>
-      <c r="O51" s="48" t="n"/>
-      <c r="P51" s="48" t="n"/>
-      <c r="Q51" s="48" t="n"/>
-      <c r="R51" s="48" t="n"/>
-      <c r="S51" s="48" t="n"/>
-      <c r="T51" s="48" t="n"/>
-      <c r="U51" s="48" t="n"/>
-      <c r="V51" s="48" t="n"/>
-      <c r="W51" s="48" t="n"/>
-      <c r="X51" s="48" t="n"/>
-      <c r="Y51" s="48" t="n"/>
-      <c r="Z51" s="48" t="n"/>
-      <c r="AA51" s="48" t="n"/>
-      <c r="AB51" s="48" t="n"/>
-      <c r="AC51" s="48" t="n"/>
-      <c r="AD51" s="48" t="n"/>
-      <c r="AE51" s="48" t="n"/>
-      <c r="AF51" s="48" t="n"/>
-      <c r="AG51" s="48" t="n"/>
-      <c r="AH51" s="48" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AT1">

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-27
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -1247,7 +1247,7 @@
         <v/>
       </c>
       <c r="E8" s="39" t="n">
-        <v>68750</v>
+        <v>69750</v>
       </c>
       <c r="F8" s="39" t="n"/>
       <c r="G8" s="41" t="n"/>
@@ -1255,7 +1255,7 @@
         <v>1300</v>
       </c>
       <c r="I8" s="41" t="n">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="J8" s="41" t="n"/>
       <c r="K8" s="41" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-01-28
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -1439,7 +1439,7 @@
         <v/>
       </c>
       <c r="E13" s="25" t="n">
-        <v>70150</v>
+        <v>70250</v>
       </c>
       <c r="F13" s="33" t="n"/>
       <c r="G13" s="33" t="n"/>
@@ -1447,7 +1447,7 @@
         <v>1300</v>
       </c>
       <c r="I13" s="33" t="n">
-        <v>3900</v>
+        <v>4000</v>
       </c>
       <c r="J13" s="33" t="n"/>
       <c r="K13" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-01-31
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3246,7 +3246,7 @@
       </c>
       <c r="N1" s="7" t="inlineStr">
         <is>
-          <t>Colonna12</t>
+          <t>30/01/2026</t>
         </is>
       </c>
       <c r="O1" s="7" t="inlineStr">
@@ -3377,6 +3377,9 @@
       <c r="M2" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="inlineStr">
@@ -3402,6 +3405,9 @@
       <c r="M3" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="inlineStr">
@@ -3448,6 +3454,9 @@
       <c r="M4" s="9" t="n">
         <v>6</v>
       </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="14" t="inlineStr">
@@ -3476,6 +3485,9 @@
       <c r="M5" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="14" t="inlineStr">
@@ -3498,6 +3510,9 @@
       <c r="M6" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="14" t="inlineStr">
@@ -3520,6 +3535,9 @@
       <c r="M7" s="9" t="n">
         <v>6</v>
       </c>
+      <c r="N7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="inlineStr">
@@ -3557,6 +3575,9 @@
       <c r="M8" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="14" t="inlineStr">
@@ -3603,6 +3624,9 @@
       <c r="M9" s="9" t="n">
         <v>6</v>
       </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="14" t="inlineStr">
@@ -3649,6 +3673,9 @@
       <c r="M10" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="14" t="inlineStr">
@@ -3686,32 +3713,54 @@
       <c r="M11" s="9" t="n">
         <v>5</v>
       </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="14" t="inlineStr">
         <is>
-          <t>DARKGOST9</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B12" s="16" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C12" s="14">
         <f>ROUND(AVERAGE(D12:AH12), 0)</f>
         <v/>
       </c>
-      <c r="K12" s="10" t="n"/>
-      <c r="L12" s="11" t="n"/>
+      <c r="G12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="11" t="n">
+        <v>6</v>
+      </c>
       <c r="M12" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="14" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>ER DANDI 1927</t>
         </is>
       </c>
       <c r="B13" s="16" t="inlineStr">
@@ -3724,31 +3773,34 @@
         <v/>
       </c>
       <c r="G13" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H13" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I13" s="9" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L13" s="11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M13" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="14" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B14" s="16" t="inlineStr">
@@ -3760,164 +3812,188 @@
         <f>ROUND(AVERAGE(D14:AH14), 0)</f>
         <v/>
       </c>
+      <c r="D14" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G14" s="9" t="n">
         <v>5</v>
       </c>
       <c r="H14" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I14" s="9" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K14" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L14" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M14" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="14" t="inlineStr">
         <is>
-          <t>fabiovesco</t>
+          <t>francesco</t>
         </is>
       </c>
       <c r="B15" s="16" t="inlineStr">
         <is>
-          <t>19/01/2026</t>
+          <t>17/01/2026</t>
         </is>
       </c>
       <c r="C15" s="14">
         <f>ROUND(AVERAGE(D15:AH15), 0)</f>
         <v/>
       </c>
+      <c r="L15" s="9" t="n">
+        <v>0</v>
+      </c>
       <c r="M15" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="14" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>Fryck</t>
         </is>
       </c>
       <c r="B16" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C16" s="14">
         <f>ROUND(AVERAGE(D16:AH16), 0)</f>
         <v/>
       </c>
-      <c r="D16" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G16" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="H16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J16" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K16" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L16" s="11" t="n">
-        <v>6</v>
+      <c r="L16" s="9" t="n">
+        <v>2</v>
       </c>
       <c r="M16" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="14" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B17" s="16" t="inlineStr">
         <is>
-          <t>17/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C17" s="14">
         <f>ROUND(AVERAGE(D17:AH17), 0)</f>
         <v/>
       </c>
-      <c r="L17" s="9" t="n">
-        <v>0</v>
+      <c r="D17" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J17" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K17" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L17" s="11" t="n">
+        <v>6</v>
       </c>
       <c r="M17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="14" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B18" s="16" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>29/12/2025</t>
         </is>
       </c>
       <c r="C18" s="14">
         <f>ROUND(AVERAGE(D18:AH18), 0)</f>
         <v/>
       </c>
-      <c r="L18" s="9" t="n">
+      <c r="I18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J18" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K18" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L18" s="11" t="n">
         <v>2</v>
       </c>
       <c r="M18" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="14" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B19" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C19" s="14">
         <f>ROUND(AVERAGE(D19:AH19), 0)</f>
         <v/>
       </c>
-      <c r="D19" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G19" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="H19" s="9" t="n">
         <v>6</v>
       </c>
@@ -3934,55 +4010,64 @@
         <v>6</v>
       </c>
       <c r="M19" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N19" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="14" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B20" s="16" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C20" s="14">
         <f>ROUND(AVERAGE(D20:AH20), 0)</f>
         <v/>
       </c>
-      <c r="I20" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J20" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K20" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L20" s="11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N20" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="14" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B21" s="16" t="inlineStr">
         <is>
-          <t>21/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C21" s="14">
         <f>ROUND(AVERAGE(D21:AH21), 0)</f>
         <v/>
       </c>
+      <c r="D21" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="H21" s="9" t="n">
         <v>6</v>
       </c>
@@ -4000,80 +4085,85 @@
       </c>
       <c r="M21" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="14" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B22" s="16" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C22" s="14">
         <f>ROUND(AVERAGE(D22:AH22), 0)</f>
         <v/>
       </c>
+      <c r="D22" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K22" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="L22" s="11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M22" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="14" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B23" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C23" s="14">
         <f>ROUND(AVERAGE(D23:AH23), 0)</f>
         <v/>
       </c>
-      <c r="D23" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E23" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F23" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G23" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H23" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I23" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J23" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K23" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L23" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="K23" s="10" t="n"/>
+      <c r="L23" s="11" t="n"/>
       <c r="M23" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="14" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B24" s="16" t="inlineStr">
@@ -4095,28 +4185,34 @@
         <v>6</v>
       </c>
       <c r="G24" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H24" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="I24" s="9" t="n">
+        <v>6</v>
       </c>
       <c r="J24" s="10" t="n">
         <v>6</v>
       </c>
       <c r="K24" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L24" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="14" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B25" s="16" t="inlineStr">
@@ -4133,11 +4229,14 @@
       <c r="M25" s="9" t="n">
         <v>6</v>
       </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="14" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B26" s="16" t="inlineStr">
@@ -4149,17 +4248,8 @@
         <f>ROUND(AVERAGE(D26:AH26), 0)</f>
         <v/>
       </c>
-      <c r="D26" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E26" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G26" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H26" s="9" t="n">
         <v>6</v>
@@ -4178,54 +4268,113 @@
       </c>
       <c r="M26" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="14" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B27" s="16" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C27" s="14">
         <f>ROUND(AVERAGE(D27:AH27), 0)</f>
         <v/>
       </c>
-      <c r="K27" s="10" t="n"/>
-      <c r="L27" s="11" t="n"/>
+      <c r="D27" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L27" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="M27" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="14" t="inlineStr">
         <is>
-          <t>luffy</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B28" s="16" t="inlineStr">
         <is>
-          <t>26/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C28" s="14">
         <f>ROUND(AVERAGE(D28:AH28), 0)</f>
         <v/>
       </c>
-      <c r="K28" s="10" t="n"/>
-      <c r="L28" s="11" t="n"/>
+      <c r="D28" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="I28" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J28" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="M28" s="9" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="14" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B29" s="16" t="inlineStr">
@@ -4238,7 +4387,7 @@
         <v/>
       </c>
       <c r="G29" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H29" s="9" t="n">
         <v>6</v>
@@ -4257,12 +4406,15 @@
       </c>
       <c r="M29" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="14" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B30" s="16" t="inlineStr">
@@ -4274,135 +4426,117 @@
         <f>ROUND(AVERAGE(D30:AH30), 0)</f>
         <v/>
       </c>
-      <c r="D30" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E30" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G30" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I30" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J30" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K30" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L30" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M30" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N30" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="14" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B31" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C31" s="14">
         <f>ROUND(AVERAGE(D31:AH31), 0)</f>
         <v/>
       </c>
-      <c r="D31" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E31" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J31" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K31" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="L31" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="14" t="inlineStr">
         <is>
-          <t>marcojk007</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B32" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C32" s="14">
         <f>ROUND(AVERAGE(D32:AH32), 0)</f>
         <v/>
       </c>
-      <c r="G32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="K32" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L32" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M32" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N32" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="14" t="inlineStr">
         <is>
-          <t>MASCHI</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B33" s="16" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C33" s="14">
         <f>ROUND(AVERAGE(D33:AH33), 0)</f>
         <v/>
       </c>
+      <c r="D33" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F33" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G33" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H33" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I33" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="J33" s="10" t="n">
         <v>6</v>
       </c>
@@ -4414,12 +4548,15 @@
       </c>
       <c r="M33" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="14" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B34" s="16" t="inlineStr">
@@ -4431,11 +4568,20 @@
         <f>ROUND(AVERAGE(D34:AH34), 0)</f>
         <v/>
       </c>
+      <c r="D34" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G34" s="9" t="n">
         <v>6</v>
       </c>
       <c r="H34" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34" s="9" t="n">
         <v>6</v>
@@ -4450,13 +4596,16 @@
         <v>6</v>
       </c>
       <c r="M34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N34" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="14" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B35" s="16" t="inlineStr">
@@ -4468,8 +4617,17 @@
         <f>ROUND(AVERAGE(D35:AH35), 0)</f>
         <v/>
       </c>
+      <c r="D35" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F35" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G35" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H35" s="9" t="n">
         <v>6</v>
@@ -4487,46 +4645,97 @@
         <v>6</v>
       </c>
       <c r="M35" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N35" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="14" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B36" s="16" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C36" s="14">
         <f>ROUND(AVERAGE(D36:AH36), 0)</f>
         <v/>
       </c>
+      <c r="D36" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="K36" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L36" s="11" t="n">
         <v>6</v>
       </c>
       <c r="M36" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="14" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B37" s="16" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C37" s="14">
         <f>ROUND(AVERAGE(D37:AH37), 0)</f>
         <v/>
       </c>
+      <c r="D37" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J37" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K37" s="10" t="n">
         <v>6</v>
       </c>
@@ -4534,66 +4743,67 @@
         <v>6</v>
       </c>
       <c r="M37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N37" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="14" t="inlineStr">
         <is>
-          <t>Rixxy</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B38" s="16" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C38" s="14">
         <f>ROUND(AVERAGE(D38:AH38), 0)</f>
         <v/>
       </c>
-      <c r="K38" s="10" t="n"/>
-      <c r="L38" s="11" t="n"/>
+      <c r="G38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L38" s="11" t="n">
+        <v>6</v>
+      </c>
       <c r="M38" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="N38" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="14" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>tazio</t>
         </is>
       </c>
       <c r="B39" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C39" s="14">
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
-      <c r="D39" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J39" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K39" s="10" t="n">
         <v>6</v>
       </c>
@@ -4602,12 +4812,15 @@
       </c>
       <c r="M39" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="14" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B40" s="16" t="inlineStr">
@@ -4620,40 +4833,43 @@
         <v/>
       </c>
       <c r="D40" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J40" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K40" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L40" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="E40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H40" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J40" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K40" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L40" s="11" t="n">
-        <v>6</v>
-      </c>
       <c r="M40" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="14" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B41" s="16" t="inlineStr">
@@ -4665,41 +4881,35 @@
         <f>ROUND(AVERAGE(D41:AH41), 0)</f>
         <v/>
       </c>
-      <c r="D41" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E41" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F41" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G41" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H41" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I41" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J41" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K41" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L41" s="11" t="n">
         <v>6</v>
       </c>
       <c r="M41" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="14" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B42" s="16" t="inlineStr">
@@ -4711,15 +4921,6 @@
         <f>ROUND(AVERAGE(D42:AH42), 0)</f>
         <v/>
       </c>
-      <c r="D42" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F42" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G42" s="9" t="n">
         <v>6</v>
       </c>
@@ -4730,7 +4931,7 @@
         <v>6</v>
       </c>
       <c r="J42" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K42" s="10" t="n">
         <v>6</v>
@@ -4740,44 +4941,26 @@
       </c>
       <c r="M42" s="9" t="n">
         <v>6</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="14" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B43" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C43" s="14">
         <f>ROUND(AVERAGE(D43:AH43), 0)</f>
         <v/>
       </c>
-      <c r="D43" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E43" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F43" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G43" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H43" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I43" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J43" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K43" s="10" t="n">
         <v>6</v>
       </c>
@@ -4785,256 +4968,163 @@
         <v>6</v>
       </c>
       <c r="M43" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="14" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>K A N E K I</t>
         </is>
       </c>
       <c r="B44" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C44" s="14">
         <f>ROUND(AVERAGE(D44:AH44), 0)</f>
         <v/>
       </c>
-      <c r="G44" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L44" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="M44" s="9" t="n">
-        <v>6</v>
+      <c r="K44" s="10" t="n"/>
+      <c r="L44" s="11" t="n"/>
+      <c r="M44" s="9" t="n"/>
+      <c r="N44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="14" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>tuspostati</t>
         </is>
       </c>
       <c r="B45" s="16" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C45" s="14">
         <f>ROUND(AVERAGE(D45:AH45), 0)</f>
         <v/>
       </c>
-      <c r="K45" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L45" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="M45" s="9" t="n">
-        <v>6</v>
+      <c r="K45" s="10" t="n"/>
+      <c r="L45" s="11" t="n"/>
+      <c r="M45" s="9" t="n"/>
+      <c r="N45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="14" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Leonida</t>
         </is>
       </c>
       <c r="B46" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C46" s="14">
         <f>ROUND(AVERAGE(D46:AH46), 0)</f>
         <v/>
       </c>
-      <c r="D46" s="15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E46" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F46" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G46" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H46" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I46" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J46" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K46" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L46" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="M46" s="9" t="n">
-        <v>6</v>
+      <c r="K46" s="10" t="n"/>
+      <c r="L46" s="11" t="n"/>
+      <c r="M46" s="9" t="n"/>
+      <c r="N46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="14" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>Diti</t>
         </is>
       </c>
       <c r="B47" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C47" s="14">
         <f>ROUND(AVERAGE(D47:AH47), 0)</f>
         <v/>
       </c>
-      <c r="G47" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J47" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L47" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="M47" s="9" t="n">
-        <v>6</v>
+      <c r="K47" s="10" t="n"/>
+      <c r="L47" s="11" t="n"/>
+      <c r="M47" s="9" t="n"/>
+      <c r="N47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="14" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>IL MAGO NERO</t>
         </is>
       </c>
       <c r="B48" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C48" s="14">
         <f>ROUND(AVERAGE(D48:AH48), 0)</f>
         <v/>
       </c>
-      <c r="G48" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H48" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I48" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J48" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K48" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L48" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="M48" s="9" t="n">
-        <v>6</v>
+      <c r="K48" s="10" t="n"/>
+      <c r="L48" s="11" t="n"/>
+      <c r="M48" s="9" t="n"/>
+      <c r="N48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="14" t="inlineStr">
         <is>
-          <t>zombra</t>
+          <t>NITHING</t>
         </is>
       </c>
       <c r="B49" s="16" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C49" s="14">
         <f>ROUND(AVERAGE(D49:AH49), 0)</f>
         <v/>
       </c>
-      <c r="E49" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F49" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G49" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H49" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L49" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="M49" s="9" t="n">
+      <c r="K49" s="10" t="n"/>
+      <c r="L49" s="11" t="n"/>
+      <c r="M49" s="9" t="n"/>
+      <c r="N49" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="34">
       <c r="A50" s="14" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>dast</t>
         </is>
       </c>
       <c r="B50" s="16" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>31/01/2026</t>
         </is>
       </c>
       <c r="C50" s="14">
         <f>ROUND(AVERAGE(D50:AH50), 0)</f>
         <v/>
       </c>
-      <c r="K50" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L50" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="M50" s="9" t="n">
+      <c r="K50" s="10" t="n"/>
+      <c r="L50" s="11" t="n"/>
+      <c r="M50" s="9" t="n"/>
+      <c r="N50" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-01
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3157,7 +3157,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH50"/>
+  <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:XFD31"/>
@@ -3511,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -3714,7 +3714,7 @@
         <v>5</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -4087,7 +4087,7 @@
         <v>6</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -4206,7 +4206,7 @@
         <v>6</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -4270,7 +4270,7 @@
         <v>6</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -4408,7 +4408,7 @@
         <v>6</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -4448,7 +4448,7 @@
         <v>6</v>
       </c>
       <c r="N30" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -4473,7 +4473,7 @@
         <v>6</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -4697,7 +4697,7 @@
         <v>6</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -4814,7 +4814,7 @@
         <v>6</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -4863,7 +4863,7 @@
         <v>6</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -4903,7 +4903,7 @@
         <v>6</v>
       </c>
       <c r="N41" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -4943,7 +4943,7 @@
         <v>6</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -5125,6 +5125,28 @@
       <c r="L50" s="11" t="n"/>
       <c r="M50" s="9" t="n"/>
       <c r="N50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="14" t="inlineStr">
+        <is>
+          <t>Darvix27</t>
+        </is>
+      </c>
+      <c r="B51" s="16" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="C51" s="14">
+        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
+        <v/>
+      </c>
+      <c r="K51" s="10" t="n"/>
+      <c r="L51" s="11" t="n"/>
+      <c r="M51" s="9" t="n"/>
+      <c r="N51" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-02
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3157,7 +3157,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:XFD31"/>
@@ -4999,7 +4999,7 @@
     <row r="45">
       <c r="A45" s="14" t="inlineStr">
         <is>
-          <t>tuspostati</t>
+          <t>Leonida</t>
         </is>
       </c>
       <c r="B45" s="16" t="inlineStr">
@@ -5021,7 +5021,7 @@
     <row r="46">
       <c r="A46" s="14" t="inlineStr">
         <is>
-          <t>Leonida</t>
+          <t>Diti</t>
         </is>
       </c>
       <c r="B46" s="16" t="inlineStr">
@@ -5043,7 +5043,7 @@
     <row r="47">
       <c r="A47" s="14" t="inlineStr">
         <is>
-          <t>Diti</t>
+          <t>IL MAGO NERO</t>
         </is>
       </c>
       <c r="B47" s="16" t="inlineStr">
@@ -5065,12 +5065,12 @@
     <row r="48">
       <c r="A48" s="14" t="inlineStr">
         <is>
-          <t>IL MAGO NERO</t>
+          <t>Darvix27</t>
         </is>
       </c>
       <c r="B48" s="16" t="inlineStr">
         <is>
-          <t>31/01/2026</t>
+          <t>01/02/2026</t>
         </is>
       </c>
       <c r="C48" s="14">
@@ -5087,12 +5087,12 @@
     <row r="49">
       <c r="A49" s="14" t="inlineStr">
         <is>
-          <t>NITHING</t>
+          <t>favretto</t>
         </is>
       </c>
       <c r="B49" s="16" t="inlineStr">
         <is>
-          <t>31/01/2026</t>
+          <t>02/02/2026</t>
         </is>
       </c>
       <c r="C49" s="14">
@@ -5102,19 +5102,16 @@
       <c r="K49" s="10" t="n"/>
       <c r="L49" s="11" t="n"/>
       <c r="M49" s="9" t="n"/>
-      <c r="N49" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1" s="34">
       <c r="A50" s="14" t="inlineStr">
         <is>
-          <t>dast</t>
+          <t>caccialama</t>
         </is>
       </c>
       <c r="B50" s="16" t="inlineStr">
         <is>
-          <t>31/01/2026</t>
+          <t>02/02/2026</t>
         </is>
       </c>
       <c r="C50" s="14">
@@ -5124,31 +5121,6 @@
       <c r="K50" s="10" t="n"/>
       <c r="L50" s="11" t="n"/>
       <c r="M50" s="9" t="n"/>
-      <c r="N50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="14" t="inlineStr">
-        <is>
-          <t>Darvix27</t>
-        </is>
-      </c>
-      <c r="B51" s="16" t="inlineStr">
-        <is>
-          <t>01/02/2026</t>
-        </is>
-      </c>
-      <c r="C51" s="14">
-        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
-        <v/>
-      </c>
-      <c r="K51" s="10" t="n"/>
-      <c r="L51" s="11" t="n"/>
-      <c r="M51" s="9" t="n"/>
-      <c r="N51" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AT1">

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-08
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3565,7 +3565,7 @@
         <v>4</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -4011,7 +4011,7 @@
         <v>6</v>
       </c>
       <c r="O18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -4329,7 +4329,7 @@
         <v>6</v>
       </c>
       <c r="O26" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -4433,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -4734,7 +4734,7 @@
         <v>6</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -4838,7 +4838,7 @@
         <v>6</v>
       </c>
       <c r="O37" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -4876,23 +4876,44 @@
     <row r="39">
       <c r="A39" s="13" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B39" s="15" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C39" s="13">
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
+      <c r="D39" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E39" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F39" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G39" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H39" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I39" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J39" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K39" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L39" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M39" s="9" t="n">
         <v>6</v>
@@ -4907,7 +4928,7 @@
     <row r="40">
       <c r="A40" s="13" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
@@ -4919,32 +4940,23 @@
         <f>ROUND(AVERAGE(D40:AH40), 0)</f>
         <v/>
       </c>
-      <c r="D40" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G40" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H40" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I40" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J40" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K40" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L40" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M40" s="9" t="n">
         <v>6</v>
@@ -4953,13 +4965,13 @@
         <v>6</v>
       </c>
       <c r="O40" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
@@ -4972,19 +4984,19 @@
         <v/>
       </c>
       <c r="G41" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I41" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J41" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K41" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L41" s="10" t="n">
         <v>6</v>
@@ -4992,40 +5004,28 @@
       <c r="M41" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="N41" s="33" t="n">
+      <c r="N41" s="10" t="n">
         <v>6</v>
       </c>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C42" s="13">
         <f>ROUND(AVERAGE(D42:AH42), 0)</f>
         <v/>
       </c>
-      <c r="G42" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H42" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I42" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J42" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K42" s="10" t="n">
         <v>6</v>
       </c>
@@ -5033,10 +5033,10 @@
         <v>6</v>
       </c>
       <c r="M42" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N42" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
         <v>6</v>
@@ -5045,38 +5045,30 @@
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C43" s="13">
         <f>ROUND(AVERAGE(D43:AH43), 0)</f>
         <v/>
       </c>
-      <c r="K43" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L43" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M43" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K43" s="10" t="n"/>
+      <c r="L43" s="10" t="n"/>
+      <c r="M43" s="9" t="n"/>
+      <c r="N43" s="10" t="n"/>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>umberto</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
@@ -5093,13 +5085,13 @@
       <c r="M44" s="9" t="n"/>
       <c r="N44" s="10" t="n"/>
       <c r="O44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>umberto</t>
+          <t>Lorenzo</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
@@ -5122,7 +5114,7 @@
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>Lorenzo</t>
+          <t>thor</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
@@ -5145,7 +5137,7 @@
     <row r="47">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>thor</t>
+          <t>doson</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
@@ -5168,7 +5160,7 @@
     <row r="48">
       <c r="A48" s="13" t="inlineStr">
         <is>
-          <t>doson</t>
+          <t>luka</t>
         </is>
       </c>
       <c r="B48" s="15" t="inlineStr">
@@ -5191,7 +5183,7 @@
     <row r="49">
       <c r="A49" s="13" t="inlineStr">
         <is>
-          <t>luka</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B49" s="15" t="inlineStr">
@@ -5208,13 +5200,13 @@
       <c r="M49" s="9" t="n"/>
       <c r="N49" s="10" t="n"/>
       <c r="O49" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="13" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>Fus</t>
         </is>
       </c>
       <c r="B50" s="15" t="inlineStr">
@@ -5237,12 +5229,12 @@
     <row r="51">
       <c r="A51" s="13" t="inlineStr">
         <is>
-          <t>Fus</t>
+          <t>KingVanze98</t>
         </is>
       </c>
       <c r="B51" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>08/02/2026</t>
         </is>
       </c>
       <c r="C51" s="13">

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-09
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3158,7 +3158,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3617,27 +3617,57 @@
         <v>6</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
         <is>
-          <t>caccialama</t>
+          <t>Chabby</t>
         </is>
       </c>
       <c r="B9" s="15" t="inlineStr">
         <is>
-          <t>02/02/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C9" s="13">
         <f>ROUND(AVERAGE(D9:AH9), 0)</f>
         <v/>
       </c>
-      <c r="K9" s="10" t="n"/>
-      <c r="L9" s="10" t="n"/>
-      <c r="N9" s="32" t="n"/>
+      <c r="D9" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="33" t="n">
+        <v>6</v>
+      </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
@@ -3645,7 +3675,7 @@
     <row r="10">
       <c r="A10" s="13" t="inlineStr">
         <is>
-          <t>Chabby</t>
+          <t>dado</t>
         </is>
       </c>
       <c r="B10" s="15" t="inlineStr">
@@ -3657,47 +3687,38 @@
         <f>ROUND(AVERAGE(D10:AH10), 0)</f>
         <v/>
       </c>
-      <c r="D10" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G10" s="9" t="n">
         <v>6</v>
       </c>
       <c r="H10" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I10" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K10" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L10" s="10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M10" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N10" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="inlineStr">
         <is>
-          <t>dado</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B11" s="15" t="inlineStr">
@@ -3710,16 +3731,16 @@
         <v/>
       </c>
       <c r="G11" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H11" s="9" t="n">
         <v>6</v>
       </c>
       <c r="I11" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J11" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K11" s="10" t="n">
         <v>6</v>
@@ -3728,19 +3749,19 @@
         <v>6</v>
       </c>
       <c r="M11" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N11" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>ER DANDI 1927</t>
         </is>
       </c>
       <c r="B12" s="15" t="inlineStr">
@@ -3753,28 +3774,28 @@
         <v/>
       </c>
       <c r="G12" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H12" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" s="9" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L12" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M12" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N12" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
@@ -3783,72 +3804,81 @@
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
+          <t>favretto</t>
         </is>
       </c>
       <c r="B13" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>02/02/2026</t>
         </is>
       </c>
       <c r="C13" s="13">
         <f>ROUND(AVERAGE(D13:AH13), 0)</f>
         <v/>
       </c>
-      <c r="G13" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="H13" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I13" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J13" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L13" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="M13" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="33" t="n">
-        <v>0</v>
-      </c>
+      <c r="K13" s="10" t="n"/>
+      <c r="L13" s="10" t="n"/>
+      <c r="N13" s="32" t="n"/>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="inlineStr">
         <is>
-          <t>favretto</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B14" s="15" t="inlineStr">
         <is>
-          <t>02/02/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C14" s="13">
         <f>ROUND(AVERAGE(D14:AH14), 0)</f>
         <v/>
       </c>
-      <c r="K14" s="10" t="n"/>
-      <c r="L14" s="10" t="n"/>
-      <c r="N14" s="32" t="n"/>
+      <c r="D14" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K14" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="M14" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N14" s="33" t="n">
+        <v>6</v>
+      </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
@@ -3870,7 +3900,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="9" t="n">
         <v>6</v>
@@ -3900,58 +3930,55 @@
     <row r="16">
       <c r="A16" s="13" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B16" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>29/12/2025</t>
         </is>
       </c>
       <c r="C16" s="13">
         <f>ROUND(AVERAGE(D16:AH16), 0)</f>
         <v/>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="I16" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J16" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K16" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L16" s="10" t="n">
         <v>2</v>
       </c>
       <c r="M16" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N16" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B17" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C17" s="13">
         <f>ROUND(AVERAGE(D17:AH17), 0)</f>
         <v/>
       </c>
-      <c r="D17" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F17" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G17" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="H17" s="9" t="n">
         <v>6</v>
       </c>
@@ -3974,35 +4001,26 @@
         <v>6</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B18" s="15" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C18" s="13">
         <f>ROUND(AVERAGE(D18:AH18), 0)</f>
         <v/>
       </c>
-      <c r="I18" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J18" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K18" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L18" s="10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M18" s="9" t="n">
         <v>6</v>
@@ -4011,24 +4029,36 @@
         <v>6</v>
       </c>
       <c r="O18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B19" s="15" t="inlineStr">
         <is>
-          <t>21/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C19" s="13">
         <f>ROUND(AVERAGE(D19:AH19), 0)</f>
         <v/>
       </c>
+      <c r="D19" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="H19" s="9" t="n">
         <v>6</v>
       </c>
@@ -4057,78 +4087,74 @@
     <row r="20">
       <c r="A20" s="13" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B20" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C20" s="13">
         <f>ROUND(AVERAGE(D20:AH20), 0)</f>
         <v/>
       </c>
+      <c r="D20" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K20" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="L20" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M20" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N20" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B21" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C21" s="13">
         <f>ROUND(AVERAGE(D21:AH21), 0)</f>
         <v/>
       </c>
-      <c r="D21" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J21" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K21" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L21" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="K21" s="10" t="n"/>
+      <c r="L21" s="10" t="n"/>
       <c r="M21" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O21" t="n">
         <v>6</v>
@@ -4137,7 +4163,7 @@
     <row r="22">
       <c r="A22" s="13" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B22" s="15" t="inlineStr">
@@ -4159,34 +4185,37 @@
         <v>6</v>
       </c>
       <c r="G22" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H22" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="I22" s="9" t="n">
+        <v>6</v>
       </c>
       <c r="J22" s="10" t="n">
         <v>6</v>
       </c>
       <c r="K22" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L22" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M22" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N22" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B23" s="15" t="inlineStr">
@@ -4204,7 +4233,7 @@
         <v>6</v>
       </c>
       <c r="N23" s="33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
         <v>6</v>
@@ -4213,7 +4242,7 @@
     <row r="24">
       <c r="A24" s="13" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B24" s="15" t="inlineStr">
@@ -4225,17 +4254,8 @@
         <f>ROUND(AVERAGE(D24:AH24), 0)</f>
         <v/>
       </c>
-      <c r="D24" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E24" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F24" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G24" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H24" s="9" t="n">
         <v>6</v>
@@ -4265,34 +4285,59 @@
     <row r="25">
       <c r="A25" s="13" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B25" s="15" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C25" s="13">
         <f>ROUND(AVERAGE(D25:AH25), 0)</f>
         <v/>
       </c>
-      <c r="K25" s="10" t="n"/>
-      <c r="L25" s="10" t="n"/>
+      <c r="D25" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="M25" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N25" s="33" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B26" s="15" t="inlineStr">
@@ -4304,11 +4349,20 @@
         <f>ROUND(AVERAGE(D26:AH26), 0)</f>
         <v/>
       </c>
+      <c r="D26" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G26" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I26" s="9" t="n">
         <v>6</v>
@@ -4317,16 +4371,16 @@
         <v>6</v>
       </c>
       <c r="K26" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L26" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M26" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N26" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O26" t="n">
         <v>6</v>
@@ -4335,7 +4389,7 @@
     <row r="27">
       <c r="A27" s="13" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B27" s="15" t="inlineStr">
@@ -4347,47 +4401,38 @@
         <f>ROUND(AVERAGE(D27:AH27), 0)</f>
         <v/>
       </c>
-      <c r="D27" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E27" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G27" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H27" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I27" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J27" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K27" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L27" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M27" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N27" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B28" s="15" t="inlineStr">
@@ -4399,20 +4444,11 @@
         <f>ROUND(AVERAGE(D28:AH28), 0)</f>
         <v/>
       </c>
-      <c r="D28" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G28" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I28" s="9" t="n">
         <v>6</v>
@@ -4421,16 +4457,16 @@
         <v>6</v>
       </c>
       <c r="K28" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L28" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M28" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N28" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O28" t="n">
         <v>6</v>
@@ -4439,33 +4475,18 @@
     <row r="29">
       <c r="A29" s="13" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B29" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C29" s="13">
         <f>ROUND(AVERAGE(D29:AH29), 0)</f>
         <v/>
       </c>
-      <c r="G29" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H29" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I29" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J29" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K29" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L29" s="10" t="n">
         <v>6</v>
       </c>
@@ -4476,36 +4497,24 @@
         <v>6</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="13" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B30" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C30" s="13">
         <f>ROUND(AVERAGE(D30:AH30), 0)</f>
         <v/>
       </c>
-      <c r="G30" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I30" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J30" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K30" s="10" t="n">
         <v>6</v>
       </c>
@@ -4519,24 +4528,48 @@
         <v>6</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="13" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B31" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C31" s="13">
         <f>ROUND(AVERAGE(D31:AH31), 0)</f>
         <v/>
       </c>
+      <c r="D31" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K31" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L31" s="10" t="n">
         <v>6</v>
       </c>
@@ -4553,18 +4586,39 @@
     <row r="32">
       <c r="A32" s="13" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B32" s="15" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C32" s="13">
         <f>ROUND(AVERAGE(D32:AH32), 0)</f>
         <v/>
       </c>
+      <c r="D32" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G32" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H32" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="I32" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J32" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K32" s="10" t="n">
         <v>6</v>
       </c>
@@ -4584,7 +4638,7 @@
     <row r="33">
       <c r="A33" s="13" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B33" s="15" t="inlineStr">
@@ -4636,7 +4690,7 @@
     <row r="34">
       <c r="A34" s="13" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B34" s="15" t="inlineStr">
@@ -4649,25 +4703,25 @@
         <v/>
       </c>
       <c r="D34" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I34" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" s="10" t="n">
         <v>5</v>
-      </c>
-      <c r="E34" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F34" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G34" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H34" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I34" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J34" s="10" t="n">
-        <v>6</v>
       </c>
       <c r="K34" s="10" t="n">
         <v>6</v>
@@ -4688,7 +4742,7 @@
     <row r="35">
       <c r="A35" s="13" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B35" s="15" t="inlineStr">
@@ -4740,7 +4794,7 @@
     <row r="36">
       <c r="A36" s="13" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B36" s="15" t="inlineStr">
@@ -4752,27 +4806,7 @@
         <f>ROUND(AVERAGE(D36:AH36), 0)</f>
         <v/>
       </c>
-      <c r="D36" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J36" s="10" t="n">
-        <v>5</v>
-      </c>
+      <c r="J36" s="10" t="n"/>
       <c r="K36" s="10" t="n">
         <v>6</v>
       </c>
@@ -4786,13 +4820,13 @@
         <v>6</v>
       </c>
       <c r="O36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="13" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B37" s="15" t="inlineStr">
@@ -4829,7 +4863,7 @@
         <v>6</v>
       </c>
       <c r="L37" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M37" s="9" t="n">
         <v>6</v>
@@ -4844,7 +4878,7 @@
     <row r="38">
       <c r="A38" s="13" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B38" s="15" t="inlineStr">
@@ -4856,9 +4890,20 @@
         <f>ROUND(AVERAGE(D38:AH38), 0)</f>
         <v/>
       </c>
-      <c r="J38" s="10" t="n"/>
+      <c r="G38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="K38" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L38" s="10" t="n">
         <v>6</v>
@@ -4876,7 +4921,7 @@
     <row r="39">
       <c r="A39" s="13" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B39" s="15" t="inlineStr">
@@ -4888,15 +4933,6 @@
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
-      <c r="D39" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G39" s="9" t="n">
         <v>6</v>
       </c>
@@ -4913,12 +4949,12 @@
         <v>6</v>
       </c>
       <c r="L39" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M39" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="N39" s="33" t="n">
+      <c r="N39" s="10" t="n">
         <v>6</v>
       </c>
       <c r="O39" t="n">
@@ -4928,124 +4964,84 @@
     <row r="40">
       <c r="A40" s="13" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C40" s="13">
         <f>ROUND(AVERAGE(D40:AH40), 0)</f>
         <v/>
       </c>
-      <c r="G40" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="K40" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L40" s="10" t="n">
         <v>6</v>
       </c>
       <c r="M40" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N40" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N40" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C41" s="13">
         <f>ROUND(AVERAGE(D41:AH41), 0)</f>
         <v/>
       </c>
-      <c r="G41" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H41" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I41" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J41" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K41" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L41" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M41" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N41" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="K41" s="10" t="n"/>
+      <c r="L41" s="10" t="n"/>
+      <c r="M41" s="9" t="n"/>
+      <c r="N41" s="10" t="n"/>
       <c r="O41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>Lorenzo</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C42" s="13">
         <f>ROUND(AVERAGE(D42:AH42), 0)</f>
         <v/>
       </c>
-      <c r="K42" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L42" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K42" s="10" t="n"/>
+      <c r="L42" s="10" t="n"/>
+      <c r="M42" s="9" t="n"/>
+      <c r="N42" s="10" t="n"/>
       <c r="O42" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>thor</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
@@ -5062,13 +5058,13 @@
       <c r="M43" s="9" t="n"/>
       <c r="N43" s="10" t="n"/>
       <c r="O43" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>umberto</t>
+          <t>doson</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
@@ -5091,7 +5087,7 @@
     <row r="45">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>Lorenzo</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
@@ -5108,18 +5104,18 @@
       <c r="M45" s="9" t="n"/>
       <c r="N45" s="10" t="n"/>
       <c r="O45" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>thor</t>
+          <t>KingVanze98</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>08/02/2026</t>
         </is>
       </c>
       <c r="C46" s="13">
@@ -5137,12 +5133,12 @@
     <row r="47">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>doson</t>
+          <t>~Oblivion~</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>09/02/2026</t>
         </is>
       </c>
       <c r="C47" s="13">
@@ -5157,98 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="13" t="inlineStr">
-        <is>
-          <t>luka</t>
-        </is>
-      </c>
-      <c r="B48" s="15" t="inlineStr">
-        <is>
-          <t>07/02/2026</t>
-        </is>
-      </c>
-      <c r="C48" s="13">
-        <f>ROUND(AVERAGE(D48:AH48), 0)</f>
-        <v/>
-      </c>
-      <c r="K48" s="10" t="n"/>
-      <c r="L48" s="10" t="n"/>
-      <c r="M48" s="9" t="n"/>
-      <c r="N48" s="10" t="n"/>
-      <c r="O48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="13" t="inlineStr">
-        <is>
-          <t>cucco</t>
-        </is>
-      </c>
-      <c r="B49" s="15" t="inlineStr">
-        <is>
-          <t>07/02/2026</t>
-        </is>
-      </c>
-      <c r="C49" s="13">
-        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
-        <v/>
-      </c>
-      <c r="K49" s="10" t="n"/>
-      <c r="L49" s="10" t="n"/>
-      <c r="M49" s="9" t="n"/>
-      <c r="N49" s="10" t="n"/>
-      <c r="O49" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="13" t="inlineStr">
-        <is>
-          <t>Fus</t>
-        </is>
-      </c>
-      <c r="B50" s="15" t="inlineStr">
-        <is>
-          <t>07/02/2026</t>
-        </is>
-      </c>
-      <c r="C50" s="13">
-        <f>ROUND(AVERAGE(D50:AH50), 0)</f>
-        <v/>
-      </c>
-      <c r="K50" s="10" t="n"/>
-      <c r="L50" s="10" t="n"/>
-      <c r="M50" s="9" t="n"/>
-      <c r="N50" s="10" t="n"/>
-      <c r="O50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="13" t="inlineStr">
-        <is>
-          <t>KingVanze98</t>
-        </is>
-      </c>
-      <c r="B51" s="15" t="inlineStr">
-        <is>
-          <t>08/02/2026</t>
-        </is>
-      </c>
-      <c r="C51" s="13">
-        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
-        <v/>
-      </c>
-      <c r="K51" s="10" t="n"/>
-      <c r="L51" s="10" t="n"/>
-      <c r="M51" s="9" t="n"/>
-      <c r="N51" s="10" t="n"/>
-      <c r="O51" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="50" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:AT1">
     <sortState ref="A2:AH50">

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-14
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3258,7 +3258,7 @@
       </c>
       <c r="P1" s="7" t="inlineStr">
         <is>
-          <t>Colonna14</t>
+          <t>13/02/2026</t>
         </is>
       </c>
       <c r="Q1" s="7" t="inlineStr">
@@ -3385,6 +3385,9 @@
       <c r="O2" t="n">
         <v>6</v>
       </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -3416,6 +3419,9 @@
       <c r="O3" t="n">
         <v>6</v>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -3468,6 +3474,9 @@
       <c r="O4" t="n">
         <v>6</v>
       </c>
+      <c r="P4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -3496,6 +3505,9 @@
       <c r="O5" t="n">
         <v>6</v>
       </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
@@ -3524,6 +3536,9 @@
       <c r="O6" t="n">
         <v>5</v>
       </c>
+      <c r="P6" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
@@ -3567,6 +3582,9 @@
       <c r="O7" t="n">
         <v>6</v>
       </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13" t="inlineStr">
@@ -3619,6 +3637,9 @@
       <c r="O8" t="n">
         <v>6</v>
       </c>
+      <c r="P8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
@@ -3671,6 +3692,9 @@
       <c r="O9" t="n">
         <v>0</v>
       </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="inlineStr">
@@ -3714,6 +3738,9 @@
       <c r="O10" t="n">
         <v>1</v>
       </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="inlineStr">
@@ -3757,6 +3784,9 @@
       <c r="O11" t="n">
         <v>6</v>
       </c>
+      <c r="P11" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="inlineStr">
@@ -3800,33 +3830,69 @@
       <c r="O12" t="n">
         <v>0</v>
       </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
         <is>
-          <t>favretto</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B13" s="15" t="inlineStr">
         <is>
-          <t>02/02/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C13" s="13">
         <f>ROUND(AVERAGE(D13:AH13), 0)</f>
         <v/>
       </c>
-      <c r="K13" s="10" t="n"/>
-      <c r="L13" s="10" t="n"/>
-      <c r="N13" s="32" t="n"/>
+      <c r="D13" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K13" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="M13" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N13" s="33" t="n">
+        <v>6</v>
+      </c>
       <c r="O13" t="n">
         <v>6</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B14" s="15" t="inlineStr">
@@ -3848,7 +3914,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="9" t="n">
         <v>6</v>
@@ -3872,39 +3938,27 @@
         <v>6</v>
       </c>
       <c r="O14" t="n">
+        <v>6</v>
+      </c>
+      <c r="P14" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>29/12/2025</t>
         </is>
       </c>
       <c r="C15" s="13">
         <f>ROUND(AVERAGE(D15:AH15), 0)</f>
         <v/>
       </c>
-      <c r="D15" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F15" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G15" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H15" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="I15" s="9" t="n">
         <v>6</v>
       </c>
@@ -3915,7 +3969,7 @@
         <v>6</v>
       </c>
       <c r="L15" s="10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M15" s="9" t="n">
         <v>6</v>
@@ -3925,23 +3979,29 @@
       </c>
       <c r="O15" t="n">
         <v>6</v>
+      </c>
+      <c r="P15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B16" s="15" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C16" s="13">
         <f>ROUND(AVERAGE(D16:AH16), 0)</f>
         <v/>
       </c>
+      <c r="H16" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="I16" s="9" t="n">
         <v>6</v>
       </c>
@@ -3952,7 +4012,7 @@
         <v>6</v>
       </c>
       <c r="L16" s="10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M16" s="9" t="n">
         <v>6</v>
@@ -3961,36 +4021,27 @@
         <v>6</v>
       </c>
       <c r="O16" t="n">
+        <v>6</v>
+      </c>
+      <c r="P16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B17" s="15" t="inlineStr">
         <is>
-          <t>21/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C17" s="13">
         <f>ROUND(AVERAGE(D17:AH17), 0)</f>
         <v/>
       </c>
-      <c r="H17" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I17" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J17" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K17" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L17" s="10" t="n">
         <v>6</v>
       </c>
@@ -4001,24 +4052,51 @@
         <v>6</v>
       </c>
       <c r="O17" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B18" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C18" s="13">
         <f>ROUND(AVERAGE(D18:AH18), 0)</f>
         <v/>
       </c>
+      <c r="D18" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I18" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J18" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K18" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L18" s="10" t="n">
         <v>6</v>
       </c>
@@ -4029,13 +4107,16 @@
         <v>6</v>
       </c>
       <c r="O18" t="n">
+        <v>6</v>
+      </c>
+      <c r="P18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B19" s="15" t="inlineStr">
@@ -4057,192 +4138,198 @@
         <v>6</v>
       </c>
       <c r="G19" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H19" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I19" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10" t="n">
         <v>6</v>
       </c>
       <c r="K19" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L19" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M19" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N19" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O19" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="13" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B20" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C20" s="13">
         <f>ROUND(AVERAGE(D20:AH20), 0)</f>
         <v/>
       </c>
-      <c r="D20" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E20" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F20" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G20" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K20" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K20" s="10" t="n"/>
+      <c r="L20" s="10" t="n"/>
       <c r="M20" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N20" s="33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="P20" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B21" s="15" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C21" s="13">
         <f>ROUND(AVERAGE(D21:AH21), 0)</f>
         <v/>
       </c>
-      <c r="K21" s="10" t="n"/>
-      <c r="L21" s="10" t="n"/>
+      <c r="D21" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J21" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K21" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="M21" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O21" t="n">
+        <v>6</v>
+      </c>
+      <c r="P21" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B22" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C22" s="13">
         <f>ROUND(AVERAGE(D22:AH22), 0)</f>
         <v/>
       </c>
-      <c r="D22" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E22" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F22" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G22" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H22" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I22" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J22" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K22" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L22" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="K22" s="10" t="n"/>
+      <c r="L22" s="10" t="n"/>
       <c r="M22" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N22" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B23" s="15" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C23" s="13">
         <f>ROUND(AVERAGE(D23:AH23), 0)</f>
         <v/>
       </c>
-      <c r="K23" s="10" t="n"/>
-      <c r="L23" s="10" t="n"/>
+      <c r="G23" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I23" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J23" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K23" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="M23" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N23" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O23" t="n">
+        <v>6</v>
+      </c>
+      <c r="P23" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B24" s="15" t="inlineStr">
@@ -4254,38 +4341,50 @@
         <f>ROUND(AVERAGE(D24:AH24), 0)</f>
         <v/>
       </c>
+      <c r="D24" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G24" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I24" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J24" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K24" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M24" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N24" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B25" s="15" t="inlineStr">
@@ -4310,16 +4409,16 @@
         <v>0</v>
       </c>
       <c r="H25" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I25" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J25" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K25" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L25" s="10" t="n">
         <v>0</v>
@@ -4331,13 +4430,16 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
+        <v>6</v>
+      </c>
+      <c r="P25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B26" s="15" t="inlineStr">
@@ -4349,20 +4451,11 @@
         <f>ROUND(AVERAGE(D26:AH26), 0)</f>
         <v/>
       </c>
-      <c r="D26" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E26" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G26" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H26" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I26" s="9" t="n">
         <v>6</v>
@@ -4371,25 +4464,28 @@
         <v>6</v>
       </c>
       <c r="K26" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L26" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M26" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N26" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O26" t="n">
         <v>6</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="13" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B27" s="15" t="inlineStr">
@@ -4402,7 +4498,7 @@
         <v/>
       </c>
       <c r="G27" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H27" s="9" t="n">
         <v>6</v>
@@ -4427,38 +4523,26 @@
       </c>
       <c r="O27" t="n">
         <v>6</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B28" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C28" s="13">
         <f>ROUND(AVERAGE(D28:AH28), 0)</f>
         <v/>
       </c>
-      <c r="G28" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I28" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J28" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K28" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L28" s="10" t="n">
         <v>6</v>
       </c>
@@ -4470,23 +4554,29 @@
       </c>
       <c r="O28" t="n">
         <v>6</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B29" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C29" s="13">
         <f>ROUND(AVERAGE(D29:AH29), 0)</f>
         <v/>
       </c>
+      <c r="K29" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L29" s="10" t="n">
         <v>6</v>
       </c>
@@ -4497,24 +4587,48 @@
         <v>6</v>
       </c>
       <c r="O29" t="n">
+        <v>6</v>
+      </c>
+      <c r="P29" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="13" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B30" s="15" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C30" s="13">
         <f>ROUND(AVERAGE(D30:AH30), 0)</f>
         <v/>
       </c>
+      <c r="D30" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E30" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F30" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G30" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H30" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I30" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J30" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K30" s="10" t="n">
         <v>6</v>
       </c>
@@ -4529,12 +4643,15 @@
       </c>
       <c r="O30" t="n">
         <v>6</v>
+      </c>
+      <c r="P30" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="13" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B31" s="15" t="inlineStr">
@@ -4547,7 +4664,7 @@
         <v/>
       </c>
       <c r="D31" s="14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="9" t="n">
         <v>6</v>
@@ -4559,7 +4676,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I31" s="9" t="n">
         <v>6</v>
@@ -4580,13 +4697,16 @@
         <v>6</v>
       </c>
       <c r="O31" t="n">
+        <v>6</v>
+      </c>
+      <c r="P31" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="13" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B32" s="15" t="inlineStr">
@@ -4599,7 +4719,7 @@
         <v/>
       </c>
       <c r="D32" s="14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32" s="9" t="n">
         <v>6</v>
@@ -4611,7 +4731,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I32" s="9" t="n">
         <v>6</v>
@@ -4632,13 +4752,16 @@
         <v>6</v>
       </c>
       <c r="O32" t="n">
+        <v>6</v>
+      </c>
+      <c r="P32" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="13" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B33" s="15" t="inlineStr">
@@ -4651,7 +4774,7 @@
         <v/>
       </c>
       <c r="D33" s="14" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E33" s="9" t="n">
         <v>6</v>
@@ -4669,7 +4792,7 @@
         <v>6</v>
       </c>
       <c r="J33" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K33" s="10" t="n">
         <v>6</v>
@@ -4685,12 +4808,15 @@
       </c>
       <c r="O33" t="n">
         <v>6</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="13" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B34" s="15" t="inlineStr">
@@ -4703,7 +4829,7 @@
         <v/>
       </c>
       <c r="D34" s="14" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E34" s="9" t="n">
         <v>6</v>
@@ -4721,7 +4847,7 @@
         <v>6</v>
       </c>
       <c r="J34" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K34" s="10" t="n">
         <v>6</v>
@@ -4736,13 +4862,16 @@
         <v>6</v>
       </c>
       <c r="O34" t="n">
+        <v>6</v>
+      </c>
+      <c r="P34" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="13" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B35" s="15" t="inlineStr">
@@ -4754,27 +4883,7 @@
         <f>ROUND(AVERAGE(D35:AH35), 0)</f>
         <v/>
       </c>
-      <c r="D35" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F35" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G35" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H35" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I35" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J35" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="J35" s="10" t="n"/>
       <c r="K35" s="10" t="n">
         <v>6</v>
       </c>
@@ -4789,12 +4898,15 @@
       </c>
       <c r="O35" t="n">
         <v>6</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="13" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B36" s="15" t="inlineStr">
@@ -4806,12 +4918,32 @@
         <f>ROUND(AVERAGE(D36:AH36), 0)</f>
         <v/>
       </c>
-      <c r="J36" s="10" t="n"/>
+      <c r="D36" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I36" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K36" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L36" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M36" s="9" t="n">
         <v>6</v>
@@ -4820,13 +4952,16 @@
         <v>6</v>
       </c>
       <c r="O36" t="n">
+        <v>6</v>
+      </c>
+      <c r="P36" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="13" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B37" s="15" t="inlineStr">
@@ -4838,32 +4973,23 @@
         <f>ROUND(AVERAGE(D37:AH37), 0)</f>
         <v/>
       </c>
-      <c r="D37" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E37" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F37" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G37" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H37" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I37" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J37" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K37" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L37" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M37" s="9" t="n">
         <v>6</v>
@@ -4873,12 +4999,15 @@
       </c>
       <c r="O37" t="n">
         <v>6</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="13" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B38" s="15" t="inlineStr">
@@ -4891,19 +5020,19 @@
         <v/>
       </c>
       <c r="G38" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H38" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I38" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J38" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K38" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L38" s="10" t="n">
         <v>6</v>
@@ -4911,40 +5040,31 @@
       <c r="M38" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="N38" s="33" t="n">
+      <c r="N38" s="10" t="n">
         <v>6</v>
       </c>
       <c r="O38" t="n">
         <v>6</v>
+      </c>
+      <c r="P38" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="13" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B39" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C39" s="13">
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
-      <c r="G39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J39" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K39" s="10" t="n">
         <v>6</v>
       </c>
@@ -4952,50 +5072,48 @@
         <v>6</v>
       </c>
       <c r="M39" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N39" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O39" t="n">
+        <v>6</v>
+      </c>
+      <c r="P39" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="13" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C40" s="13">
         <f>ROUND(AVERAGE(D40:AH40), 0)</f>
         <v/>
       </c>
-      <c r="K40" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L40" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M40" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K40" s="10" t="n"/>
+      <c r="L40" s="10" t="n"/>
+      <c r="M40" s="9" t="n"/>
+      <c r="N40" s="10" t="n"/>
       <c r="O40" t="n">
+        <v>5</v>
+      </c>
+      <c r="P40" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>thor</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
@@ -5012,13 +5130,16 @@
       <c r="M41" s="9" t="n"/>
       <c r="N41" s="10" t="n"/>
       <c r="O41" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>Lorenzo</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
@@ -5035,18 +5156,21 @@
       <c r="M42" s="9" t="n"/>
       <c r="N42" s="10" t="n"/>
       <c r="O42" t="n">
+        <v>6</v>
+      </c>
+      <c r="P42" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>thor</t>
+          <t>KingVanze98</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>08/02/2026</t>
         </is>
       </c>
       <c r="C43" s="13">
@@ -5060,16 +5184,19 @@
       <c r="O43" t="n">
         <v>0</v>
       </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>doson</t>
+          <t>~Oblivion~</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>09/02/2026</t>
         </is>
       </c>
       <c r="C44" s="13">
@@ -5083,16 +5210,19 @@
       <c r="O44" t="n">
         <v>0</v>
       </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C45" s="13">
@@ -5103,19 +5233,19 @@
       <c r="L45" s="10" t="n"/>
       <c r="M45" s="9" t="n"/>
       <c r="N45" s="10" t="n"/>
-      <c r="O45" t="n">
-        <v>6</v>
+      <c r="P45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>KingVanze98</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
         <is>
-          <t>08/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C46" s="13">
@@ -5126,19 +5256,19 @@
       <c r="L46" s="10" t="n"/>
       <c r="M46" s="9" t="n"/>
       <c r="N46" s="10" t="n"/>
-      <c r="O46" t="n">
+      <c r="P46" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>~Oblivion~</t>
+          <t>Ahmo</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
         <is>
-          <t>09/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C47" s="13">
@@ -5149,7 +5279,7 @@
       <c r="L47" s="10" t="n"/>
       <c r="M47" s="9" t="n"/>
       <c r="N47" s="10" t="n"/>
-      <c r="O47" t="n">
+      <c r="P47" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-15
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3158,7 +3158,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3506,7 +3506,7 @@
         <v>6</v>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -3693,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -3886,7 +3886,7 @@
         <v>6</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -3981,7 +3981,7 @@
         <v>6</v>
       </c>
       <c r="P15" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -4110,7 +4110,7 @@
         <v>6</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -4433,7 +4433,7 @@
         <v>6</v>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -4479,7 +4479,7 @@
         <v>6</v>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -4525,7 +4525,7 @@
         <v>6</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
@@ -4556,7 +4556,7 @@
         <v>6</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -4645,7 +4645,7 @@
         <v>6</v>
       </c>
       <c r="P30" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -4810,7 +4810,7 @@
         <v>6</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -5113,7 +5113,7 @@
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>thor</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
@@ -5130,7 +5130,7 @@
       <c r="M41" s="9" t="n"/>
       <c r="N41" s="10" t="n"/>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P41" t="n">
         <v>0</v>
@@ -5139,12 +5139,12 @@
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>KingVanze98</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>08/02/2026</t>
         </is>
       </c>
       <c r="C42" s="13">
@@ -5156,7 +5156,7 @@
       <c r="M42" s="9" t="n"/>
       <c r="N42" s="10" t="n"/>
       <c r="O42" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P42" t="n">
         <v>0</v>
@@ -5165,12 +5165,12 @@
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>KingVanze98</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>08/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C43" s="13">
@@ -5181,22 +5181,19 @@
       <c r="L43" s="10" t="n"/>
       <c r="M43" s="9" t="n"/>
       <c r="N43" s="10" t="n"/>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>~Oblivion~</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>09/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C44" s="13">
@@ -5207,79 +5204,7 @@
       <c r="L44" s="10" t="n"/>
       <c r="M44" s="9" t="n"/>
       <c r="N44" s="10" t="n"/>
-      <c r="O44" t="n">
-        <v>0</v>
-      </c>
       <c r="P44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="13" t="inlineStr">
-        <is>
-          <t>Amazonie</t>
-        </is>
-      </c>
-      <c r="B45" s="15" t="inlineStr">
-        <is>
-          <t>14/02/2026</t>
-        </is>
-      </c>
-      <c r="C45" s="13">
-        <f>ROUND(AVERAGE(D45:AH45), 0)</f>
-        <v/>
-      </c>
-      <c r="K45" s="10" t="n"/>
-      <c r="L45" s="10" t="n"/>
-      <c r="M45" s="9" t="n"/>
-      <c r="N45" s="10" t="n"/>
-      <c r="P45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="13" t="inlineStr">
-        <is>
-          <t>terracrom</t>
-        </is>
-      </c>
-      <c r="B46" s="15" t="inlineStr">
-        <is>
-          <t>14/02/2026</t>
-        </is>
-      </c>
-      <c r="C46" s="13">
-        <f>ROUND(AVERAGE(D46:AH46), 0)</f>
-        <v/>
-      </c>
-      <c r="K46" s="10" t="n"/>
-      <c r="L46" s="10" t="n"/>
-      <c r="M46" s="9" t="n"/>
-      <c r="N46" s="10" t="n"/>
-      <c r="P46" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="13" t="inlineStr">
-        <is>
-          <t>Ahmo</t>
-        </is>
-      </c>
-      <c r="B47" s="15" t="inlineStr">
-        <is>
-          <t>14/02/2026</t>
-        </is>
-      </c>
-      <c r="C47" s="13">
-        <f>ROUND(AVERAGE(D47:AH47), 0)</f>
-        <v/>
-      </c>
-      <c r="K47" s="10" t="n"/>
-      <c r="L47" s="10" t="n"/>
-      <c r="M47" s="9" t="n"/>
-      <c r="N47" s="10" t="n"/>
-      <c r="P47" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-16
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3158,7 +3158,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH44"/>
+  <dimension ref="A1:AH46"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3583,7 +3583,7 @@
         <v>6</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -3739,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -4162,7 +4162,7 @@
         <v>4</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -4900,7 +4900,7 @@
         <v>6</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -5139,12 +5139,12 @@
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>KingVanze98</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>08/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C42" s="13">
@@ -5155,17 +5155,14 @@
       <c r="L42" s="10" t="n"/>
       <c r="M42" s="9" t="n"/>
       <c r="N42" s="10" t="n"/>
-      <c r="O42" t="n">
-        <v>0</v>
-      </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>Amazonie</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
@@ -5182,18 +5179,18 @@
       <c r="M43" s="9" t="n"/>
       <c r="N43" s="10" t="n"/>
       <c r="P43" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>terracrom</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>14/02/2026</t>
+          <t>16/02/2026</t>
         </is>
       </c>
       <c r="C44" s="13">
@@ -5206,6 +5203,52 @@
       <c r="N44" s="10" t="n"/>
       <c r="P44" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="13" t="inlineStr">
+        <is>
+          <t>fede61mito</t>
+        </is>
+      </c>
+      <c r="B45" s="15" t="inlineStr">
+        <is>
+          <t>16/02/2026</t>
+        </is>
+      </c>
+      <c r="C45" s="13">
+        <f>ROUND(AVERAGE(D45:AH45), 0)</f>
+        <v/>
+      </c>
+      <c r="K45" s="10" t="n"/>
+      <c r="L45" s="10" t="n"/>
+      <c r="M45" s="9" t="n"/>
+      <c r="N45" s="10" t="n"/>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="13" t="inlineStr">
+        <is>
+          <t>Dasters79</t>
+        </is>
+      </c>
+      <c r="B46" s="15" t="inlineStr">
+        <is>
+          <t>16/02/2026</t>
+        </is>
+      </c>
+      <c r="C46" s="13">
+        <f>ROUND(AVERAGE(D46:AH46), 0)</f>
+        <v/>
+      </c>
+      <c r="K46" s="10" t="n"/>
+      <c r="L46" s="10" t="n"/>
+      <c r="M46" s="9" t="n"/>
+      <c r="N46" s="10" t="n"/>
+      <c r="P46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-21
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -763,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -1063,7 +1063,7 @@
     <row r="5">
       <c r="A5" s="24" t="inlineStr">
         <is>
-          <t>Ale22</t>
+          <t>alhfmfh</t>
         </is>
       </c>
       <c r="B5" s="27" t="inlineStr">
@@ -1080,13 +1080,13 @@
         <v/>
       </c>
       <c r="E5" s="24" t="n">
-        <v>56020</v>
+        <v>20225</v>
       </c>
       <c r="F5" s="33" t="n"/>
       <c r="G5" s="33" t="n"/>
       <c r="H5" s="33" t="n"/>
       <c r="I5" s="33" t="n">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="J5" s="33" t="n"/>
       <c r="K5" s="33" t="n"/>
@@ -1106,7 +1106,7 @@
     <row r="6">
       <c r="A6" s="24" t="inlineStr">
         <is>
-          <t>alhfmfh</t>
+          <t>andriu07</t>
         </is>
       </c>
       <c r="B6" s="27" t="inlineStr">
@@ -1123,13 +1123,13 @@
         <v/>
       </c>
       <c r="E6" s="24" t="n">
-        <v>20225</v>
+        <v>11310</v>
       </c>
       <c r="F6" s="33" t="n"/>
       <c r="G6" s="33" t="n"/>
       <c r="H6" s="33" t="n"/>
       <c r="I6" s="33" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="J6" s="33" t="n"/>
       <c r="K6" s="33" t="n"/>
@@ -1149,12 +1149,12 @@
     <row r="7">
       <c r="A7" s="24" t="inlineStr">
         <is>
-          <t>andriu07</t>
+          <t>BigMc23</t>
         </is>
       </c>
       <c r="B7" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C7" s="19">
@@ -1166,13 +1166,15 @@
         <v/>
       </c>
       <c r="E7" s="24" t="n">
-        <v>11310</v>
+        <v>15150</v>
       </c>
       <c r="F7" s="33" t="n"/>
       <c r="G7" s="33" t="n"/>
-      <c r="H7" s="33" t="n"/>
+      <c r="H7" s="33" t="n">
+        <v>500</v>
+      </c>
       <c r="I7" s="33" t="n">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="J7" s="33" t="n"/>
       <c r="K7" s="33" t="n"/>
@@ -1192,7 +1194,7 @@
     <row r="8">
       <c r="A8" s="24" t="inlineStr">
         <is>
-          <t>BigMc23</t>
+          <t>buff x-bow</t>
         </is>
       </c>
       <c r="B8" s="27" t="inlineStr">
@@ -1209,15 +1211,19 @@
         <v/>
       </c>
       <c r="E8" s="24" t="n">
-        <v>15150</v>
-      </c>
-      <c r="F8" s="33" t="n"/>
-      <c r="G8" s="33" t="n"/>
+        <v>27500</v>
+      </c>
+      <c r="F8" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G8" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="H8" s="33" t="n">
-        <v>500</v>
+        <v>4100</v>
       </c>
       <c r="I8" s="33" t="n">
-        <v>1500</v>
+        <v>4400</v>
       </c>
       <c r="J8" s="33" t="n"/>
       <c r="K8" s="33" t="n"/>
@@ -1237,7 +1243,7 @@
     <row r="9">
       <c r="A9" s="24" t="inlineStr">
         <is>
-          <t>buff x-bow</t>
+          <t>Chabby</t>
         </is>
       </c>
       <c r="B9" s="27" t="inlineStr">
@@ -1254,19 +1260,17 @@
         <v/>
       </c>
       <c r="E9" s="24" t="n">
-        <v>27500</v>
-      </c>
-      <c r="F9" s="33" t="n">
-        <v>4000</v>
-      </c>
+        <v>12250</v>
+      </c>
+      <c r="F9" s="33" t="n"/>
       <c r="G9" s="33" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="33" t="n">
-        <v>4100</v>
+        <v>0</v>
       </c>
       <c r="I9" s="33" t="n">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="J9" s="33" t="n"/>
       <c r="K9" s="33" t="n"/>
@@ -1286,7 +1290,7 @@
     <row r="10">
       <c r="A10" s="24" t="inlineStr">
         <is>
-          <t>Chabby</t>
+          <t>dado</t>
         </is>
       </c>
       <c r="B10" s="27" t="inlineStr">
@@ -1303,17 +1307,15 @@
         <v/>
       </c>
       <c r="E10" s="24" t="n">
-        <v>12250</v>
+        <v>40850</v>
       </c>
       <c r="F10" s="33" t="n"/>
-      <c r="G10" s="33" t="n">
-        <v>0</v>
-      </c>
+      <c r="G10" s="33" t="n"/>
       <c r="H10" s="33" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="I10" s="33" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="J10" s="33" t="n"/>
       <c r="K10" s="33" t="n"/>
@@ -1333,7 +1335,7 @@
     <row r="11">
       <c r="A11" s="24" t="inlineStr">
         <is>
-          <t>dado</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B11" s="27" t="inlineStr">
@@ -1350,15 +1352,15 @@
         <v/>
       </c>
       <c r="E11" s="24" t="n">
-        <v>40850</v>
+        <v>25300</v>
       </c>
       <c r="F11" s="33" t="n"/>
       <c r="G11" s="33" t="n"/>
       <c r="H11" s="33" t="n">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="I11" s="33" t="n">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J11" s="33" t="n"/>
       <c r="K11" s="33" t="n"/>
@@ -1378,7 +1380,7 @@
     <row r="12">
       <c r="A12" s="24" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>ER DANDI 1927</t>
         </is>
       </c>
       <c r="B12" s="27" t="inlineStr">
@@ -1395,15 +1397,15 @@
         <v/>
       </c>
       <c r="E12" s="24" t="n">
-        <v>25300</v>
+        <v>70250</v>
       </c>
       <c r="F12" s="33" t="n"/>
       <c r="G12" s="33" t="n"/>
       <c r="H12" s="33" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="I12" s="33" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="J12" s="33" t="n"/>
       <c r="K12" s="33" t="n"/>
@@ -1423,7 +1425,7 @@
     <row r="13">
       <c r="A13" s="24" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B13" s="27" t="inlineStr">
@@ -1440,15 +1442,19 @@
         <v/>
       </c>
       <c r="E13" s="24" t="n">
-        <v>70250</v>
-      </c>
-      <c r="F13" s="33" t="n"/>
-      <c r="G13" s="33" t="n"/>
+        <v>29650</v>
+      </c>
+      <c r="F13" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G13" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="H13" s="33" t="n">
-        <v>1300</v>
+        <v>10000</v>
       </c>
       <c r="I13" s="33" t="n">
-        <v>4000</v>
+        <v>2450</v>
       </c>
       <c r="J13" s="33" t="n"/>
       <c r="K13" s="33" t="n"/>
@@ -1468,12 +1474,12 @@
     <row r="14">
       <c r="A14" s="24" t="inlineStr">
         <is>
-          <t>fabiovesco</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B14" s="27" t="inlineStr">
         <is>
-          <t>21/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C14" s="19">
@@ -1485,13 +1491,17 @@
         <v/>
       </c>
       <c r="E14" s="24" t="n">
-        <v>3100</v>
+        <v>16050</v>
       </c>
       <c r="F14" s="33" t="n"/>
-      <c r="G14" s="33" t="n"/>
-      <c r="H14" s="33" t="n"/>
+      <c r="G14" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="33" t="n">
+        <v>6050</v>
+      </c>
       <c r="I14" s="33" t="n">
-        <v>1000</v>
+        <v>8300</v>
       </c>
       <c r="J14" s="33" t="n"/>
       <c r="K14" s="33" t="n"/>
@@ -1511,12 +1521,12 @@
     <row r="15">
       <c r="A15" s="24" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B15" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>26/12/2025</t>
         </is>
       </c>
       <c r="C15" s="19">
@@ -1528,19 +1538,15 @@
         <v/>
       </c>
       <c r="E15" s="24" t="n">
-        <v>29650</v>
-      </c>
-      <c r="F15" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G15" s="33" t="n">
-        <v>4000</v>
-      </c>
+        <v>21950</v>
+      </c>
+      <c r="F15" s="33" t="n"/>
+      <c r="G15" s="33" t="n"/>
       <c r="H15" s="33" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="I15" s="33" t="n">
-        <v>2450</v>
+        <v>1000</v>
       </c>
       <c r="J15" s="33" t="n"/>
       <c r="K15" s="33" t="n"/>
@@ -1560,12 +1566,12 @@
     <row r="16">
       <c r="A16" s="24" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B16" s="27" t="inlineStr">
         <is>
-          <t>21/01/2026</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C16" s="19">
@@ -1577,13 +1583,15 @@
         <v/>
       </c>
       <c r="E16" s="24" t="n">
-        <v>0</v>
+        <v>119800</v>
       </c>
       <c r="F16" s="33" t="n"/>
       <c r="G16" s="33" t="n"/>
-      <c r="H16" s="33" t="n"/>
+      <c r="H16" s="33" t="n">
+        <v>4050</v>
+      </c>
       <c r="I16" s="33" t="n">
-        <v>0</v>
+        <v>4100</v>
       </c>
       <c r="J16" s="33" t="n"/>
       <c r="K16" s="33" t="n"/>
@@ -1603,7 +1611,7 @@
     <row r="17">
       <c r="A17" s="24" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B17" s="27" t="inlineStr">
@@ -1620,13 +1628,13 @@
         <v/>
       </c>
       <c r="E17" s="24" t="n">
-        <v>0</v>
+        <v>61020</v>
       </c>
       <c r="F17" s="33" t="n"/>
       <c r="G17" s="33" t="n"/>
       <c r="H17" s="33" t="n"/>
       <c r="I17" s="33" t="n">
-        <v>0</v>
+        <v>6350</v>
       </c>
       <c r="J17" s="33" t="n"/>
       <c r="K17" s="33" t="n"/>
@@ -1646,7 +1654,7 @@
     <row r="18">
       <c r="A18" s="24" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B18" s="27" t="inlineStr">
@@ -1663,17 +1671,19 @@
         <v/>
       </c>
       <c r="E18" s="24" t="n">
-        <v>16050</v>
-      </c>
-      <c r="F18" s="33" t="n"/>
+        <v>36600</v>
+      </c>
+      <c r="F18" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="G18" s="33" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H18" s="33" t="n">
-        <v>6050</v>
+        <v>10000</v>
       </c>
       <c r="I18" s="33" t="n">
-        <v>8300</v>
+        <v>10000</v>
       </c>
       <c r="J18" s="33" t="n"/>
       <c r="K18" s="33" t="n"/>
@@ -1693,12 +1703,12 @@
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B19" s="27" t="inlineStr">
         <is>
-          <t>26/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C19" s="19">
@@ -1710,15 +1720,17 @@
         <v/>
       </c>
       <c r="E19" s="24" t="n">
-        <v>21950</v>
+        <v>28500</v>
       </c>
       <c r="F19" s="33" t="n"/>
-      <c r="G19" s="33" t="n"/>
+      <c r="G19" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="H19" s="33" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="I19" s="33" t="n">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="J19" s="33" t="n"/>
       <c r="K19" s="33" t="n"/>
@@ -1738,12 +1750,12 @@
     <row r="20">
       <c r="A20" s="24" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B20" s="27" t="inlineStr">
         <is>
-          <t>21/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C20" s="19">
@@ -1755,15 +1767,13 @@
         <v/>
       </c>
       <c r="E20" s="24" t="n">
-        <v>119800</v>
+        <v>74050</v>
       </c>
       <c r="F20" s="33" t="n"/>
       <c r="G20" s="33" t="n"/>
-      <c r="H20" s="33" t="n">
-        <v>4050</v>
-      </c>
+      <c r="H20" s="33" t="n"/>
       <c r="I20" s="33" t="n">
-        <v>4100</v>
+        <v>0</v>
       </c>
       <c r="J20" s="33" t="n"/>
       <c r="K20" s="33" t="n"/>
@@ -1783,12 +1793,12 @@
     <row r="21">
       <c r="A21" s="24" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B21" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C21" s="19">
@@ -1800,13 +1810,17 @@
         <v/>
       </c>
       <c r="E21" s="24" t="n">
-        <v>61020</v>
+        <v>45200</v>
       </c>
       <c r="F21" s="33" t="n"/>
-      <c r="G21" s="33" t="n"/>
-      <c r="H21" s="33" t="n"/>
+      <c r="G21" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H21" s="33" t="n">
+        <v>10000</v>
+      </c>
       <c r="I21" s="33" t="n">
-        <v>6350</v>
+        <v>10000</v>
       </c>
       <c r="J21" s="33" t="n"/>
       <c r="K21" s="33" t="n"/>
@@ -1826,12 +1840,12 @@
     <row r="22">
       <c r="A22" s="24" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B22" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C22" s="19">
@@ -1843,19 +1857,13 @@
         <v/>
       </c>
       <c r="E22" s="24" t="n">
-        <v>36600</v>
-      </c>
-      <c r="F22" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G22" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="H22" s="33" t="n">
-        <v>10000</v>
-      </c>
+        <v>62125</v>
+      </c>
+      <c r="F22" s="33" t="n"/>
+      <c r="G22" s="33" t="n"/>
+      <c r="H22" s="33" t="n"/>
       <c r="I22" s="33" t="n">
-        <v>10000</v>
+        <v>6250</v>
       </c>
       <c r="J22" s="33" t="n"/>
       <c r="K22" s="33" t="n"/>
@@ -1875,7 +1883,7 @@
     <row r="23">
       <c r="A23" s="24" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B23" s="27" t="inlineStr">
@@ -1892,21 +1900,19 @@
         <v/>
       </c>
       <c r="E23" s="24" t="n">
-        <v>28500</v>
+        <v>45300</v>
       </c>
       <c r="F23" s="33" t="n"/>
-      <c r="G23" s="33" t="n">
-        <v>4000</v>
-      </c>
+      <c r="G23" s="33" t="n"/>
       <c r="H23" s="33" t="n">
         <v>10000</v>
       </c>
       <c r="I23" s="33" t="n">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="J23" s="33" t="n"/>
       <c r="K23" s="33" t="n"/>
-      <c r="L23" s="33" t="n"/>
+      <c r="L23" s="21" t="n"/>
       <c r="M23" s="33" t="n"/>
       <c r="N23" s="33" t="n"/>
       <c r="O23" s="33" t="n"/>
@@ -1922,12 +1928,12 @@
     <row r="24">
       <c r="A24" s="24" t="inlineStr">
         <is>
-          <t>Killer46</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B24" s="27" t="inlineStr">
         <is>
-          <t>26/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C24" s="19">
@@ -1939,13 +1945,19 @@
         <v/>
       </c>
       <c r="E24" s="24" t="n">
-        <v>11065</v>
-      </c>
-      <c r="F24" s="33" t="n"/>
-      <c r="G24" s="33" t="n"/>
-      <c r="H24" s="33" t="n"/>
+        <v>6175</v>
+      </c>
+      <c r="F24" s="33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G24" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="I24" s="33" t="n">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="J24" s="33" t="n"/>
       <c r="K24" s="33" t="n"/>
@@ -1965,12 +1977,12 @@
     <row r="25">
       <c r="A25" s="24" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B25" s="27" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C25" s="19">
@@ -1982,13 +1994,19 @@
         <v/>
       </c>
       <c r="E25" s="24" t="n">
-        <v>74050</v>
-      </c>
-      <c r="F25" s="33" t="n"/>
-      <c r="G25" s="33" t="n"/>
-      <c r="H25" s="33" t="n"/>
+        <v>28700</v>
+      </c>
+      <c r="F25" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G25" s="33" t="n">
+        <v>2100</v>
+      </c>
+      <c r="H25" s="33" t="n">
+        <v>5800</v>
+      </c>
       <c r="I25" s="33" t="n">
-        <v>0</v>
+        <v>4050</v>
       </c>
       <c r="J25" s="33" t="n"/>
       <c r="K25" s="33" t="n"/>
@@ -2008,7 +2026,7 @@
     <row r="26">
       <c r="A26" s="24" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B26" s="27" t="inlineStr">
@@ -2025,12 +2043,10 @@
         <v/>
       </c>
       <c r="E26" s="24" t="n">
-        <v>45200</v>
+        <v>48650</v>
       </c>
       <c r="F26" s="33" t="n"/>
-      <c r="G26" s="33" t="n">
-        <v>4000</v>
-      </c>
+      <c r="G26" s="33" t="n"/>
       <c r="H26" s="33" t="n">
         <v>10000</v>
       </c>
@@ -2055,12 +2071,12 @@
     <row r="27">
       <c r="A27" s="24" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B27" s="27" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C27" s="19">
@@ -2072,13 +2088,15 @@
         <v/>
       </c>
       <c r="E27" s="24" t="n">
-        <v>62125</v>
+        <v>40900</v>
       </c>
       <c r="F27" s="33" t="n"/>
       <c r="G27" s="33" t="n"/>
-      <c r="H27" s="33" t="n"/>
+      <c r="H27" s="33" t="n">
+        <v>10000</v>
+      </c>
       <c r="I27" s="33" t="n">
-        <v>6250</v>
+        <v>10000</v>
       </c>
       <c r="J27" s="33" t="n"/>
       <c r="K27" s="33" t="n"/>
@@ -2098,12 +2116,12 @@
     <row r="28">
       <c r="A28" s="24" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B28" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C28" s="19">
@@ -2115,19 +2133,17 @@
         <v/>
       </c>
       <c r="E28" s="24" t="n">
-        <v>45300</v>
+        <v>96625</v>
       </c>
       <c r="F28" s="33" t="n"/>
       <c r="G28" s="33" t="n"/>
-      <c r="H28" s="33" t="n">
-        <v>10000</v>
-      </c>
+      <c r="H28" s="33" t="n"/>
       <c r="I28" s="33" t="n">
         <v>10000</v>
       </c>
       <c r="J28" s="33" t="n"/>
       <c r="K28" s="33" t="n"/>
-      <c r="L28" s="21" t="n"/>
+      <c r="L28" s="33" t="n"/>
       <c r="M28" s="33" t="n"/>
       <c r="N28" s="33" t="n"/>
       <c r="O28" s="33" t="n"/>
@@ -2143,12 +2159,12 @@
     <row r="29">
       <c r="A29" s="24" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B29" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C29" s="19">
@@ -2160,19 +2176,13 @@
         <v/>
       </c>
       <c r="E29" s="24" t="n">
-        <v>6175</v>
-      </c>
-      <c r="F29" s="33" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G29" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="33" t="n">
-        <v>0</v>
-      </c>
+        <v>40450</v>
+      </c>
+      <c r="F29" s="33" t="n"/>
+      <c r="G29" s="33" t="n"/>
+      <c r="H29" s="33" t="n"/>
       <c r="I29" s="33" t="n">
-        <v>1150</v>
+        <v>4300</v>
       </c>
       <c r="J29" s="33" t="n"/>
       <c r="K29" s="33" t="n"/>
@@ -2192,7 +2202,7 @@
     <row r="30">
       <c r="A30" s="24" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B30" s="27" t="inlineStr">
@@ -2209,19 +2219,19 @@
         <v/>
       </c>
       <c r="E30" s="24" t="n">
-        <v>28700</v>
+        <v>38600</v>
       </c>
       <c r="F30" s="33" t="n">
         <v>4000</v>
       </c>
       <c r="G30" s="33" t="n">
-        <v>2100</v>
+        <v>4000</v>
       </c>
       <c r="H30" s="33" t="n">
-        <v>5800</v>
+        <v>4050</v>
       </c>
       <c r="I30" s="33" t="n">
-        <v>4050</v>
+        <v>5600</v>
       </c>
       <c r="J30" s="33" t="n"/>
       <c r="K30" s="33" t="n"/>
@@ -2241,7 +2251,7 @@
     <row r="31">
       <c r="A31" s="24" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B31" s="27" t="inlineStr">
@@ -2258,15 +2268,17 @@
         <v/>
       </c>
       <c r="E31" s="24" t="n">
-        <v>48650</v>
+        <v>17930</v>
       </c>
       <c r="F31" s="33" t="n"/>
-      <c r="G31" s="33" t="n"/>
+      <c r="G31" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="H31" s="33" t="n">
-        <v>10000</v>
+        <v>5150</v>
       </c>
       <c r="I31" s="33" t="n">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="J31" s="33" t="n"/>
       <c r="K31" s="33" t="n"/>
@@ -2286,7 +2298,7 @@
     <row r="32">
       <c r="A32" s="24" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B32" s="27" t="inlineStr">
@@ -2303,15 +2315,19 @@
         <v/>
       </c>
       <c r="E32" s="24" t="n">
-        <v>40900</v>
-      </c>
-      <c r="F32" s="33" t="n"/>
-      <c r="G32" s="33" t="n"/>
+        <v>45550</v>
+      </c>
+      <c r="F32" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G32" s="33" t="n">
+        <v>4000</v>
+      </c>
       <c r="H32" s="33" t="n">
         <v>10000</v>
       </c>
       <c r="I32" s="33" t="n">
-        <v>10000</v>
+        <v>7150</v>
       </c>
       <c r="J32" s="33" t="n"/>
       <c r="K32" s="33" t="n"/>
@@ -2319,7 +2335,7 @@
       <c r="M32" s="33" t="n"/>
       <c r="N32" s="33" t="n"/>
       <c r="O32" s="33" t="n"/>
-      <c r="P32" s="33" t="n"/>
+      <c r="P32" s="21" t="n"/>
       <c r="Q32" s="33" t="n"/>
       <c r="R32" s="33" t="n"/>
       <c r="S32" s="33" t="n"/>
@@ -2331,12 +2347,12 @@
     <row r="33">
       <c r="A33" s="24" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B33" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C33" s="19">
@@ -2348,13 +2364,17 @@
         <v/>
       </c>
       <c r="E33" s="24" t="n">
-        <v>96625</v>
+        <v>23200</v>
       </c>
       <c r="F33" s="33" t="n"/>
-      <c r="G33" s="33" t="n"/>
-      <c r="H33" s="33" t="n"/>
+      <c r="G33" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H33" s="33" t="n">
+        <v>10000</v>
+      </c>
       <c r="I33" s="33" t="n">
-        <v>10000</v>
+        <v>4500</v>
       </c>
       <c r="J33" s="33" t="n"/>
       <c r="K33" s="33" t="n"/>
@@ -2374,12 +2394,12 @@
     <row r="34">
       <c r="A34" s="24" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B34" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C34" s="19">
@@ -2391,13 +2411,19 @@
         <v/>
       </c>
       <c r="E34" s="24" t="n">
-        <v>40450</v>
-      </c>
-      <c r="F34" s="33" t="n"/>
-      <c r="G34" s="33" t="n"/>
-      <c r="H34" s="33" t="n"/>
+        <v>29025</v>
+      </c>
+      <c r="F34" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G34" s="33" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H34" s="33" t="n">
+        <v>4050</v>
+      </c>
       <c r="I34" s="33" t="n">
-        <v>4300</v>
+        <v>4850</v>
       </c>
       <c r="J34" s="33" t="n"/>
       <c r="K34" s="33" t="n"/>
@@ -2417,12 +2443,12 @@
     <row r="35">
       <c r="A35" s="24" t="inlineStr">
         <is>
-          <t>Rixxy</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B35" s="27" t="inlineStr">
         <is>
-          <t>24/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C35" s="19">
@@ -2434,13 +2460,15 @@
         <v/>
       </c>
       <c r="E35" s="24" t="n">
-        <v>450</v>
+        <v>28675</v>
       </c>
       <c r="F35" s="33" t="n"/>
       <c r="G35" s="33" t="n"/>
-      <c r="H35" s="33" t="n"/>
+      <c r="H35" s="33" t="n">
+        <v>3650</v>
+      </c>
       <c r="I35" s="33" t="n">
-        <v>0</v>
+        <v>7600</v>
       </c>
       <c r="J35" s="33" t="n"/>
       <c r="K35" s="33" t="n"/>
@@ -2460,7 +2488,7 @@
     <row r="36">
       <c r="A36" s="24" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B36" s="27" t="inlineStr">
@@ -2477,7 +2505,7 @@
         <v/>
       </c>
       <c r="E36" s="24" t="n">
-        <v>38600</v>
+        <v>29450</v>
       </c>
       <c r="F36" s="33" t="n">
         <v>4000</v>
@@ -2486,10 +2514,10 @@
         <v>4000</v>
       </c>
       <c r="H36" s="33" t="n">
-        <v>4050</v>
+        <v>5750</v>
       </c>
       <c r="I36" s="33" t="n">
-        <v>5600</v>
+        <v>4500</v>
       </c>
       <c r="J36" s="33" t="n"/>
       <c r="K36" s="33" t="n"/>
@@ -2509,7 +2537,7 @@
     <row r="37">
       <c r="A37" s="24" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B37" s="27" t="inlineStr">
@@ -2526,17 +2554,15 @@
         <v/>
       </c>
       <c r="E37" s="24" t="n">
-        <v>17930</v>
+        <v>30350</v>
       </c>
       <c r="F37" s="33" t="n"/>
-      <c r="G37" s="33" t="n">
-        <v>4000</v>
-      </c>
+      <c r="G37" s="33" t="n"/>
       <c r="H37" s="33" t="n">
-        <v>5150</v>
+        <v>150</v>
       </c>
       <c r="I37" s="33" t="n">
-        <v>2500</v>
+        <v>5300</v>
       </c>
       <c r="J37" s="33" t="n"/>
       <c r="K37" s="33" t="n"/>
@@ -2556,7 +2582,7 @@
     <row r="38">
       <c r="A38" s="24" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B38" s="27" t="inlineStr">
@@ -2573,19 +2599,15 @@
         <v/>
       </c>
       <c r="E38" s="24" t="n">
-        <v>45550</v>
-      </c>
-      <c r="F38" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G38" s="33" t="n">
-        <v>4000</v>
-      </c>
+        <v>109220</v>
+      </c>
+      <c r="F38" s="33" t="n"/>
+      <c r="G38" s="33" t="n"/>
       <c r="H38" s="33" t="n">
+        <v>3850</v>
+      </c>
+      <c r="I38" s="33" t="n">
         <v>10000</v>
-      </c>
-      <c r="I38" s="33" t="n">
-        <v>7150</v>
       </c>
       <c r="J38" s="33" t="n"/>
       <c r="K38" s="33" t="n"/>
@@ -2593,7 +2615,7 @@
       <c r="M38" s="33" t="n"/>
       <c r="N38" s="33" t="n"/>
       <c r="O38" s="33" t="n"/>
-      <c r="P38" s="21" t="n"/>
+      <c r="P38" s="33" t="n"/>
       <c r="Q38" s="33" t="n"/>
       <c r="R38" s="33" t="n"/>
       <c r="S38" s="33" t="n"/>
@@ -2605,12 +2627,12 @@
     <row r="39">
       <c r="A39" s="24" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B39" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C39" s="19">
@@ -2622,17 +2644,13 @@
         <v/>
       </c>
       <c r="E39" s="24" t="n">
-        <v>23200</v>
+        <v>58950</v>
       </c>
       <c r="F39" s="33" t="n"/>
-      <c r="G39" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="H39" s="33" t="n">
+      <c r="G39" s="33" t="n"/>
+      <c r="H39" s="33" t="n"/>
+      <c r="I39" s="33" t="n">
         <v>10000</v>
-      </c>
-      <c r="I39" s="33" t="n">
-        <v>4500</v>
       </c>
       <c r="J39" s="33" t="n"/>
       <c r="K39" s="33" t="n"/>
@@ -2652,12 +2670,12 @@
     <row r="40">
       <c r="A40" s="24" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B40" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C40" s="19">
@@ -2669,20 +2687,12 @@
         <v/>
       </c>
       <c r="E40" s="24" t="n">
-        <v>29025</v>
-      </c>
-      <c r="F40" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G40" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="H40" s="33" t="n">
-        <v>4050</v>
-      </c>
-      <c r="I40" s="33" t="n">
-        <v>4850</v>
-      </c>
+        <v>71700</v>
+      </c>
+      <c r="F40" s="33" t="n"/>
+      <c r="G40" s="33" t="n"/>
+      <c r="H40" s="33" t="n"/>
+      <c r="I40" s="33" t="n"/>
       <c r="J40" s="33" t="n"/>
       <c r="K40" s="33" t="n"/>
       <c r="L40" s="33" t="n"/>
@@ -2701,12 +2711,12 @@
     <row r="41">
       <c r="A41" s="24" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>Amir✴</t>
         </is>
       </c>
       <c r="B41" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C41" s="19">
@@ -2718,16 +2728,12 @@
         <v/>
       </c>
       <c r="E41" s="24" t="n">
-        <v>28675</v>
+        <v>59875</v>
       </c>
       <c r="F41" s="33" t="n"/>
       <c r="G41" s="33" t="n"/>
-      <c r="H41" s="33" t="n">
-        <v>3650</v>
-      </c>
-      <c r="I41" s="33" t="n">
-        <v>7600</v>
-      </c>
+      <c r="H41" s="33" t="n"/>
+      <c r="I41" s="33" t="n"/>
       <c r="J41" s="33" t="n"/>
       <c r="K41" s="33" t="n"/>
       <c r="L41" s="33" t="n"/>
@@ -2746,12 +2752,12 @@
     <row r="42">
       <c r="A42" s="24" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B42" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C42" s="19">
@@ -2763,14 +2769,12 @@
         <v/>
       </c>
       <c r="E42" s="24" t="n">
-        <v>13350</v>
+        <v>20875</v>
       </c>
       <c r="F42" s="33" t="n"/>
       <c r="G42" s="33" t="n"/>
       <c r="H42" s="33" t="n"/>
-      <c r="I42" s="33" t="n">
-        <v>4150</v>
-      </c>
+      <c r="I42" s="33" t="n"/>
       <c r="J42" s="33" t="n"/>
       <c r="K42" s="33" t="n"/>
       <c r="L42" s="33" t="n"/>
@@ -2789,12 +2793,12 @@
     <row r="43">
       <c r="A43" s="24" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Anto</t>
         </is>
       </c>
       <c r="B43" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C43" s="19">
@@ -2806,20 +2810,12 @@
         <v/>
       </c>
       <c r="E43" s="24" t="n">
-        <v>29450</v>
-      </c>
-      <c r="F43" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G43" s="33" t="n">
-        <v>4000</v>
-      </c>
-      <c r="H43" s="33" t="n">
-        <v>5750</v>
-      </c>
-      <c r="I43" s="33" t="n">
-        <v>4500</v>
-      </c>
+        <v>7650</v>
+      </c>
+      <c r="F43" s="33" t="n"/>
+      <c r="G43" s="33" t="n"/>
+      <c r="H43" s="33" t="n"/>
+      <c r="I43" s="33" t="n"/>
       <c r="J43" s="33" t="n"/>
       <c r="K43" s="33" t="n"/>
       <c r="L43" s="33" t="n"/>
@@ -2838,12 +2834,12 @@
     <row r="44">
       <c r="A44" s="24" t="inlineStr">
         <is>
-          <t>The_Boff01</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B44" s="27" t="inlineStr">
         <is>
-          <t>26/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C44" s="19">
@@ -2855,14 +2851,12 @@
         <v/>
       </c>
       <c r="E44" s="24" t="n">
-        <v>27805</v>
+        <v>22905</v>
       </c>
       <c r="F44" s="33" t="n"/>
       <c r="G44" s="33" t="n"/>
       <c r="H44" s="33" t="n"/>
-      <c r="I44" s="33" t="n">
-        <v>300</v>
-      </c>
+      <c r="I44" s="33" t="n"/>
       <c r="J44" s="33" t="n"/>
       <c r="K44" s="33" t="n"/>
       <c r="L44" s="33" t="n"/>
@@ -2881,12 +2875,12 @@
     <row r="45">
       <c r="A45" s="24" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>dibba10</t>
         </is>
       </c>
       <c r="B45" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C45" s="19">
@@ -2898,16 +2892,12 @@
         <v/>
       </c>
       <c r="E45" s="24" t="n">
-        <v>30350</v>
+        <v>12460</v>
       </c>
       <c r="F45" s="33" t="n"/>
       <c r="G45" s="33" t="n"/>
-      <c r="H45" s="33" t="n">
-        <v>150</v>
-      </c>
-      <c r="I45" s="33" t="n">
-        <v>5300</v>
-      </c>
+      <c r="H45" s="33" t="n"/>
+      <c r="I45" s="33" t="n"/>
       <c r="J45" s="33" t="n"/>
       <c r="K45" s="33" t="n"/>
       <c r="L45" s="33" t="n"/>
@@ -2926,12 +2916,12 @@
     <row r="46">
       <c r="A46" s="24" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B46" s="27" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C46" s="19">
@@ -2943,16 +2933,12 @@
         <v/>
       </c>
       <c r="E46" s="24" t="n">
-        <v>109220</v>
+        <v>21350</v>
       </c>
       <c r="F46" s="33" t="n"/>
       <c r="G46" s="33" t="n"/>
-      <c r="H46" s="33" t="n">
-        <v>3850</v>
-      </c>
-      <c r="I46" s="33" t="n">
-        <v>10000</v>
-      </c>
+      <c r="H46" s="33" t="n"/>
+      <c r="I46" s="33" t="n"/>
       <c r="J46" s="33" t="n"/>
       <c r="K46" s="33" t="n"/>
       <c r="L46" s="33" t="n"/>
@@ -2971,12 +2957,12 @@
     <row r="47">
       <c r="A47" s="24" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B47" s="27" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C47" s="19">
@@ -2988,14 +2974,12 @@
         <v/>
       </c>
       <c r="E47" s="24" t="n">
-        <v>58950</v>
+        <v>400</v>
       </c>
       <c r="F47" s="33" t="n"/>
       <c r="G47" s="33" t="n"/>
       <c r="H47" s="33" t="n"/>
-      <c r="I47" s="33" t="n">
-        <v>10000</v>
-      </c>
+      <c r="I47" s="33" t="n"/>
       <c r="J47" s="33" t="n"/>
       <c r="K47" s="33" t="n"/>
       <c r="L47" s="33" t="n"/>
@@ -3014,12 +2998,12 @@
     <row r="48">
       <c r="A48" s="24" t="inlineStr">
         <is>
-          <t>Leonida</t>
+          <t>Xx_Herman_xX</t>
         </is>
       </c>
       <c r="B48" s="27" t="inlineStr">
         <is>
-          <t>28/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C48" s="19">
@@ -3031,14 +3015,12 @@
         <v/>
       </c>
       <c r="E48" s="24" t="n">
-        <v>21035</v>
+        <v>11235</v>
       </c>
       <c r="F48" s="33" t="n"/>
       <c r="G48" s="33" t="n"/>
       <c r="H48" s="33" t="n"/>
-      <c r="I48" s="33" t="n">
-        <v>0</v>
-      </c>
+      <c r="I48" s="33" t="n"/>
       <c r="J48" s="33" t="n"/>
       <c r="K48" s="33" t="n"/>
       <c r="L48" s="33" t="n"/>
@@ -3057,12 +3039,12 @@
     <row r="49">
       <c r="A49" s="24" t="inlineStr">
         <is>
-          <t>tuspostati</t>
+          <t>Artur</t>
         </is>
       </c>
       <c r="B49" s="27" t="inlineStr">
         <is>
-          <t>28/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C49" s="19">
@@ -3074,14 +3056,12 @@
         <v/>
       </c>
       <c r="E49" s="24" t="n">
-        <v>6525</v>
+        <v>1800</v>
       </c>
       <c r="F49" s="33" t="n"/>
       <c r="G49" s="33" t="n"/>
       <c r="H49" s="33" t="n"/>
-      <c r="I49" s="33" t="n">
-        <v>0</v>
-      </c>
+      <c r="I49" s="33" t="n"/>
       <c r="J49" s="33" t="n"/>
       <c r="K49" s="33" t="n"/>
       <c r="L49" s="33" t="n"/>
@@ -3100,12 +3080,12 @@
     <row r="50">
       <c r="A50" s="24" t="inlineStr">
         <is>
-          <t>IL MAGO NERO</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="B50" s="27" t="inlineStr">
         <is>
-          <t>28/01/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C50" s="19">
@@ -3117,14 +3097,12 @@
         <v/>
       </c>
       <c r="E50" s="24" t="n">
-        <v>4075</v>
+        <v>450</v>
       </c>
       <c r="F50" s="33" t="n"/>
       <c r="G50" s="33" t="n"/>
       <c r="H50" s="33" t="n"/>
-      <c r="I50" s="33" t="n">
-        <v>0</v>
-      </c>
+      <c r="I50" s="33" t="n"/>
       <c r="J50" s="33" t="n"/>
       <c r="K50" s="33" t="n"/>
       <c r="L50" s="33" t="n"/>
@@ -3140,7 +3118,47 @@
       <c r="V50" s="33" t="n"/>
       <c r="W50" s="33" t="n"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="51" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A51" s="24" t="inlineStr">
+        <is>
+          <t>MIRIAM MIRIAM</t>
+        </is>
+      </c>
+      <c r="B51" s="27" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C51" s="19">
+        <f>ROUND(AVERAGE(F51:AB51), 0)</f>
+        <v/>
+      </c>
+      <c r="D51" s="1">
+        <f>SUM(F51:AB51)</f>
+        <v/>
+      </c>
+      <c r="E51" s="24" t="n">
+        <v>19450</v>
+      </c>
+      <c r="F51" s="33" t="n"/>
+      <c r="G51" s="33" t="n"/>
+      <c r="H51" s="33" t="n"/>
+      <c r="I51" s="33" t="n"/>
+      <c r="J51" s="33" t="n"/>
+      <c r="K51" s="33" t="n"/>
+      <c r="L51" s="33" t="n"/>
+      <c r="M51" s="33" t="n"/>
+      <c r="N51" s="33" t="n"/>
+      <c r="O51" s="33" t="n"/>
+      <c r="P51" s="33" t="n"/>
+      <c r="Q51" s="33" t="n"/>
+      <c r="R51" s="33" t="n"/>
+      <c r="S51" s="33" t="n"/>
+      <c r="T51" s="33" t="n"/>
+      <c r="U51" s="33" t="n"/>
+      <c r="V51" s="33" t="n"/>
+      <c r="W51" s="33" t="n"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AA1">
     <sortState ref="A2:AA51">

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-21
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3176,7 +3176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="Q1" s="7" t="inlineStr">
         <is>
-          <t>Colonna15</t>
+          <t>20/02/2026</t>
         </is>
       </c>
       <c r="R1" s="7" t="inlineStr">
@@ -3406,6 +3406,9 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -3440,6 +3443,9 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -3495,6 +3501,9 @@
       <c r="P4" t="n">
         <v>6</v>
       </c>
+      <c r="Q4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -3526,6 +3535,9 @@
       <c r="P5" t="n">
         <v>6</v>
       </c>
+      <c r="Q5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
@@ -3557,6 +3569,9 @@
       <c r="P6" t="n">
         <v>6</v>
       </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
@@ -3603,6 +3618,9 @@
       <c r="P7" t="n">
         <v>6</v>
       </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13" t="inlineStr">
@@ -3658,6 +3676,9 @@
       <c r="P8" t="n">
         <v>6</v>
       </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
@@ -3713,6 +3734,9 @@
       <c r="P9" t="n">
         <v>3</v>
       </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="inlineStr">
@@ -3759,6 +3783,9 @@
       <c r="P10" t="n">
         <v>2</v>
       </c>
+      <c r="Q10" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="inlineStr">
@@ -3805,6 +3832,9 @@
       <c r="P11" t="n">
         <v>6</v>
       </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="inlineStr">
@@ -3851,6 +3881,9 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
@@ -3906,6 +3939,9 @@
       <c r="P13" t="n">
         <v>6</v>
       </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="inlineStr">
@@ -3961,6 +3997,9 @@
       <c r="P14" t="n">
         <v>6</v>
       </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="inlineStr">
@@ -4001,6 +4040,9 @@
       <c r="P15" t="n">
         <v>6</v>
       </c>
+      <c r="Q15" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="inlineStr">
@@ -4044,6 +4086,9 @@
       <c r="P16" t="n">
         <v>6</v>
       </c>
+      <c r="Q16" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="inlineStr">
@@ -4075,6 +4120,9 @@
       <c r="P17" t="n">
         <v>6</v>
       </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="inlineStr">
@@ -4130,6 +4178,9 @@
       <c r="P18" t="n">
         <v>6</v>
       </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="inlineStr">
@@ -4181,6 +4232,9 @@
       </c>
       <c r="P19" t="n">
         <v>4</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -4212,6 +4266,9 @@
       <c r="P20" t="n">
         <v>6</v>
       </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="inlineStr">
@@ -4265,6 +4322,9 @@
         <v>6</v>
       </c>
       <c r="P21" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q21" t="n">
         <v>6</v>
       </c>
     </row>
@@ -4297,6 +4357,9 @@
       <c r="P22" t="n">
         <v>6</v>
       </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="inlineStr">
@@ -4343,6 +4406,9 @@
       <c r="P23" t="n">
         <v>6</v>
       </c>
+      <c r="Q23" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="inlineStr">
@@ -4398,6 +4464,9 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="inlineStr">
@@ -4453,6 +4522,9 @@
       <c r="P25" t="n">
         <v>6</v>
       </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="inlineStr">
@@ -4499,6 +4571,9 @@
       <c r="P26" t="n">
         <v>6</v>
       </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="13" t="inlineStr">
@@ -4545,6 +4620,9 @@
       <c r="P27" t="n">
         <v>6</v>
       </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="inlineStr">
@@ -4576,6 +4654,9 @@
       <c r="P28" t="n">
         <v>6</v>
       </c>
+      <c r="Q28" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="inlineStr">
@@ -4610,6 +4691,9 @@
       <c r="P29" t="n">
         <v>6</v>
       </c>
+      <c r="Q29" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="13" t="inlineStr">
@@ -4665,6 +4749,9 @@
       <c r="P30" t="n">
         <v>6</v>
       </c>
+      <c r="Q30" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="13" t="inlineStr">
@@ -4720,6 +4807,9 @@
       <c r="P31" t="n">
         <v>6</v>
       </c>
+      <c r="Q31" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="13" t="inlineStr">
@@ -4775,6 +4865,9 @@
       <c r="P32" t="n">
         <v>6</v>
       </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="13" t="inlineStr">
@@ -4830,6 +4923,9 @@
       <c r="P33" t="n">
         <v>6</v>
       </c>
+      <c r="Q33" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="13" t="inlineStr">
@@ -4885,6 +4981,9 @@
       <c r="P34" t="n">
         <v>6</v>
       </c>
+      <c r="Q34" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="13" t="inlineStr">
@@ -4920,6 +5019,9 @@
       <c r="P35" t="n">
         <v>6</v>
       </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="13" t="inlineStr">
@@ -4975,6 +5077,9 @@
       <c r="P36" t="n">
         <v>6</v>
       </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="13" t="inlineStr">
@@ -5021,6 +5126,9 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="13" t="inlineStr">
@@ -5067,6 +5175,9 @@
       <c r="P38" t="n">
         <v>1</v>
       </c>
+      <c r="Q38" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="13" t="inlineStr">
@@ -5100,6 +5211,9 @@
       </c>
       <c r="P39" t="n">
         <v>6</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -5127,6 +5241,9 @@
       <c r="P40" t="n">
         <v>6</v>
       </c>
+      <c r="Q40" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
@@ -5153,6 +5270,9 @@
       <c r="P41" t="n">
         <v>0</v>
       </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
@@ -5176,6 +5296,9 @@
       <c r="P42" t="n">
         <v>6</v>
       </c>
+      <c r="Q42" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
@@ -5199,11 +5322,14 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
@@ -5222,11 +5348,14 @@
       <c r="P44" t="n">
         <v>0</v>
       </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
@@ -5243,18 +5372,21 @@
       <c r="M45" s="9" t="n"/>
       <c r="N45" s="10" t="n"/>
       <c r="P45" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>Dasters79</t>
+          <t>Amir✴</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
         <is>
-          <t>16/02/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C46" s="13">
@@ -5265,11 +5397,125 @@
       <c r="L46" s="10" t="n"/>
       <c r="M46" s="9" t="n"/>
       <c r="N46" s="10" t="n"/>
-      <c r="P46" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1"/>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="13" t="inlineStr">
+        <is>
+          <t>Artur</t>
+        </is>
+      </c>
+      <c r="B47" s="15" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C47" s="13">
+        <f>ROUND(AVERAGE(D47:AH47), 0)</f>
+        <v/>
+      </c>
+      <c r="K47" s="10" t="n"/>
+      <c r="L47" s="10" t="n"/>
+      <c r="M47" s="9" t="n"/>
+      <c r="N47" s="10" t="n"/>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="13" t="inlineStr">
+        <is>
+          <t>Xx_Herman_xX</t>
+        </is>
+      </c>
+      <c r="B48" s="15" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C48" s="13">
+        <f>ROUND(AVERAGE(D48:AH48), 0)</f>
+        <v/>
+      </c>
+      <c r="K48" s="10" t="n"/>
+      <c r="L48" s="10" t="n"/>
+      <c r="M48" s="9" t="n"/>
+      <c r="N48" s="10" t="n"/>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="13" t="inlineStr">
+        <is>
+          <t>dibba10</t>
+        </is>
+      </c>
+      <c r="B49" s="15" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C49" s="13">
+        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
+        <v/>
+      </c>
+      <c r="K49" s="10" t="n"/>
+      <c r="L49" s="10" t="n"/>
+      <c r="M49" s="9" t="n"/>
+      <c r="N49" s="10" t="n"/>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="13" t="inlineStr">
+        <is>
+          <t>Anto</t>
+        </is>
+      </c>
+      <c r="B50" s="15" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C50" s="13">
+        <f>ROUND(AVERAGE(D50:AH50), 0)</f>
+        <v/>
+      </c>
+      <c r="K50" s="10" t="n"/>
+      <c r="L50" s="10" t="n"/>
+      <c r="M50" s="9" t="n"/>
+      <c r="N50" s="10" t="n"/>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="13" t="inlineStr">
+        <is>
+          <t>Michele</t>
+        </is>
+      </c>
+      <c r="B51" s="15" t="inlineStr">
+        <is>
+          <t>21/02/2026</t>
+        </is>
+      </c>
+      <c r="C51" s="13">
+        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
+        <v/>
+      </c>
+      <c r="K51" s="10" t="n"/>
+      <c r="L51" s="10" t="n"/>
+      <c r="M51" s="9" t="n"/>
+      <c r="N51" s="10" t="n"/>
+      <c r="Q51" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AT1">
     <sortState ref="A2:AH50">

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-22
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -951,7 +951,9 @@
       <c r="I2" s="17" t="n">
         <v>1500</v>
       </c>
-      <c r="J2" s="17" t="n"/>
+      <c r="J2" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="K2" s="17" t="n"/>
       <c r="L2" s="17" t="n"/>
       <c r="M2" s="17" t="n"/>
@@ -998,7 +1000,9 @@
       <c r="I3" s="33" t="n">
         <v>4150</v>
       </c>
-      <c r="J3" s="33" t="n"/>
+      <c r="J3" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" s="33" t="n"/>
       <c r="L3" s="33" t="n"/>
       <c r="M3" s="33" t="n"/>
@@ -1045,7 +1049,9 @@
       <c r="I4" s="33" t="n">
         <v>5000</v>
       </c>
-      <c r="J4" s="33" t="n"/>
+      <c r="J4" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" s="33" t="n"/>
       <c r="L4" s="33" t="n"/>
       <c r="M4" s="33" t="n"/>
@@ -1088,7 +1094,9 @@
       <c r="I5" s="33" t="n">
         <v>2000</v>
       </c>
-      <c r="J5" s="33" t="n"/>
+      <c r="J5" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K5" s="33" t="n"/>
       <c r="L5" s="33" t="n"/>
       <c r="M5" s="33" t="n"/>
@@ -1131,7 +1139,9 @@
       <c r="I6" s="33" t="n">
         <v>2500</v>
       </c>
-      <c r="J6" s="33" t="n"/>
+      <c r="J6" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" s="33" t="n"/>
       <c r="L6" s="33" t="n"/>
       <c r="M6" s="33" t="n"/>
@@ -1176,7 +1186,9 @@
       <c r="I7" s="33" t="n">
         <v>1500</v>
       </c>
-      <c r="J7" s="33" t="n"/>
+      <c r="J7" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K7" s="33" t="n"/>
       <c r="L7" s="33" t="n"/>
       <c r="M7" s="33" t="n"/>
@@ -1225,7 +1237,9 @@
       <c r="I8" s="33" t="n">
         <v>4400</v>
       </c>
-      <c r="J8" s="33" t="n"/>
+      <c r="J8" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" s="33" t="n"/>
       <c r="L8" s="33" t="n"/>
       <c r="M8" s="33" t="n"/>
@@ -1272,7 +1286,9 @@
       <c r="I9" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="33" t="n"/>
+      <c r="J9" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" s="33" t="n"/>
       <c r="L9" s="33" t="n"/>
       <c r="M9" s="33" t="n"/>
@@ -1317,7 +1333,9 @@
       <c r="I10" s="33" t="n">
         <v>4000</v>
       </c>
-      <c r="J10" s="33" t="n"/>
+      <c r="J10" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K10" s="33" t="n"/>
       <c r="L10" s="33" t="n"/>
       <c r="M10" s="33" t="n"/>
@@ -1362,7 +1380,9 @@
       <c r="I11" s="33" t="n">
         <v>3500</v>
       </c>
-      <c r="J11" s="33" t="n"/>
+      <c r="J11" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K11" s="33" t="n"/>
       <c r="L11" s="33" t="n"/>
       <c r="M11" s="33" t="n"/>
@@ -1407,7 +1427,9 @@
       <c r="I12" s="33" t="n">
         <v>4000</v>
       </c>
-      <c r="J12" s="33" t="n"/>
+      <c r="J12" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K12" s="33" t="n"/>
       <c r="L12" s="33" t="n"/>
       <c r="M12" s="33" t="n"/>
@@ -1456,7 +1478,9 @@
       <c r="I13" s="33" t="n">
         <v>2450</v>
       </c>
-      <c r="J13" s="33" t="n"/>
+      <c r="J13" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K13" s="33" t="n"/>
       <c r="L13" s="33" t="n"/>
       <c r="M13" s="33" t="n"/>
@@ -1503,7 +1527,9 @@
       <c r="I14" s="33" t="n">
         <v>8300</v>
       </c>
-      <c r="J14" s="33" t="n"/>
+      <c r="J14" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K14" s="33" t="n"/>
       <c r="L14" s="33" t="n"/>
       <c r="M14" s="33" t="n"/>
@@ -1548,7 +1574,9 @@
       <c r="I15" s="33" t="n">
         <v>1000</v>
       </c>
-      <c r="J15" s="33" t="n"/>
+      <c r="J15" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K15" s="33" t="n"/>
       <c r="L15" s="33" t="n"/>
       <c r="M15" s="33" t="n"/>
@@ -1593,7 +1621,9 @@
       <c r="I16" s="33" t="n">
         <v>4100</v>
       </c>
-      <c r="J16" s="33" t="n"/>
+      <c r="J16" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K16" s="33" t="n"/>
       <c r="L16" s="33" t="n"/>
       <c r="M16" s="33" t="n"/>
@@ -1636,7 +1666,9 @@
       <c r="I17" s="33" t="n">
         <v>6350</v>
       </c>
-      <c r="J17" s="33" t="n"/>
+      <c r="J17" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K17" s="33" t="n"/>
       <c r="L17" s="33" t="n"/>
       <c r="M17" s="33" t="n"/>
@@ -1685,7 +1717,9 @@
       <c r="I18" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J18" s="33" t="n"/>
+      <c r="J18" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K18" s="33" t="n"/>
       <c r="L18" s="33" t="n"/>
       <c r="M18" s="33" t="n"/>
@@ -1732,7 +1766,9 @@
       <c r="I19" s="33" t="n">
         <v>5000</v>
       </c>
-      <c r="J19" s="33" t="n"/>
+      <c r="J19" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K19" s="33" t="n"/>
       <c r="L19" s="33" t="n"/>
       <c r="M19" s="33" t="n"/>
@@ -1775,7 +1811,9 @@
       <c r="I20" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="33" t="n"/>
+      <c r="J20" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K20" s="33" t="n"/>
       <c r="L20" s="33" t="n"/>
       <c r="M20" s="33" t="n"/>
@@ -1822,7 +1860,9 @@
       <c r="I21" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J21" s="33" t="n"/>
+      <c r="J21" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K21" s="33" t="n"/>
       <c r="L21" s="33" t="n"/>
       <c r="M21" s="33" t="n"/>
@@ -1865,7 +1905,9 @@
       <c r="I22" s="33" t="n">
         <v>6250</v>
       </c>
-      <c r="J22" s="33" t="n"/>
+      <c r="J22" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K22" s="33" t="n"/>
       <c r="L22" s="33" t="n"/>
       <c r="M22" s="33" t="n"/>
@@ -1910,7 +1952,9 @@
       <c r="I23" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J23" s="33" t="n"/>
+      <c r="J23" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K23" s="33" t="n"/>
       <c r="L23" s="21" t="n"/>
       <c r="M23" s="33" t="n"/>
@@ -1959,7 +2003,9 @@
       <c r="I24" s="33" t="n">
         <v>1150</v>
       </c>
-      <c r="J24" s="33" t="n"/>
+      <c r="J24" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K24" s="33" t="n"/>
       <c r="L24" s="33" t="n"/>
       <c r="M24" s="33" t="n"/>
@@ -2008,7 +2054,9 @@
       <c r="I25" s="33" t="n">
         <v>4050</v>
       </c>
-      <c r="J25" s="33" t="n"/>
+      <c r="J25" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K25" s="33" t="n"/>
       <c r="L25" s="33" t="n"/>
       <c r="M25" s="33" t="n"/>
@@ -2053,7 +2101,9 @@
       <c r="I26" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J26" s="33" t="n"/>
+      <c r="J26" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K26" s="33" t="n"/>
       <c r="L26" s="33" t="n"/>
       <c r="M26" s="33" t="n"/>
@@ -2098,7 +2148,9 @@
       <c r="I27" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J27" s="33" t="n"/>
+      <c r="J27" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K27" s="33" t="n"/>
       <c r="L27" s="33" t="n"/>
       <c r="M27" s="33" t="n"/>
@@ -2141,7 +2193,9 @@
       <c r="I28" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J28" s="33" t="n"/>
+      <c r="J28" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K28" s="33" t="n"/>
       <c r="L28" s="33" t="n"/>
       <c r="M28" s="33" t="n"/>
@@ -2184,7 +2238,9 @@
       <c r="I29" s="33" t="n">
         <v>4300</v>
       </c>
-      <c r="J29" s="33" t="n"/>
+      <c r="J29" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K29" s="33" t="n"/>
       <c r="L29" s="33" t="n"/>
       <c r="M29" s="33" t="n"/>
@@ -2233,7 +2289,9 @@
       <c r="I30" s="33" t="n">
         <v>5600</v>
       </c>
-      <c r="J30" s="33" t="n"/>
+      <c r="J30" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K30" s="33" t="n"/>
       <c r="L30" s="33" t="n"/>
       <c r="M30" s="33" t="n"/>
@@ -2280,7 +2338,9 @@
       <c r="I31" s="33" t="n">
         <v>2500</v>
       </c>
-      <c r="J31" s="33" t="n"/>
+      <c r="J31" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K31" s="33" t="n"/>
       <c r="L31" s="33" t="n"/>
       <c r="M31" s="33" t="n"/>
@@ -2329,7 +2389,9 @@
       <c r="I32" s="33" t="n">
         <v>7150</v>
       </c>
-      <c r="J32" s="33" t="n"/>
+      <c r="J32" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K32" s="33" t="n"/>
       <c r="L32" s="33" t="n"/>
       <c r="M32" s="33" t="n"/>
@@ -2376,7 +2438,9 @@
       <c r="I33" s="33" t="n">
         <v>4500</v>
       </c>
-      <c r="J33" s="33" t="n"/>
+      <c r="J33" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K33" s="33" t="n"/>
       <c r="L33" s="33" t="n"/>
       <c r="M33" s="33" t="n"/>
@@ -2425,7 +2489,9 @@
       <c r="I34" s="33" t="n">
         <v>4850</v>
       </c>
-      <c r="J34" s="33" t="n"/>
+      <c r="J34" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K34" s="33" t="n"/>
       <c r="L34" s="33" t="n"/>
       <c r="M34" s="33" t="n"/>
@@ -2470,7 +2536,9 @@
       <c r="I35" s="33" t="n">
         <v>7600</v>
       </c>
-      <c r="J35" s="33" t="n"/>
+      <c r="J35" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K35" s="33" t="n"/>
       <c r="L35" s="33" t="n"/>
       <c r="M35" s="33" t="n"/>
@@ -2519,7 +2587,9 @@
       <c r="I36" s="33" t="n">
         <v>4500</v>
       </c>
-      <c r="J36" s="33" t="n"/>
+      <c r="J36" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K36" s="33" t="n"/>
       <c r="L36" s="33" t="n"/>
       <c r="M36" s="33" t="n"/>
@@ -2564,7 +2634,9 @@
       <c r="I37" s="33" t="n">
         <v>5300</v>
       </c>
-      <c r="J37" s="33" t="n"/>
+      <c r="J37" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K37" s="33" t="n"/>
       <c r="L37" s="33" t="n"/>
       <c r="M37" s="33" t="n"/>
@@ -2609,7 +2681,9 @@
       <c r="I38" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J38" s="33" t="n"/>
+      <c r="J38" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K38" s="33" t="n"/>
       <c r="L38" s="33" t="n"/>
       <c r="M38" s="33" t="n"/>
@@ -2652,7 +2726,9 @@
       <c r="I39" s="33" t="n">
         <v>10000</v>
       </c>
-      <c r="J39" s="33" t="n"/>
+      <c r="J39" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K39" s="33" t="n"/>
       <c r="L39" s="33" t="n"/>
       <c r="M39" s="33" t="n"/>
@@ -2693,7 +2769,9 @@
       <c r="G40" s="33" t="n"/>
       <c r="H40" s="33" t="n"/>
       <c r="I40" s="33" t="n"/>
-      <c r="J40" s="33" t="n"/>
+      <c r="J40" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K40" s="33" t="n"/>
       <c r="L40" s="33" t="n"/>
       <c r="M40" s="33" t="n"/>
@@ -2734,7 +2812,9 @@
       <c r="G41" s="33" t="n"/>
       <c r="H41" s="33" t="n"/>
       <c r="I41" s="33" t="n"/>
-      <c r="J41" s="33" t="n"/>
+      <c r="J41" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K41" s="33" t="n"/>
       <c r="L41" s="33" t="n"/>
       <c r="M41" s="33" t="n"/>
@@ -2775,7 +2855,9 @@
       <c r="G42" s="33" t="n"/>
       <c r="H42" s="33" t="n"/>
       <c r="I42" s="33" t="n"/>
-      <c r="J42" s="33" t="n"/>
+      <c r="J42" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K42" s="33" t="n"/>
       <c r="L42" s="33" t="n"/>
       <c r="M42" s="33" t="n"/>
@@ -2816,7 +2898,9 @@
       <c r="G43" s="33" t="n"/>
       <c r="H43" s="33" t="n"/>
       <c r="I43" s="33" t="n"/>
-      <c r="J43" s="33" t="n"/>
+      <c r="J43" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K43" s="33" t="n"/>
       <c r="L43" s="33" t="n"/>
       <c r="M43" s="33" t="n"/>
@@ -2857,7 +2941,9 @@
       <c r="G44" s="33" t="n"/>
       <c r="H44" s="33" t="n"/>
       <c r="I44" s="33" t="n"/>
-      <c r="J44" s="33" t="n"/>
+      <c r="J44" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K44" s="33" t="n"/>
       <c r="L44" s="33" t="n"/>
       <c r="M44" s="33" t="n"/>
@@ -2898,7 +2984,9 @@
       <c r="G45" s="33" t="n"/>
       <c r="H45" s="33" t="n"/>
       <c r="I45" s="33" t="n"/>
-      <c r="J45" s="33" t="n"/>
+      <c r="J45" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K45" s="33" t="n"/>
       <c r="L45" s="33" t="n"/>
       <c r="M45" s="33" t="n"/>
@@ -2939,7 +3027,9 @@
       <c r="G46" s="33" t="n"/>
       <c r="H46" s="33" t="n"/>
       <c r="I46" s="33" t="n"/>
-      <c r="J46" s="33" t="n"/>
+      <c r="J46" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K46" s="33" t="n"/>
       <c r="L46" s="33" t="n"/>
       <c r="M46" s="33" t="n"/>
@@ -2980,7 +3070,9 @@
       <c r="G47" s="33" t="n"/>
       <c r="H47" s="33" t="n"/>
       <c r="I47" s="33" t="n"/>
-      <c r="J47" s="33" t="n"/>
+      <c r="J47" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K47" s="33" t="n"/>
       <c r="L47" s="33" t="n"/>
       <c r="M47" s="33" t="n"/>
@@ -3021,7 +3113,9 @@
       <c r="G48" s="33" t="n"/>
       <c r="H48" s="33" t="n"/>
       <c r="I48" s="33" t="n"/>
-      <c r="J48" s="33" t="n"/>
+      <c r="J48" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K48" s="33" t="n"/>
       <c r="L48" s="33" t="n"/>
       <c r="M48" s="33" t="n"/>
@@ -3062,7 +3156,9 @@
       <c r="G49" s="33" t="n"/>
       <c r="H49" s="33" t="n"/>
       <c r="I49" s="33" t="n"/>
-      <c r="J49" s="33" t="n"/>
+      <c r="J49" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K49" s="33" t="n"/>
       <c r="L49" s="33" t="n"/>
       <c r="M49" s="33" t="n"/>
@@ -3103,7 +3199,9 @@
       <c r="G50" s="33" t="n"/>
       <c r="H50" s="33" t="n"/>
       <c r="I50" s="33" t="n"/>
-      <c r="J50" s="33" t="n"/>
+      <c r="J50" s="33" t="n">
+        <v>0</v>
+      </c>
       <c r="K50" s="33" t="n"/>
       <c r="L50" s="33" t="n"/>
       <c r="M50" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-22
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3234,7 +3234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3998,7 +3998,7 @@
         <v>6</v>
       </c>
       <c r="Q13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -4237,7 +4237,7 @@
         <v>6</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -4325,7 +4325,7 @@
         <v>6</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -4465,7 +4465,7 @@
         <v>6</v>
       </c>
       <c r="Q23" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -4581,7 +4581,7 @@
         <v>6</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -5078,7 +5078,7 @@
         <v>6</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -5136,7 +5136,7 @@
         <v>6</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -5271,7 +5271,7 @@
         <v>6</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -5439,7 +5439,7 @@
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>Amir✴</t>
+          <t>Artur</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
@@ -5462,7 +5462,7 @@
     <row r="47">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>Artur</t>
+          <t>Xx_Herman_xX</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
@@ -5485,7 +5485,7 @@
     <row r="48">
       <c r="A48" s="13" t="inlineStr">
         <is>
-          <t>Xx_Herman_xX</t>
+          <t>dibba10</t>
         </is>
       </c>
       <c r="B48" s="15" t="inlineStr">
@@ -5502,13 +5502,13 @@
       <c r="M48" s="9" t="n"/>
       <c r="N48" s="10" t="n"/>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="13" t="inlineStr">
         <is>
-          <t>dibba10</t>
+          <t>Anto</t>
         </is>
       </c>
       <c r="B49" s="15" t="inlineStr">
@@ -5531,7 +5531,7 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="13" t="inlineStr">
         <is>
-          <t>Anto</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="B50" s="15" t="inlineStr">
@@ -5548,30 +5548,7 @@
       <c r="M50" s="9" t="n"/>
       <c r="N50" s="10" t="n"/>
       <c r="Q50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="13" t="inlineStr">
-        <is>
-          <t>Michele</t>
-        </is>
-      </c>
-      <c r="B51" s="15" t="inlineStr">
-        <is>
-          <t>21/02/2026</t>
-        </is>
-      </c>
-      <c r="C51" s="13">
-        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
-        <v/>
-      </c>
-      <c r="K51" s="10" t="n"/>
-      <c r="L51" s="10" t="n"/>
-      <c r="M51" s="9" t="n"/>
-      <c r="N51" s="10" t="n"/>
-      <c r="Q51" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-23
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2892,14 +2892,14 @@
         <v/>
       </c>
       <c r="E43" s="24" t="n">
-        <v>22905</v>
+        <v>23005</v>
       </c>
       <c r="F43" s="33" t="n"/>
       <c r="G43" s="33" t="n"/>
       <c r="H43" s="33" t="n"/>
       <c r="I43" s="33" t="n"/>
       <c r="J43" s="33" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K43" s="33" t="n"/>
       <c r="L43" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-23
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3276,7 +3276,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH50"/>
+  <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3719,7 +3719,7 @@
         <v>6</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -3777,7 +3777,7 @@
         <v>6</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -3933,7 +3933,7 @@
         <v>6</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -4098,7 +4098,7 @@
         <v>6</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -4334,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -4458,7 +4458,7 @@
         <v>6</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
@@ -4623,7 +4623,7 @@
         <v>6</v>
       </c>
       <c r="Q25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -4672,7 +4672,7 @@
         <v>6</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -4721,7 +4721,7 @@
         <v>6</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
@@ -4850,7 +4850,7 @@
         <v>6</v>
       </c>
       <c r="Q30" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -4966,7 +4966,7 @@
         <v>6</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -5591,6 +5591,29 @@
       <c r="N50" s="10" t="n"/>
       <c r="Q50" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="13" t="inlineStr">
+        <is>
+          <t>SanBucaツ</t>
+        </is>
+      </c>
+      <c r="B51" s="15" t="inlineStr">
+        <is>
+          <t>23/02/2026</t>
+        </is>
+      </c>
+      <c r="C51" s="13">
+        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
+        <v/>
+      </c>
+      <c r="K51" s="10" t="n"/>
+      <c r="L51" s="10" t="n"/>
+      <c r="M51" s="9" t="n"/>
+      <c r="N51" s="10" t="n"/>
+      <c r="Q51" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-24
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2716,14 +2716,14 @@
         <v/>
       </c>
       <c r="E39" s="24" t="n">
-        <v>74200</v>
+        <v>74600</v>
       </c>
       <c r="F39" s="33" t="n"/>
       <c r="G39" s="33" t="n"/>
       <c r="H39" s="33" t="n"/>
       <c r="I39" s="33" t="n"/>
       <c r="J39" s="33" t="n">
-        <v>2500</v>
+        <v>2900</v>
       </c>
       <c r="K39" s="33" t="n"/>
       <c r="L39" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-25
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -1613,7 +1613,7 @@
         <v/>
       </c>
       <c r="E16" s="24" t="n">
-        <v>64020</v>
+        <v>65520</v>
       </c>
       <c r="F16" s="33" t="n"/>
       <c r="G16" s="33" t="n"/>
@@ -1622,7 +1622,7 @@
         <v>6350</v>
       </c>
       <c r="J16" s="33" t="n">
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="K16" s="33" t="n"/>
       <c r="L16" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-26
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -1086,7 +1086,7 @@
         <v/>
       </c>
       <c r="E5" s="24" t="n">
-        <v>22225</v>
+        <v>25225</v>
       </c>
       <c r="F5" s="33" t="n"/>
       <c r="G5" s="33" t="n"/>
@@ -1095,7 +1095,7 @@
         <v>2000</v>
       </c>
       <c r="J5" s="33" t="n">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="K5" s="33" t="n"/>
       <c r="L5" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-27
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -2620,14 +2620,14 @@
         <v/>
       </c>
       <c r="E37" s="24" t="n">
-        <v>76300</v>
+        <v>76450</v>
       </c>
       <c r="F37" s="33" t="n"/>
       <c r="G37" s="33" t="n"/>
       <c r="H37" s="33" t="n"/>
       <c r="I37" s="33" t="n"/>
       <c r="J37" s="33" t="n">
-        <v>4600</v>
+        <v>4750</v>
       </c>
       <c r="K37" s="33" t="n"/>
       <c r="L37" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Games data - 2026-02-28
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -943,7 +943,7 @@
         <v/>
       </c>
       <c r="E2" s="23" t="n">
-        <v>31255</v>
+        <v>32505</v>
       </c>
       <c r="F2" s="17" t="n"/>
       <c r="G2" s="17" t="n"/>
@@ -952,7 +952,7 @@
         <v>1500</v>
       </c>
       <c r="J2" s="17" t="n">
-        <v>1700</v>
+        <v>2950</v>
       </c>
       <c r="K2" s="17" t="n"/>
       <c r="L2" s="17" t="n"/>
@@ -1419,7 +1419,7 @@
         <v/>
       </c>
       <c r="E12" s="24" t="n">
-        <v>32800</v>
+        <v>33700</v>
       </c>
       <c r="F12" s="33" t="n">
         <v>4000</v>
@@ -1434,7 +1434,7 @@
         <v>2450</v>
       </c>
       <c r="J12" s="33" t="n">
-        <v>3150</v>
+        <v>4050</v>
       </c>
       <c r="K12" s="33" t="n"/>
       <c r="L12" s="33" t="n"/>

</xml_diff>

<commit_message>
Update Clan Capital data - 2026-02-28
</commit_message>
<xml_diff>
--- a/cc_cg_events.xlsx
+++ b/cc_cg_events.xlsx
@@ -3134,7 +3134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH48"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="R1" s="7" t="inlineStr">
         <is>
-          <t>Colonna16</t>
+          <t>27/02/2026</t>
         </is>
       </c>
       <c r="S1" s="7" t="inlineStr">
@@ -3367,6 +3367,9 @@
       <c r="Q2" t="n">
         <v>0</v>
       </c>
+      <c r="R2" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -3404,6 +3407,9 @@
       <c r="Q3" t="n">
         <v>0</v>
       </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -3462,6 +3468,9 @@
       <c r="Q4" t="n">
         <v>6</v>
       </c>
+      <c r="R4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -3496,45 +3505,66 @@
       <c r="Q5" t="n">
         <v>6</v>
       </c>
+      <c r="R5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>andriu07</t>
+          <t>BigMc23</t>
         </is>
       </c>
       <c r="B6" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C6" s="13">
         <f>ROUND(AVERAGE(D6:AH6), 0)</f>
         <v/>
       </c>
+      <c r="G6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K6" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L6" s="10" t="n">
         <v>5</v>
       </c>
       <c r="M6" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N6" s="33" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P6" t="n">
         <v>6</v>
       </c>
       <c r="Q6" t="n">
+        <v>6</v>
+      </c>
+      <c r="R6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>BigMc23</t>
+          <t>buff x-bow</t>
         </is>
       </c>
       <c r="B7" s="15" t="inlineStr">
@@ -3546,11 +3576,20 @@
         <f>ROUND(AVERAGE(D7:AH7), 0)</f>
         <v/>
       </c>
+      <c r="D7" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G7" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H7" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I7" s="9" t="n">
         <v>6</v>
@@ -3562,13 +3601,13 @@
         <v>6</v>
       </c>
       <c r="L7" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M7" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N7" s="33" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O7" t="n">
         <v>6</v>
@@ -3578,12 +3617,15 @@
       </c>
       <c r="Q7" t="n">
         <v>6</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="13" t="inlineStr">
         <is>
-          <t>buff x-bow</t>
+          <t>Chabby</t>
         </is>
       </c>
       <c r="B8" s="15" t="inlineStr">
@@ -3611,37 +3653,40 @@
         <v>0</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J8" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K8" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L8" s="10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M8" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N8" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q8" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
         <is>
-          <t>Chabby</t>
+          <t>dado</t>
         </is>
       </c>
       <c r="B9" s="15" t="inlineStr">
@@ -3653,53 +3698,47 @@
         <f>ROUND(AVERAGE(D9:AH9), 0)</f>
         <v/>
       </c>
-      <c r="D9" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G9" s="9" t="n">
         <v>6</v>
       </c>
       <c r="H9" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I9" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K9" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L9" s="10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M9" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N9" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q9" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="inlineStr">
         <is>
-          <t>dado</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B10" s="15" t="inlineStr">
@@ -3712,16 +3751,16 @@
         <v/>
       </c>
       <c r="G10" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H10" s="9" t="n">
         <v>6</v>
       </c>
       <c r="I10" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J10" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K10" s="10" t="n">
         <v>6</v>
@@ -3730,25 +3769,28 @@
         <v>6</v>
       </c>
       <c r="M10" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N10" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q10" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="R10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>ER DANDI 1927</t>
         </is>
       </c>
       <c r="B11" s="15" t="inlineStr">
@@ -3761,43 +3803,46 @@
         <v/>
       </c>
       <c r="G11" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H11" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="9" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L11" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M11" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N11" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B12" s="15" t="inlineStr">
@@ -3809,44 +3854,56 @@
         <f>ROUND(AVERAGE(D12:AH12), 0)</f>
         <v/>
       </c>
+      <c r="D12" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G12" s="9" t="n">
         <v>5</v>
       </c>
       <c r="H12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="M12" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="N12" s="33" t="n">
+        <v>6</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="n">
         <v>5</v>
       </c>
-      <c r="I12" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J12" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L12" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="M12" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
+      <c r="R12" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B13" s="15" t="inlineStr">
@@ -3868,7 +3925,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="9" t="n">
         <v>6</v>
@@ -3898,39 +3955,27 @@
         <v>6</v>
       </c>
       <c r="Q13" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B14" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>29/12/2025</t>
         </is>
       </c>
       <c r="C14" s="13">
         <f>ROUND(AVERAGE(D14:AH14), 0)</f>
         <v/>
       </c>
-      <c r="D14" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F14" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G14" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H14" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="I14" s="9" t="n">
         <v>6</v>
       </c>
@@ -3941,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="L14" s="10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M14" s="9" t="n">
         <v>6</v>
@@ -3956,24 +4001,30 @@
         <v>6</v>
       </c>
       <c r="Q14" t="n">
+        <v>6</v>
+      </c>
+      <c r="R14" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
         <is>
-          <t>29/12/2025</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C15" s="13">
         <f>ROUND(AVERAGE(D15:AH15), 0)</f>
         <v/>
       </c>
+      <c r="H15" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="I15" s="9" t="n">
         <v>6</v>
       </c>
@@ -3984,7 +4035,7 @@
         <v>6</v>
       </c>
       <c r="L15" s="10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M15" s="9" t="n">
         <v>6</v>
@@ -3999,36 +4050,27 @@
         <v>6</v>
       </c>
       <c r="Q15" t="n">
+        <v>6</v>
+      </c>
+      <c r="R15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B16" s="15" t="inlineStr">
         <is>
-          <t>21/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C16" s="13">
         <f>ROUND(AVERAGE(D16:AH16), 0)</f>
         <v/>
       </c>
-      <c r="H16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I16" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J16" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K16" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L16" s="10" t="n">
         <v>6</v>
       </c>
@@ -4039,30 +4081,57 @@
         <v>6</v>
       </c>
       <c r="O16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
         <v>6</v>
       </c>
       <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B17" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C17" s="13">
         <f>ROUND(AVERAGE(D17:AH17), 0)</f>
         <v/>
       </c>
+      <c r="D17" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J17" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K17" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L17" s="10" t="n">
         <v>6</v>
       </c>
@@ -4073,19 +4142,22 @@
         <v>6</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P17" t="n">
         <v>6</v>
       </c>
       <c r="Q17" t="n">
+        <v>6</v>
+      </c>
+      <c r="R17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B18" s="15" t="inlineStr">
@@ -4107,116 +4179,122 @@
         <v>6</v>
       </c>
       <c r="G18" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H18" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I18" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J18" s="10" t="n">
         <v>6</v>
       </c>
       <c r="K18" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L18" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M18" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N18" s="33" t="n">
         <v>6</v>
       </c>
       <c r="O18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q18" t="n">
         <v>6</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B19" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C19" s="13">
         <f>ROUND(AVERAGE(D19:AH19), 0)</f>
         <v/>
       </c>
-      <c r="D19" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G19" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K19" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K19" s="10" t="n"/>
+      <c r="L19" s="10" t="n"/>
       <c r="M19" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N19" s="33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O19" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P19" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q19" t="n">
+        <v>6</v>
+      </c>
+      <c r="R19" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="13" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B20" s="15" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C20" s="13">
         <f>ROUND(AVERAGE(D20:AH20), 0)</f>
         <v/>
       </c>
-      <c r="K20" s="10" t="n"/>
-      <c r="L20" s="10" t="n"/>
+      <c r="D20" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I20" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J20" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K20" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="M20" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N20" s="33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O20" t="n">
         <v>6</v>
@@ -4225,56 +4303,34 @@
         <v>6</v>
       </c>
       <c r="Q20" t="n">
+        <v>6</v>
+      </c>
+      <c r="R20" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B21" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>25/01/2026</t>
         </is>
       </c>
       <c r="C21" s="13">
         <f>ROUND(AVERAGE(D21:AH21), 0)</f>
         <v/>
       </c>
-      <c r="D21" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I21" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J21" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K21" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L21" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="K21" s="10" t="n"/>
+      <c r="L21" s="10" t="n"/>
       <c r="M21" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
         <v>6</v>
@@ -4284,30 +4340,49 @@
       </c>
       <c r="Q21" t="n">
         <v>6</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B22" s="15" t="inlineStr">
         <is>
-          <t>25/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C22" s="13">
         <f>ROUND(AVERAGE(D22:AH22), 0)</f>
         <v/>
       </c>
-      <c r="K22" s="10" t="n"/>
-      <c r="L22" s="10" t="n"/>
+      <c r="G22" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I22" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J22" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="K22" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="M22" s="9" t="n">
         <v>6</v>
       </c>
       <c r="N22" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O22" t="n">
         <v>6</v>
@@ -4317,12 +4392,15 @@
       </c>
       <c r="Q22" t="n">
         <v>6</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B23" s="15" t="inlineStr">
@@ -4334,44 +4412,56 @@
         <f>ROUND(AVERAGE(D23:AH23), 0)</f>
         <v/>
       </c>
+      <c r="D23" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E23" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="G23" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I23" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J23" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K23" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L23" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M23" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N23" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B24" s="15" t="inlineStr">
@@ -4396,16 +4486,16 @@
         <v>0</v>
       </c>
       <c r="H24" s="9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I24" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J24" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K24" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L24" s="10" t="n">
         <v>0</v>
@@ -4417,19 +4507,22 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q24" t="n">
+        <v>6</v>
+      </c>
+      <c r="R24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B25" s="15" t="inlineStr">
@@ -4441,20 +4534,11 @@
         <f>ROUND(AVERAGE(D25:AH25), 0)</f>
         <v/>
       </c>
-      <c r="D25" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E25" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="9" t="n">
-        <v>6</v>
-      </c>
       <c r="G25" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H25" s="9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I25" s="9" t="n">
         <v>6</v>
@@ -4463,16 +4547,16 @@
         <v>6</v>
       </c>
       <c r="K25" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L25" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M25" s="9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N25" s="33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O25" t="n">
         <v>6</v>
@@ -4482,12 +4566,15 @@
       </c>
       <c r="Q25" t="n">
         <v>6</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B26" s="15" t="inlineStr">
@@ -4500,7 +4587,7 @@
         <v/>
       </c>
       <c r="G26" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H26" s="9" t="n">
         <v>6</v>
@@ -4531,38 +4618,26 @@
       </c>
       <c r="Q26" t="n">
         <v>6</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="13" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B27" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>16/01/2026</t>
         </is>
       </c>
       <c r="C27" s="13">
         <f>ROUND(AVERAGE(D27:AH27), 0)</f>
         <v/>
       </c>
-      <c r="G27" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I27" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J27" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K27" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="L27" s="10" t="n">
         <v>6</v>
       </c>
@@ -4579,24 +4654,30 @@
         <v>6</v>
       </c>
       <c r="Q27" t="n">
+        <v>6</v>
+      </c>
+      <c r="R27" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B28" s="15" t="inlineStr">
         <is>
-          <t>16/01/2026</t>
+          <t>12/01/2026</t>
         </is>
       </c>
       <c r="C28" s="13">
         <f>ROUND(AVERAGE(D28:AH28), 0)</f>
         <v/>
       </c>
+      <c r="K28" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="L28" s="10" t="n">
         <v>6</v>
       </c>
@@ -4614,23 +4695,47 @@
       </c>
       <c r="Q28" t="n">
         <v>6</v>
+      </c>
+      <c r="R28" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B29" s="15" t="inlineStr">
         <is>
-          <t>12/01/2026</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="C29" s="13">
         <f>ROUND(AVERAGE(D29:AH29), 0)</f>
         <v/>
       </c>
+      <c r="D29" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J29" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K29" s="10" t="n">
         <v>6</v>
       </c>
@@ -4651,12 +4756,15 @@
       </c>
       <c r="Q29" t="n">
         <v>6</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="13" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B30" s="15" t="inlineStr">
@@ -4669,7 +4777,7 @@
         <v/>
       </c>
       <c r="D30" s="14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" s="9" t="n">
         <v>6</v>
@@ -4681,7 +4789,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I30" s="9" t="n">
         <v>6</v>
@@ -4709,12 +4817,15 @@
       </c>
       <c r="Q30" t="n">
         <v>6</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="13" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B31" s="15" t="inlineStr">
@@ -4727,26 +4838,26 @@
         <v/>
       </c>
       <c r="D31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="E31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H31" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I31" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J31" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K31" s="10" t="n">
         <v>6</v>
       </c>
@@ -4767,12 +4878,15 @@
       </c>
       <c r="Q31" t="n">
         <v>6</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="13" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B32" s="15" t="inlineStr">
@@ -4826,11 +4940,14 @@
       <c r="Q32" t="n">
         <v>6</v>
       </c>
+      <c r="R32" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="13" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B33" s="15" t="inlineStr">
@@ -4842,27 +4959,7 @@
         <f>ROUND(AVERAGE(D33:AH33), 0)</f>
         <v/>
       </c>
-      <c r="D33" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F33" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G33" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H33" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I33" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J33" s="10" t="n">
-        <v>5</v>
-      </c>
+      <c r="J33" s="10" t="n"/>
       <c r="K33" s="10" t="n">
         <v>6</v>
       </c>
@@ -4882,13 +4979,16 @@
         <v>6</v>
       </c>
       <c r="Q33" t="n">
+        <v>6</v>
+      </c>
+      <c r="R33" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="13" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B34" s="15" t="inlineStr">
@@ -4925,7 +5025,7 @@
         <v>6</v>
       </c>
       <c r="L34" s="10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M34" s="9" t="n">
         <v>6</v>
@@ -4941,12 +5041,15 @@
       </c>
       <c r="Q34" t="n">
         <v>6</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="13" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B35" s="15" t="inlineStr">
@@ -4958,7 +5061,18 @@
         <f>ROUND(AVERAGE(D35:AH35), 0)</f>
         <v/>
       </c>
-      <c r="J35" s="10" t="n"/>
+      <c r="G35" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H35" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I35" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" s="10" t="n">
+        <v>6</v>
+      </c>
       <c r="K35" s="10" t="n">
         <v>6</v>
       </c>
@@ -4968,66 +5082,48 @@
       <c r="M35" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="N35" s="33" t="n">
+      <c r="N35" s="10" t="n">
         <v>6</v>
       </c>
       <c r="O35" t="n">
         <v>6</v>
       </c>
       <c r="P35" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q35" t="n">
         <v>6</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="13" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B36" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>05/01/2026</t>
         </is>
       </c>
       <c r="C36" s="13">
         <f>ROUND(AVERAGE(D36:AH36), 0)</f>
         <v/>
       </c>
-      <c r="D36" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J36" s="10" t="n">
-        <v>6</v>
-      </c>
       <c r="K36" s="10" t="n">
         <v>6</v>
       </c>
       <c r="L36" s="10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M36" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N36" s="33" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="N36" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="O36" t="n">
         <v>6</v>
@@ -5037,152 +5133,113 @@
       </c>
       <c r="Q36" t="n">
         <v>6</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="13" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B37" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C37" s="13">
         <f>ROUND(AVERAGE(D37:AH37), 0)</f>
         <v/>
       </c>
-      <c r="G37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" s="10" t="n">
+      <c r="K37" s="10" t="n"/>
+      <c r="L37" s="10" t="n"/>
+      <c r="M37" s="9" t="n"/>
+      <c r="N37" s="10" t="n"/>
+      <c r="O37" t="n">
         <v>5</v>
       </c>
-      <c r="L37" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M37" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N37" s="33" t="n">
-        <v>6</v>
-      </c>
-      <c r="O37" t="n">
-        <v>6</v>
-      </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="13" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B38" s="15" t="inlineStr">
         <is>
-          <t>15/12/2025</t>
+          <t>07/02/2026</t>
         </is>
       </c>
       <c r="C38" s="13">
         <f>ROUND(AVERAGE(D38:AH38), 0)</f>
         <v/>
       </c>
-      <c r="G38" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H38" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I38" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="J38" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="K38" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L38" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M38" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="N38" s="10" t="n">
-        <v>6</v>
-      </c>
+      <c r="K38" s="10" t="n"/>
+      <c r="L38" s="10" t="n"/>
+      <c r="M38" s="9" t="n"/>
+      <c r="N38" s="10" t="n"/>
       <c r="O38" t="n">
         <v>6</v>
       </c>
       <c r="P38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="13" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B39" s="15" t="inlineStr">
         <is>
-          <t>05/01/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C39" s="13">
         <f>ROUND(AVERAGE(D39:AH39), 0)</f>
         <v/>
       </c>
-      <c r="K39" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="L39" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="M39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>6</v>
-      </c>
+      <c r="K39" s="10" t="n"/>
+      <c r="L39" s="10" t="n"/>
+      <c r="M39" s="9" t="n"/>
+      <c r="N39" s="10" t="n"/>
       <c r="P39" t="n">
         <v>6</v>
       </c>
       <c r="Q39" t="n">
         <v>6</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="13" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>14/02/2026</t>
         </is>
       </c>
       <c r="C40" s="13">
@@ -5193,25 +5250,25 @@
       <c r="L40" s="10" t="n"/>
       <c r="M40" s="9" t="n"/>
       <c r="N40" s="10" t="n"/>
-      <c r="O40" t="n">
-        <v>5</v>
-      </c>
       <c r="P40" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
         <is>
-          <t>07/02/2026</t>
+          <t>16/02/2026</t>
         </is>
       </c>
       <c r="C41" s="13">
@@ -5222,25 +5279,25 @@
       <c r="L41" s="10" t="n"/>
       <c r="M41" s="9" t="n"/>
       <c r="N41" s="10" t="n"/>
-      <c r="O41" t="n">
-        <v>6</v>
-      </c>
       <c r="P41" t="n">
         <v>0</v>
       </c>
       <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="inlineStr">
         <is>
-          <t>Amazonie</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>14/02/2026</t>
+          <t>16/02/2026</t>
         </is>
       </c>
       <c r="C42" s="13">
@@ -5252,21 +5309,24 @@
       <c r="M42" s="9" t="n"/>
       <c r="N42" s="10" t="n"/>
       <c r="P42" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q42" t="n">
+        <v>2</v>
+      </c>
+      <c r="R42" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>terracrom</t>
+          <t>Xx_Herman_xX</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>14/02/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C43" s="13">
@@ -5277,22 +5337,22 @@
       <c r="L43" s="10" t="n"/>
       <c r="M43" s="9" t="n"/>
       <c r="N43" s="10" t="n"/>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
       <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>dibba10</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>16/02/2026</t>
+          <t>21/02/2026</t>
         </is>
       </c>
       <c r="C44" s="13">
@@ -5303,22 +5363,22 @@
       <c r="L44" s="10" t="n"/>
       <c r="M44" s="9" t="n"/>
       <c r="N44" s="10" t="n"/>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
       <c r="Q44" t="n">
+        <v>2</v>
+      </c>
+      <c r="R44" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>Dasters79</t>
+          <t>GGfresco_08</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
         <is>
-          <t>16/02/2026</t>
+          <t>28/02/2026</t>
         </is>
       </c>
       <c r="C45" s="13">
@@ -5329,22 +5389,19 @@
       <c r="L45" s="10" t="n"/>
       <c r="M45" s="9" t="n"/>
       <c r="N45" s="10" t="n"/>
-      <c r="P45" t="n">
+      <c r="R45" t="n">
         <v>1</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="13" t="inlineStr">
         <is>
-          <t>Artur</t>
+          <t>PESCARA MANZIA</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
         <is>
-          <t>21/02/2026</t>
+          <t>28/02/2026</t>
         </is>
       </c>
       <c r="C46" s="13">
@@ -5355,19 +5412,19 @@
       <c r="L46" s="10" t="n"/>
       <c r="M46" s="9" t="n"/>
       <c r="N46" s="10" t="n"/>
-      <c r="Q46" t="n">
-        <v>0</v>
+      <c r="R46" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>Xx_Herman_xX</t>
+          <t>eltishqipe</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
         <is>
-          <t>21/02/2026</t>
+          <t>28/02/2026</t>
         </is>
       </c>
       <c r="C47" s="13">
@@ -5378,19 +5435,19 @@
       <c r="L47" s="10" t="n"/>
       <c r="M47" s="9" t="n"/>
       <c r="N47" s="10" t="n"/>
-      <c r="Q47" t="n">
+      <c r="R47" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="13" t="inlineStr">
         <is>
-          <t>dibba10</t>
+          <t>VERRETHERULER</t>
         </is>
       </c>
       <c r="B48" s="15" t="inlineStr">
         <is>
-          <t>21/02/2026</t>
+          <t>28/02/2026</t>
         </is>
       </c>
       <c r="C48" s="13">
@@ -5401,79 +5458,11 @@
       <c r="L48" s="10" t="n"/>
       <c r="M48" s="9" t="n"/>
       <c r="N48" s="10" t="n"/>
-      <c r="Q48" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="13" t="inlineStr">
-        <is>
-          <t>Anto</t>
-        </is>
-      </c>
-      <c r="B49" s="15" t="inlineStr">
-        <is>
-          <t>21/02/2026</t>
-        </is>
-      </c>
-      <c r="C49" s="13">
-        <f>ROUND(AVERAGE(D49:AH49), 0)</f>
-        <v/>
-      </c>
-      <c r="K49" s="10" t="n"/>
-      <c r="L49" s="10" t="n"/>
-      <c r="M49" s="9" t="n"/>
-      <c r="N49" s="10" t="n"/>
-      <c r="Q49" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="13" t="inlineStr">
-        <is>
-          <t>Michele</t>
-        </is>
-      </c>
-      <c r="B50" s="15" t="inlineStr">
-        <is>
-          <t>21/02/2026</t>
-        </is>
-      </c>
-      <c r="C50" s="13">
-        <f>ROUND(AVERAGE(D50:AH50), 0)</f>
-        <v/>
-      </c>
-      <c r="K50" s="10" t="n"/>
-      <c r="L50" s="10" t="n"/>
-      <c r="M50" s="9" t="n"/>
-      <c r="N50" s="10" t="n"/>
-      <c r="Q50" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="13" t="inlineStr">
-        <is>
-          <t>SanBucaツ</t>
-        </is>
-      </c>
-      <c r="B51" s="15" t="inlineStr">
-        <is>
-          <t>23/02/2026</t>
-        </is>
-      </c>
-      <c r="C51" s="13">
-        <f>ROUND(AVERAGE(D51:AH51), 0)</f>
-        <v/>
-      </c>
-      <c r="K51" s="10" t="n"/>
-      <c r="L51" s="10" t="n"/>
-      <c r="M51" s="9" t="n"/>
-      <c r="N51" s="10" t="n"/>
-      <c r="Q51" t="n">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:AT1">
     <sortState ref="A2:AH50">

</xml_diff>